<commit_message>
Actualizar calificaciones y añadir codigo para consultar tweets
</commit_message>
<xml_diff>
--- a/grades/Calificaciones.xlsx
+++ b/grades/Calificaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/02_Studies/2022_MCD_UDG/03_Desarrollo_proyectos_II/2022-s1_Material_Vic/05_Calificaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE33EA7A-B87A-BB4A-8E9D-3449FC72C357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C440307C-9EAE-3A46-928A-C9FFCB72B25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="500" windowWidth="27940" windowHeight="16440" activeTab="5" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
+    <workbookView xWindow="460" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN FINAL" sheetId="5" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="1102">
   <si>
     <t>Id. estudiante</t>
   </si>
@@ -3797,12 +3797,6 @@
     <t>MARTHA OLIVIA</t>
   </si>
   <si>
-    <t>Publicación</t>
-  </si>
-  <si>
-    <t>Exposición en congreso</t>
-  </si>
-  <si>
     <t>ACTIVIDAD</t>
   </si>
   <si>
@@ -3821,9 +3815,6 @@
       </rPr>
       <t>1/</t>
     </r>
-  </si>
-  <si>
-    <t>Puntos acumulados al 2022-04-06</t>
   </si>
   <si>
     <t>1/ Para hacerse acreedores a los puntos extras, el alumno tiene que tener una calificación acumulada mínima de 70.</t>
@@ -3869,6 +3860,18 @@
   </si>
   <si>
     <t>Nomeclatura: n.a. se refiere a "no aplica".</t>
+  </si>
+  <si>
+    <t>@Risk+Project</t>
+  </si>
+  <si>
+    <t>2 actividades</t>
+  </si>
+  <si>
+    <t>Exposición en congreso, publicación</t>
+  </si>
+  <si>
+    <t>Puntos acumulados al 2022-04-27</t>
   </si>
 </sst>
 </file>
@@ -4428,7 +4431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4567,21 +4570,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4648,6 +4636,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7506,21 +7512,16 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="23" customWidth="1"/>
     <col min="2" max="2" width="27" style="23" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="17"/>
-    <col min="4" max="4" width="14.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="17" customWidth="1"/>
+    <col min="3" max="8" width="16.5" style="17" customWidth="1"/>
     <col min="9" max="9" width="0" style="17" hidden="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="17"/>
   </cols>
@@ -7534,11 +7535,11 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="str">
         <f>RESUMEN!A40</f>
-        <v>Puntos acumulados al 2022-04-06</v>
+        <v>Puntos acumulados al 2022-04-27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I3" s="91" t="str">
+      <c r="I3" s="86" t="str">
         <f>"|"&amp;A4&amp;"|"&amp;B4&amp;"|"&amp;C4&amp;"|"&amp;D4&amp;"|"&amp;E4&amp;"|"&amp;F4&amp;"|"&amp;G4&amp;"|__"&amp;H4&amp;"__|"</f>
         <v>|Id. estudiante|Nombre|EXPOSICIONES (30%)|QUIZES (CONTROLES DE LECTURA, 30%)|TAREAS (20%)|EXAMEN FINAL (20%)|PUNTOS EXTRAS|__CALIF. FINAL__|</v>
       </c>
@@ -7550,25 +7551,25 @@
       <c r="B4" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="123" t="s">
         <v>991</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="125" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="84" t="s">
+      <c r="H4" s="126" t="s">
         <v>990</v>
       </c>
-      <c r="I4" s="115" t="str">
+      <c r="I4" s="110" t="str">
         <f>"|---|---|---|---|---|---|---|---|"</f>
         <v>|---|---|---|---|---|---|---|---|</v>
       </c>
@@ -7580,33 +7581,33 @@
       <c r="B5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="112">
+      <c r="C5" s="107">
         <f>RESUMEN!F5</f>
         <v>100</v>
       </c>
-      <c r="D5" s="112">
+      <c r="D5" s="107">
         <f>RESUMEN!Q5</f>
         <v>100</v>
       </c>
-      <c r="E5" s="112">
+      <c r="E5" s="107">
         <f>RESUMEN!AC5</f>
         <v>100</v>
       </c>
-      <c r="F5" s="112">
+      <c r="F5" s="107">
         <f>RESUMEN!AD5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="112">
+      <c r="G5" s="107">
         <f>RESUMEN!C24</f>
-        <v>5</v>
-      </c>
-      <c r="H5" s="90">
+        <v>10</v>
+      </c>
+      <c r="H5" s="85">
         <f t="shared" ref="H5:H14" si="0">C5*0.3+D5*0.3+E5*0.2+F5*0.2+G5</f>
-        <v>85</v>
-      </c>
-      <c r="I5" s="91" t="str">
+        <v>90</v>
+      </c>
+      <c r="I5" s="86" t="str">
         <f>"|"&amp;A5&amp;"|"&amp;B5&amp;"|"&amp;ROUND(C5,1)&amp;"|"&amp;ROUND(D5,1)&amp;"|"&amp;ROUND(E5,1)&amp;"|"&amp;ROUND(F5,1)&amp;"|"&amp;ROUND(G5,1)&amp;"|__"&amp;ROUND(H5,1)&amp;"__|"</f>
-        <v>|220981245|José Raúl Castro Esparza|100|100|100|0|5|__85__|</v>
+        <v>|220981245|José Raúl Castro Esparza|100|100|100|0|10|__90__|</v>
       </c>
     </row>
     <row r="6" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
@@ -7616,31 +7617,31 @@
       <c r="B6" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="112">
+      <c r="C6" s="107">
         <f>RESUMEN!F6</f>
         <v>100</v>
       </c>
-      <c r="D6" s="112">
+      <c r="D6" s="107">
         <f>RESUMEN!Q6</f>
         <v>100</v>
       </c>
-      <c r="E6" s="112">
+      <c r="E6" s="107">
         <f>RESUMEN!AC6</f>
         <v>100</v>
       </c>
-      <c r="F6" s="112">
+      <c r="F6" s="107">
         <f>RESUMEN!AD6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="112">
+      <c r="G6" s="107">
         <f>RESUMEN!C25</f>
         <v>0</v>
       </c>
-      <c r="H6" s="90">
+      <c r="H6" s="85">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I6" s="91" t="str">
+      <c r="I6" s="86" t="str">
         <f t="shared" ref="I6:I14" si="1">"|"&amp;A6&amp;"|"&amp;B6&amp;"|"&amp;ROUND(C6,1)&amp;"|"&amp;ROUND(D6,1)&amp;"|"&amp;ROUND(E6,1)&amp;"|"&amp;ROUND(F6,1)&amp;"|"&amp;ROUND(G6,1)&amp;"|__"&amp;ROUND(H6,1)&amp;"__|"</f>
         <v>|399515449|Martha Olivia Ramos Lara|100|100|100|0|0|__80__|</v>
       </c>
@@ -7652,31 +7653,31 @@
       <c r="B7" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="112">
+      <c r="C7" s="107">
         <f>RESUMEN!F7</f>
         <v>100</v>
       </c>
-      <c r="D7" s="112">
+      <c r="D7" s="107">
         <f>RESUMEN!Q7</f>
         <v>91.481481481481467</v>
       </c>
-      <c r="E7" s="112">
+      <c r="E7" s="107">
         <f>RESUMEN!AC7</f>
         <v>88.609393939393939</v>
       </c>
-      <c r="F7" s="112">
+      <c r="F7" s="107">
         <f>RESUMEN!AD7</f>
         <v>0</v>
       </c>
-      <c r="G7" s="112">
+      <c r="G7" s="107">
         <f>RESUMEN!C26</f>
         <v>0</v>
       </c>
-      <c r="H7" s="90">
+      <c r="H7" s="85">
         <f t="shared" si="0"/>
         <v>75.166323232323236</v>
       </c>
-      <c r="I7" s="91" t="str">
+      <c r="I7" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|207595964|Carol Desireé Ramírez Durán|100|91.5|88.6|0|0|__75.2__|</v>
       </c>
@@ -7688,31 +7689,31 @@
       <c r="B8" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="112">
+      <c r="C8" s="107">
         <f>RESUMEN!F8</f>
         <v>100</v>
       </c>
-      <c r="D8" s="112">
+      <c r="D8" s="107">
         <f>RESUMEN!Q8</f>
         <v>84.815185185185172</v>
       </c>
-      <c r="E8" s="112">
+      <c r="E8" s="107">
         <f>RESUMEN!AC8</f>
         <v>88.609393939393939</v>
       </c>
-      <c r="F8" s="112">
+      <c r="F8" s="107">
         <f>RESUMEN!AD8</f>
         <v>0</v>
       </c>
-      <c r="G8" s="112">
+      <c r="G8" s="107">
         <f>RESUMEN!C27</f>
         <v>0</v>
       </c>
-      <c r="H8" s="90">
+      <c r="H8" s="85">
         <f t="shared" si="0"/>
         <v>73.166434343434346</v>
       </c>
-      <c r="I8" s="91" t="str">
+      <c r="I8" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|211776124|César Iván Vargas López|100|84.8|88.6|0|0|__73.2__|</v>
       </c>
@@ -7724,31 +7725,31 @@
       <c r="B9" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="112">
+      <c r="C9" s="107">
         <f>RESUMEN!F9</f>
         <v>100</v>
       </c>
-      <c r="D9" s="112">
+      <c r="D9" s="107">
         <f>RESUMEN!Q9</f>
         <v>78.518333333333331</v>
       </c>
-      <c r="E9" s="112">
+      <c r="E9" s="107">
         <f>RESUMEN!AC9</f>
         <v>100</v>
       </c>
-      <c r="F9" s="112">
+      <c r="F9" s="107">
         <f>RESUMEN!AD9</f>
         <v>0</v>
       </c>
-      <c r="G9" s="112">
+      <c r="G9" s="107">
         <f>RESUMEN!C28</f>
         <v>0</v>
       </c>
-      <c r="H9" s="90">
+      <c r="H9" s="85">
         <f t="shared" si="0"/>
         <v>73.555499999999995</v>
       </c>
-      <c r="I9" s="91" t="str">
+      <c r="I9" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|220981202|Pedro Martínez Ayala|100|78.5|100|0|0|__73.6__|</v>
       </c>
@@ -7760,31 +7761,31 @@
       <c r="B10" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="107">
         <f>RESUMEN!F10</f>
         <v>100</v>
       </c>
-      <c r="D10" s="112">
+      <c r="D10" s="107">
         <f>RESUMEN!Q10</f>
         <v>100.00000000000001</v>
       </c>
-      <c r="E10" s="112">
+      <c r="E10" s="107">
         <f>RESUMEN!AC10</f>
         <v>100</v>
       </c>
-      <c r="F10" s="112">
+      <c r="F10" s="107">
         <f>RESUMEN!AD10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="112">
+      <c r="G10" s="107">
         <f>RESUMEN!C29</f>
         <v>0</v>
       </c>
-      <c r="H10" s="90">
+      <c r="H10" s="85">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I10" s="91" t="str">
+      <c r="I10" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|398813438|Afra Julieta Lomelí Avila|100|100|100|0|0|__80__|</v>
       </c>
@@ -7796,31 +7797,31 @@
       <c r="B11" s="82" t="s">
         <v>992</v>
       </c>
-      <c r="C11" s="112">
+      <c r="C11" s="107">
         <f>RESUMEN!F11</f>
         <v>100</v>
       </c>
-      <c r="D11" s="112">
+      <c r="D11" s="107">
         <f>RESUMEN!Q11</f>
         <v>52.223703703703706</v>
       </c>
-      <c r="E11" s="112">
+      <c r="E11" s="107">
         <f>RESUMEN!AC11</f>
         <v>91.612834224598927</v>
       </c>
-      <c r="F11" s="112">
+      <c r="F11" s="107">
         <f>RESUMEN!AD11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="112">
+      <c r="G11" s="107">
         <f>RESUMEN!C30</f>
         <v>0</v>
       </c>
-      <c r="H11" s="90">
+      <c r="H11" s="85">
         <f t="shared" si="0"/>
         <v>63.989677956030903</v>
       </c>
-      <c r="I11" s="91" t="str">
+      <c r="I11" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|220981261|Mónica Alonso Soria|100|52.2|91.6|0|0|__64__|</v>
       </c>
@@ -7832,31 +7833,31 @@
       <c r="B12" s="82" t="s">
         <v>993</v>
       </c>
-      <c r="C12" s="112">
+      <c r="C12" s="107">
         <f>RESUMEN!F12</f>
         <v>100</v>
       </c>
-      <c r="D12" s="112">
+      <c r="D12" s="107">
         <f>RESUMEN!Q12</f>
         <v>82.221851851851852</v>
       </c>
-      <c r="E12" s="112">
+      <c r="E12" s="107">
         <f>RESUMEN!AC12</f>
         <v>91.612834224598927</v>
       </c>
-      <c r="F12" s="112">
+      <c r="F12" s="107">
         <f>RESUMEN!AD12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="112">
+      <c r="G12" s="107">
         <f>RESUMEN!C31</f>
         <v>0</v>
       </c>
-      <c r="H12" s="90">
+      <c r="H12" s="85">
         <f t="shared" si="0"/>
         <v>72.989122400475338</v>
       </c>
-      <c r="I12" s="91" t="str">
+      <c r="I12" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|220981296|Mario Palomino Hernández|100|82.2|91.6|0|0|__73__|</v>
       </c>
@@ -7868,31 +7869,31 @@
       <c r="B13" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="112">
+      <c r="C13" s="107">
         <f>RESUMEN!F13</f>
         <v>85</v>
       </c>
-      <c r="D13" s="112">
+      <c r="D13" s="107">
         <f>RESUMEN!Q13</f>
         <v>64.258888888888876</v>
       </c>
-      <c r="E13" s="112">
+      <c r="E13" s="107">
         <f>RESUMEN!AC13</f>
         <v>89.990909090909099</v>
       </c>
-      <c r="F13" s="112">
+      <c r="F13" s="107">
         <f>RESUMEN!AD13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="112">
+      <c r="G13" s="107">
         <f>RESUMEN!C32</f>
         <v>0</v>
       </c>
-      <c r="H13" s="90">
+      <c r="H13" s="85">
         <f t="shared" si="0"/>
         <v>62.775848484848481</v>
       </c>
-      <c r="I13" s="91" t="str">
+      <c r="I13" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|220981229|Luis Enrique Neri González|85|64.3|90|0|0|__62.8__|</v>
       </c>
@@ -7904,37 +7905,37 @@
       <c r="B14" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="112">
+      <c r="C14" s="107">
         <f>RESUMEN!F14</f>
         <v>100</v>
       </c>
-      <c r="D14" s="112">
+      <c r="D14" s="107">
         <f>RESUMEN!Q14</f>
         <v>87.777777777777771</v>
       </c>
-      <c r="E14" s="112">
+      <c r="E14" s="107">
         <f>RESUMEN!AC14</f>
         <v>89.990909090909099</v>
       </c>
-      <c r="F14" s="112">
+      <c r="F14" s="107">
         <f>RESUMEN!AD14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="112">
+      <c r="G14" s="107">
         <f>RESUMEN!C33</f>
         <v>0</v>
       </c>
-      <c r="H14" s="90">
+      <c r="H14" s="85">
         <f t="shared" si="0"/>
         <v>74.331515151515148</v>
       </c>
-      <c r="I14" s="91" t="str">
+      <c r="I14" s="86" t="str">
         <f t="shared" si="1"/>
         <v>|220981288|Carlos Samuel Cruz Mariscal|100|87.8|90|0|0|__74.3__|</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="91"/>
+      <c r="I15" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7947,7 +7948,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8128,34 +8129,34 @@
         <f>AVERAGE(D5:E5)</f>
         <v>100</v>
       </c>
-      <c r="G5" s="106">
-        <v>100</v>
-      </c>
-      <c r="H5" s="107">
-        <v>100</v>
-      </c>
-      <c r="I5" s="107">
-        <v>100</v>
-      </c>
-      <c r="J5" s="107">
-        <v>100</v>
-      </c>
-      <c r="K5" s="107">
-        <v>100</v>
-      </c>
-      <c r="L5" s="107">
-        <v>100</v>
-      </c>
-      <c r="M5" s="107">
-        <v>100</v>
-      </c>
-      <c r="N5" s="107">
-        <v>100</v>
-      </c>
-      <c r="O5" s="108">
-        <v>100</v>
-      </c>
-      <c r="P5" s="108">
+      <c r="G5" s="101">
+        <v>100</v>
+      </c>
+      <c r="H5" s="102">
+        <v>100</v>
+      </c>
+      <c r="I5" s="102">
+        <v>100</v>
+      </c>
+      <c r="J5" s="102">
+        <v>100</v>
+      </c>
+      <c r="K5" s="102">
+        <v>100</v>
+      </c>
+      <c r="L5" s="102">
+        <v>100</v>
+      </c>
+      <c r="M5" s="102">
+        <v>100</v>
+      </c>
+      <c r="N5" s="102">
+        <v>100</v>
+      </c>
+      <c r="O5" s="103">
+        <v>100</v>
+      </c>
+      <c r="P5" s="103">
         <v>90</v>
       </c>
       <c r="Q5" s="68">
@@ -8224,34 +8225,34 @@
         <f t="shared" ref="F6:F14" si="1">AVERAGE(D6:E6)</f>
         <v>100</v>
       </c>
-      <c r="G6" s="106">
-        <v>100</v>
-      </c>
-      <c r="H6" s="107">
-        <v>100</v>
-      </c>
-      <c r="I6" s="107">
-        <v>100</v>
-      </c>
-      <c r="J6" s="107">
-        <v>100</v>
-      </c>
-      <c r="K6" s="107">
-        <v>100</v>
-      </c>
-      <c r="L6" s="107">
-        <v>100</v>
-      </c>
-      <c r="M6" s="107">
-        <v>100</v>
-      </c>
-      <c r="N6" s="107">
-        <v>100</v>
-      </c>
-      <c r="O6" s="108">
-        <v>100</v>
-      </c>
-      <c r="P6" s="108">
+      <c r="G6" s="101">
+        <v>100</v>
+      </c>
+      <c r="H6" s="102">
+        <v>100</v>
+      </c>
+      <c r="I6" s="102">
+        <v>100</v>
+      </c>
+      <c r="J6" s="102">
+        <v>100</v>
+      </c>
+      <c r="K6" s="102">
+        <v>100</v>
+      </c>
+      <c r="L6" s="102">
+        <v>100</v>
+      </c>
+      <c r="M6" s="102">
+        <v>100</v>
+      </c>
+      <c r="N6" s="102">
+        <v>100</v>
+      </c>
+      <c r="O6" s="103">
+        <v>100</v>
+      </c>
+      <c r="P6" s="103">
         <v>0</v>
       </c>
       <c r="Q6" s="68">
@@ -8320,34 +8321,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G7" s="106">
+      <c r="G7" s="101">
         <v>93.33</v>
       </c>
-      <c r="H7" s="107">
+      <c r="H7" s="102">
         <v>80</v>
       </c>
-      <c r="I7" s="107">
+      <c r="I7" s="102">
         <v>86.67</v>
       </c>
-      <c r="J7" s="107">
-        <v>100</v>
-      </c>
-      <c r="K7" s="107">
+      <c r="J7" s="102">
+        <v>100</v>
+      </c>
+      <c r="K7" s="102">
         <v>93.33</v>
       </c>
-      <c r="L7" s="107">
+      <c r="L7" s="102">
         <v>93.333333333333329</v>
       </c>
-      <c r="M7" s="107">
+      <c r="M7" s="102">
         <v>86.67</v>
       </c>
-      <c r="N7" s="107">
+      <c r="N7" s="102">
         <v>93.33</v>
       </c>
-      <c r="O7" s="108">
+      <c r="O7" s="103">
         <v>86.67</v>
       </c>
-      <c r="P7" s="108">
+      <c r="P7" s="103">
         <v>90</v>
       </c>
       <c r="Q7" s="68">
@@ -8416,35 +8417,35 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G8" s="106">
+      <c r="G8" s="101">
         <v>93.33</v>
       </c>
-      <c r="H8" s="107">
+      <c r="H8" s="102">
         <v>73.33</v>
       </c>
-      <c r="I8" s="107">
+      <c r="I8" s="102">
         <f>QUIZES!C35</f>
         <v>86.67</v>
       </c>
-      <c r="J8" s="107">
-        <v>100</v>
-      </c>
-      <c r="K8" s="107">
+      <c r="J8" s="102">
+        <v>100</v>
+      </c>
+      <c r="K8" s="102">
         <v>80</v>
       </c>
-      <c r="L8" s="107">
+      <c r="L8" s="102">
         <v>86.666666666666671</v>
       </c>
-      <c r="M8" s="107">
+      <c r="M8" s="102">
         <v>86.67</v>
       </c>
-      <c r="N8" s="107">
+      <c r="N8" s="102">
         <v>66.67</v>
       </c>
-      <c r="O8" s="108">
+      <c r="O8" s="103">
         <v>66.67</v>
       </c>
-      <c r="P8" s="108">
+      <c r="P8" s="103">
         <v>90</v>
       </c>
       <c r="Q8" s="68">
@@ -8513,34 +8514,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G9" s="106">
+      <c r="G9" s="101">
         <v>36.664999999999999</v>
       </c>
-      <c r="H9" s="107">
-        <v>100</v>
-      </c>
-      <c r="I9" s="107">
-        <v>100</v>
-      </c>
-      <c r="J9" s="107">
+      <c r="H9" s="102">
+        <v>100</v>
+      </c>
+      <c r="I9" s="102">
+        <v>100</v>
+      </c>
+      <c r="J9" s="102">
         <v>93.33</v>
       </c>
-      <c r="K9" s="107">
-        <v>100</v>
-      </c>
-      <c r="L9" s="107">
+      <c r="K9" s="102">
+        <v>100</v>
+      </c>
+      <c r="L9" s="102">
         <v>0</v>
       </c>
-      <c r="M9" s="107">
+      <c r="M9" s="102">
         <v>0</v>
       </c>
-      <c r="N9" s="107">
+      <c r="N9" s="102">
         <v>86.67</v>
       </c>
-      <c r="O9" s="108">
-        <v>100</v>
-      </c>
-      <c r="P9" s="108">
+      <c r="O9" s="103">
+        <v>100</v>
+      </c>
+      <c r="P9" s="103">
         <v>90</v>
       </c>
       <c r="Q9" s="68">
@@ -8609,34 +8610,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G10" s="106">
+      <c r="G10" s="101">
         <v>86.67</v>
       </c>
-      <c r="H10" s="107">
-        <v>100</v>
-      </c>
-      <c r="I10" s="107">
-        <v>100</v>
-      </c>
-      <c r="J10" s="107">
-        <v>100</v>
-      </c>
-      <c r="K10" s="107">
-        <v>100</v>
-      </c>
-      <c r="L10" s="107">
-        <v>100</v>
-      </c>
-      <c r="M10" s="107">
-        <v>100</v>
-      </c>
-      <c r="N10" s="107">
-        <v>100</v>
-      </c>
-      <c r="O10" s="108">
-        <v>100</v>
-      </c>
-      <c r="P10" s="108">
+      <c r="H10" s="102">
+        <v>100</v>
+      </c>
+      <c r="I10" s="102">
+        <v>100</v>
+      </c>
+      <c r="J10" s="102">
+        <v>100</v>
+      </c>
+      <c r="K10" s="102">
+        <v>100</v>
+      </c>
+      <c r="L10" s="102">
+        <v>100</v>
+      </c>
+      <c r="M10" s="102">
+        <v>100</v>
+      </c>
+      <c r="N10" s="102">
+        <v>100</v>
+      </c>
+      <c r="O10" s="103">
+        <v>100</v>
+      </c>
+      <c r="P10" s="103">
         <v>100</v>
       </c>
       <c r="Q10" s="68">
@@ -8705,34 +8706,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G11" s="106">
+      <c r="G11" s="101">
         <v>80</v>
       </c>
-      <c r="H11" s="107">
+      <c r="H11" s="102">
         <v>43.335000000000001</v>
       </c>
-      <c r="I11" s="107">
+      <c r="I11" s="102">
         <v>80</v>
       </c>
-      <c r="J11" s="107">
+      <c r="J11" s="102">
         <v>66.67</v>
       </c>
-      <c r="K11" s="107">
+      <c r="K11" s="102">
         <v>33.335000000000001</v>
       </c>
-      <c r="L11" s="107">
+      <c r="L11" s="102">
         <v>73.333333333333329</v>
       </c>
-      <c r="M11" s="107">
+      <c r="M11" s="102">
         <v>46.67</v>
       </c>
-      <c r="N11" s="107">
+      <c r="N11" s="102">
         <v>46.67</v>
       </c>
-      <c r="O11" s="108">
+      <c r="O11" s="103">
         <v>0</v>
       </c>
-      <c r="P11" s="108">
+      <c r="P11" s="103">
         <v>0</v>
       </c>
       <c r="Q11" s="68">
@@ -8801,34 +8802,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G12" s="106">
+      <c r="G12" s="101">
         <v>86.67</v>
       </c>
-      <c r="H12" s="107">
+      <c r="H12" s="102">
         <v>93.33</v>
       </c>
-      <c r="I12" s="107">
-        <v>100</v>
-      </c>
-      <c r="J12" s="107">
+      <c r="I12" s="102">
+        <v>100</v>
+      </c>
+      <c r="J12" s="102">
         <v>73.33</v>
       </c>
-      <c r="K12" s="107">
+      <c r="K12" s="102">
         <v>86.67</v>
       </c>
-      <c r="L12" s="107">
+      <c r="L12" s="102">
         <v>66.666666666666657</v>
       </c>
-      <c r="M12" s="107">
+      <c r="M12" s="102">
         <v>73.33</v>
       </c>
-      <c r="N12" s="107">
+      <c r="N12" s="102">
         <v>80</v>
       </c>
-      <c r="O12" s="108">
+      <c r="O12" s="103">
         <v>80</v>
       </c>
-      <c r="P12" s="108">
+      <c r="P12" s="103">
         <v>0</v>
       </c>
       <c r="Q12" s="68">
@@ -8897,34 +8898,34 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G13" s="106">
+      <c r="G13" s="101">
         <v>93.33</v>
       </c>
-      <c r="H13" s="107">
+      <c r="H13" s="102">
         <v>73.33</v>
       </c>
-      <c r="I13" s="107">
+      <c r="I13" s="102">
         <v>86.67</v>
       </c>
-      <c r="J13" s="107">
+      <c r="J13" s="102">
         <v>0</v>
       </c>
-      <c r="K13" s="107">
+      <c r="K13" s="102">
         <v>86.67</v>
       </c>
-      <c r="L13" s="107">
+      <c r="L13" s="102">
         <v>60</v>
       </c>
-      <c r="M13" s="107">
+      <c r="M13" s="102">
         <v>93.33</v>
       </c>
-      <c r="N13" s="107">
+      <c r="N13" s="102">
         <v>0</v>
       </c>
-      <c r="O13" s="108">
+      <c r="O13" s="103">
         <v>0</v>
       </c>
-      <c r="P13" s="108">
+      <c r="P13" s="103">
         <v>85</v>
       </c>
       <c r="Q13" s="68">
@@ -8993,34 +8994,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G14" s="109">
-        <v>100</v>
-      </c>
-      <c r="H14" s="110">
-        <v>100</v>
-      </c>
-      <c r="I14" s="110">
+      <c r="G14" s="104">
+        <v>100</v>
+      </c>
+      <c r="H14" s="105">
+        <v>100</v>
+      </c>
+      <c r="I14" s="105">
         <v>93.33</v>
       </c>
-      <c r="J14" s="110">
-        <v>100</v>
-      </c>
-      <c r="K14" s="110">
-        <v>100</v>
-      </c>
-      <c r="L14" s="110">
+      <c r="J14" s="105">
+        <v>100</v>
+      </c>
+      <c r="K14" s="105">
+        <v>100</v>
+      </c>
+      <c r="L14" s="105">
         <v>80</v>
       </c>
-      <c r="M14" s="110">
+      <c r="M14" s="105">
         <v>80</v>
       </c>
-      <c r="N14" s="110">
+      <c r="N14" s="105">
         <v>46.67</v>
       </c>
-      <c r="O14" s="111">
+      <c r="O14" s="106">
         <v>43.34</v>
       </c>
-      <c r="P14" s="111">
+      <c r="P14" s="106">
         <v>90</v>
       </c>
       <c r="Q14" s="71">
@@ -9087,7 +9088,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>57</v>
@@ -9101,7 +9102,7 @@
       <c r="H22" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="J22" s="116"/>
+      <c r="J22" s="111"/>
     </row>
     <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
@@ -9138,7 +9139,7 @@
       </c>
       <c r="C24" s="16">
         <f>MIN(SUM(E24:H24),4*D24*5)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D24" s="16">
         <f>IF(C5&gt;=70,1,0)</f>
@@ -9148,7 +9149,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G24" s="34">
         <v>0</v>
@@ -9410,8 +9411,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="117" t="s">
-        <v>1090</v>
+      <c r="A35" s="112" t="s">
+        <v>1087</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -9422,7 +9423,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -9450,7 +9451,7 @@
       </c>
       <c r="C43" s="16">
         <f>MIN(100,C5+C24)</f>
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -9612,7 +9613,7 @@
         <v>68</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H2" s="60" t="s">
         <v>989</v>
@@ -9640,7 +9641,7 @@
         <f>(F3-E3)*24*60</f>
         <v>1.8833332392387092</v>
       </c>
-      <c r="H3" s="92" t="str">
+      <c r="H3" s="87" t="str">
         <f>HOUR(F3)&amp;IF(MINUTE(F3)&gt;=10, ":"&amp;MINUTE(F3), ":0"&amp;MINUTE(F3))</f>
         <v>20:50</v>
       </c>
@@ -9667,7 +9668,7 @@
         <f t="shared" ref="G4:G12" si="1">(F4-E4)*24*60</f>
         <v>7.4833332491107285</v>
       </c>
-      <c r="H4" s="93" t="str">
+      <c r="H4" s="88" t="str">
         <f t="shared" ref="H4:H12" si="2">HOUR(F4)&amp;IF(MINUTE(F4)&gt;=10, ":"&amp;MINUTE(F4), ":0"&amp;MINUTE(F4))</f>
         <v>20:50</v>
       </c>
@@ -9694,7 +9695,7 @@
         <f t="shared" si="1"/>
         <v>61.233333261916414</v>
       </c>
-      <c r="H5" s="92" t="str">
+      <c r="H5" s="87" t="str">
         <f t="shared" si="2"/>
         <v>21:05</v>
       </c>
@@ -9721,7 +9722,7 @@
         <f t="shared" si="1"/>
         <v>68.300000071758404</v>
       </c>
-      <c r="H6" s="93" t="str">
+      <c r="H6" s="88" t="str">
         <f t="shared" si="2"/>
         <v>21:08</v>
       </c>
@@ -9748,7 +9749,7 @@
         <f t="shared" si="1"/>
         <v>79.10000006086193</v>
       </c>
-      <c r="H7" s="92" t="str">
+      <c r="H7" s="87" t="str">
         <f t="shared" si="2"/>
         <v>21:09</v>
       </c>
@@ -9775,7 +9776,7 @@
         <f t="shared" si="1"/>
         <v>34.200000000419095</v>
       </c>
-      <c r="H8" s="93" t="str">
+      <c r="H8" s="88" t="str">
         <f t="shared" si="2"/>
         <v>21:17</v>
       </c>
@@ -9802,7 +9803,7 @@
         <f t="shared" si="1"/>
         <v>18.366666622459888</v>
       </c>
-      <c r="H9" s="92" t="str">
+      <c r="H9" s="87" t="str">
         <f t="shared" si="2"/>
         <v>21:42</v>
       </c>
@@ -9829,7 +9830,7 @@
         <f t="shared" si="1"/>
         <v>57.050000061281025</v>
       </c>
-      <c r="H10" s="93" t="str">
+      <c r="H10" s="88" t="str">
         <f t="shared" si="2"/>
         <v>21:58</v>
       </c>
@@ -9856,7 +9857,7 @@
         <f t="shared" si="1"/>
         <v>85.250000021187589</v>
       </c>
-      <c r="H11" s="92" t="str">
+      <c r="H11" s="87" t="str">
         <f t="shared" si="2"/>
         <v>22:10</v>
       </c>
@@ -9885,7 +9886,7 @@
         <f t="shared" si="1"/>
         <v>34.449999985517934</v>
       </c>
-      <c r="H12" s="99" t="str">
+      <c r="H12" s="94" t="str">
         <f t="shared" si="2"/>
         <v>23:52</v>
       </c>
@@ -9915,7 +9916,7 @@
         <v>68</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H16" s="60" t="str">
         <f>$H$2</f>
@@ -9944,7 +9945,7 @@
         <f>(F17-E17)*24*60</f>
         <v>0.36666662665084004</v>
       </c>
-      <c r="H17" s="92" t="str">
+      <c r="H17" s="87" t="str">
         <f t="shared" ref="H17:H26" si="3">HOUR(F17)&amp;IF(MINUTE(F17)&gt;=10, ":"&amp;MINUTE(F17), ":0"&amp;MINUTE(F17))</f>
         <v>19:46</v>
       </c>
@@ -9971,7 +9972,7 @@
         <f t="shared" ref="G18:G26" si="5">(F18-E18)*24*60</f>
         <v>10.10000002454035</v>
       </c>
-      <c r="H18" s="93" t="str">
+      <c r="H18" s="88" t="str">
         <f t="shared" si="3"/>
         <v>19:54</v>
       </c>
@@ -9998,7 +9999,7 @@
         <f t="shared" si="5"/>
         <v>23.700000102398917</v>
       </c>
-      <c r="H19" s="92" t="str">
+      <c r="H19" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:32</v>
       </c>
@@ -10025,7 +10026,7 @@
         <f t="shared" si="5"/>
         <v>53.783333280589432</v>
       </c>
-      <c r="H20" s="93" t="str">
+      <c r="H20" s="88" t="str">
         <f t="shared" si="3"/>
         <v>20:33</v>
       </c>
@@ -10052,7 +10053,7 @@
         <f t="shared" si="5"/>
         <v>25.850000018253922</v>
       </c>
-      <c r="H21" s="92" t="str">
+      <c r="H21" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10079,7 +10080,7 @@
         <f t="shared" si="5"/>
         <v>20.766666680574417</v>
       </c>
-      <c r="H22" s="93" t="str">
+      <c r="H22" s="88" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10106,7 +10107,7 @@
         <f t="shared" si="5"/>
         <v>26.416666806908324</v>
       </c>
-      <c r="H23" s="92" t="str">
+      <c r="H23" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10133,7 +10134,7 @@
         <f t="shared" si="5"/>
         <v>2.366666643647477</v>
       </c>
-      <c r="H24" s="93" t="str">
+      <c r="H24" s="88" t="str">
         <f t="shared" si="3"/>
         <v>20:48</v>
       </c>
@@ -10160,7 +10161,7 @@
         <f t="shared" si="5"/>
         <v>77.049999937880784</v>
       </c>
-      <c r="H25" s="92" t="str">
+      <c r="H25" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:59</v>
       </c>
@@ -10189,7 +10190,7 @@
         <f t="shared" si="5"/>
         <v>61.149999888148159</v>
       </c>
-      <c r="H26" s="99" t="str">
+      <c r="H26" s="94" t="str">
         <f t="shared" si="3"/>
         <v>21:14</v>
       </c>
@@ -10219,7 +10220,7 @@
         <v>68</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H30" s="60" t="str">
         <f>$H$2</f>
@@ -10248,7 +10249,7 @@
         <f>(F31-E31)*24*60</f>
         <v>10.066666599595919</v>
       </c>
-      <c r="H31" s="92" t="str">
+      <c r="H31" s="87" t="str">
         <f t="shared" ref="H31:H40" si="6">HOUR(F31)&amp;IF(MINUTE(F31)&gt;=10, ":"&amp;MINUTE(F31), ":0"&amp;MINUTE(F31))</f>
         <v>18:38</v>
       </c>
@@ -10275,7 +10276,7 @@
         <f t="shared" ref="G32:G40" si="8">(F32-E32)*24*60</f>
         <v>1.2166666577104479</v>
       </c>
-      <c r="H32" s="93" t="str">
+      <c r="H32" s="88" t="str">
         <f t="shared" si="6"/>
         <v>19:29</v>
       </c>
@@ -10302,7 +10303,7 @@
         <f t="shared" si="8"/>
         <v>17.533333440078422</v>
       </c>
-      <c r="H33" s="92" t="str">
+      <c r="H33" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:24</v>
       </c>
@@ -10329,7 +10330,7 @@
         <f t="shared" si="8"/>
         <v>22.833333358867094</v>
       </c>
-      <c r="H34" s="93" t="str">
+      <c r="H34" s="88" t="str">
         <f t="shared" si="6"/>
         <v>20:29</v>
       </c>
@@ -10356,7 +10357,7 @@
         <f t="shared" si="8"/>
         <v>27.583333348156884</v>
       </c>
-      <c r="H35" s="92" t="str">
+      <c r="H35" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:36</v>
       </c>
@@ -10383,7 +10384,7 @@
         <f t="shared" si="8"/>
         <v>34.833333303686231</v>
       </c>
-      <c r="H36" s="93" t="str">
+      <c r="H36" s="88" t="str">
         <f t="shared" si="6"/>
         <v>20:40</v>
       </c>
@@ -10410,7 +10411,7 @@
         <f t="shared" si="8"/>
         <v>34.049999944400042</v>
       </c>
-      <c r="H37" s="92" t="str">
+      <c r="H37" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:41</v>
       </c>
@@ -10437,7 +10438,7 @@
         <f t="shared" si="8"/>
         <v>23.449999970616773</v>
       </c>
-      <c r="H38" s="93" t="str">
+      <c r="H38" s="88" t="str">
         <f t="shared" si="6"/>
         <v>20:42</v>
       </c>
@@ -10464,7 +10465,7 @@
         <f t="shared" si="8"/>
         <v>24.316666703671217</v>
       </c>
-      <c r="H39" s="92" t="str">
+      <c r="H39" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:44</v>
       </c>
@@ -10491,7 +10492,7 @@
         <f t="shared" si="8"/>
         <v>1.6333333903457969</v>
       </c>
-      <c r="H40" s="93" t="str">
+      <c r="H40" s="88" t="str">
         <f t="shared" si="6"/>
         <v>20:57</v>
       </c>
@@ -10521,7 +10522,7 @@
         <v>68</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H44" s="60" t="str">
         <f>$H$2</f>
@@ -10550,7 +10551,7 @@
         <f>(F45-E45)*24*60</f>
         <v>2.9000000073574483</v>
       </c>
-      <c r="H45" s="92" t="str">
+      <c r="H45" s="87" t="str">
         <f t="shared" ref="H45:H53" si="9">HOUR(F45)&amp;IF(MINUTE(F45)&gt;=10, ":"&amp;MINUTE(F45), ":0"&amp;MINUTE(F45))</f>
         <v>19:01</v>
       </c>
@@ -10577,7 +10578,7 @@
         <f t="shared" ref="G46:G53" si="11">(F46-E46)*24*60</f>
         <v>3.4500001044943929</v>
       </c>
-      <c r="H46" s="93" t="str">
+      <c r="H46" s="88" t="str">
         <f t="shared" si="9"/>
         <v>19:36</v>
       </c>
@@ -10604,7 +10605,7 @@
         <f t="shared" si="11"/>
         <v>12.300000046379864</v>
       </c>
-      <c r="H47" s="92" t="str">
+      <c r="H47" s="87" t="str">
         <f t="shared" si="9"/>
         <v>20:25</v>
       </c>
@@ -10631,7 +10632,7 @@
         <f t="shared" si="11"/>
         <v>14.150000017834827</v>
       </c>
-      <c r="H48" s="93" t="str">
+      <c r="H48" s="88" t="str">
         <f t="shared" si="9"/>
         <v>20:29</v>
       </c>
@@ -10658,7 +10659,7 @@
         <f t="shared" si="11"/>
         <v>98.449999921722338</v>
       </c>
-      <c r="H49" s="92" t="str">
+      <c r="H49" s="87" t="str">
         <f t="shared" si="9"/>
         <v>20:37</v>
       </c>
@@ -10685,7 +10686,7 @@
         <f t="shared" si="11"/>
         <v>2.0666666887700558</v>
       </c>
-      <c r="H50" s="93" t="str">
+      <c r="H50" s="88" t="str">
         <f t="shared" si="9"/>
         <v>20:41</v>
       </c>
@@ -10712,7 +10713,7 @@
         <f t="shared" si="11"/>
         <v>69.46666675969027</v>
       </c>
-      <c r="H51" s="92" t="str">
+      <c r="H51" s="87" t="str">
         <f t="shared" si="9"/>
         <v>20:41</v>
       </c>
@@ -10739,7 +10740,7 @@
         <f t="shared" si="11"/>
         <v>28.866666677640751</v>
       </c>
-      <c r="H52" s="93" t="str">
+      <c r="H52" s="88" t="str">
         <f t="shared" si="9"/>
         <v>20:42</v>
       </c>
@@ -10766,29 +10767,29 @@
         <f t="shared" si="11"/>
         <v>3.8833333924412727</v>
       </c>
-      <c r="H53" s="92" t="str">
+      <c r="H53" s="87" t="str">
         <f t="shared" si="9"/>
         <v>21:08</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="97" t="s">
+      <c r="A54" s="92" t="s">
         <v>696</v>
       </c>
-      <c r="B54" s="97">
+      <c r="B54" s="92">
         <v>0</v>
       </c>
-      <c r="C54" s="100">
+      <c r="C54" s="95">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="D54" s="97" t="s">
+      <c r="D54" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E54" s="101"/>
-      <c r="F54" s="101"/>
-      <c r="G54" s="101"/>
-      <c r="H54" s="102"/>
+      <c r="E54" s="96"/>
+      <c r="F54" s="96"/>
+      <c r="G54" s="96"/>
+      <c r="H54" s="97"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -10815,7 +10816,7 @@
         <v>68</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H58" s="60" t="str">
         <f>$H$2</f>
@@ -10844,7 +10845,7 @@
         <f>(F59-E59)*24*60</f>
         <v>1.3500000012572855</v>
       </c>
-      <c r="H59" s="92" t="str">
+      <c r="H59" s="87" t="str">
         <f t="shared" ref="H59:H68" si="12">HOUR(F59)&amp;IF(MINUTE(F59)&gt;=10, ":"&amp;MINUTE(F59), ":0"&amp;MINUTE(F59))</f>
         <v>19:20</v>
       </c>
@@ -10871,7 +10872,7 @@
         <f t="shared" ref="G60:G68" si="14">(F60-E60)*24*60</f>
         <v>1.2500000617001206</v>
       </c>
-      <c r="H60" s="93" t="str">
+      <c r="H60" s="88" t="str">
         <f t="shared" si="12"/>
         <v>19:27</v>
       </c>
@@ -10898,7 +10899,7 @@
         <f t="shared" si="14"/>
         <v>18.716666536638513</v>
       </c>
-      <c r="H61" s="92" t="str">
+      <c r="H61" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:19</v>
       </c>
@@ -10925,7 +10926,7 @@
         <f t="shared" si="14"/>
         <v>27.316666661063209</v>
       </c>
-      <c r="H62" s="93" t="str">
+      <c r="H62" s="88" t="str">
         <f t="shared" si="12"/>
         <v>20:29</v>
       </c>
@@ -10952,7 +10953,7 @@
         <f t="shared" si="14"/>
         <v>61.666666707023978</v>
       </c>
-      <c r="H63" s="92" t="str">
+      <c r="H63" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:32</v>
       </c>
@@ -10979,7 +10980,7 @@
         <f t="shared" si="14"/>
         <v>29.033333425177261</v>
       </c>
-      <c r="H64" s="93" t="str">
+      <c r="H64" s="88" t="str">
         <f t="shared" si="12"/>
         <v>20:33</v>
       </c>
@@ -11006,7 +11007,7 @@
         <f t="shared" si="14"/>
         <v>35.316666582366452</v>
       </c>
-      <c r="H65" s="92" t="str">
+      <c r="H65" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:36</v>
       </c>
@@ -11033,7 +11034,7 @@
         <f t="shared" si="14"/>
         <v>4.2999999783933163</v>
       </c>
-      <c r="H66" s="93" t="str">
+      <c r="H66" s="88" t="str">
         <f t="shared" si="12"/>
         <v>20:37</v>
       </c>
@@ -11060,7 +11061,7 @@
         <f t="shared" si="14"/>
         <v>62.583333409857005</v>
       </c>
-      <c r="H67" s="92" t="str">
+      <c r="H67" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:37</v>
       </c>
@@ -11085,11 +11086,11 @@
       <c r="F68" s="41">
         <v>44619.626990740697</v>
       </c>
-      <c r="G68" s="96">
+      <c r="G68" s="91">
         <f t="shared" si="14"/>
         <v>83.099999948171899</v>
       </c>
-      <c r="H68" s="99" t="str">
+      <c r="H68" s="94" t="str">
         <f t="shared" si="12"/>
         <v>15:02</v>
       </c>
@@ -11119,7 +11120,7 @@
         <v>68</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H72" s="60" t="str">
         <f>$H$2</f>
@@ -11150,7 +11151,7 @@
         <f>(F73-E73)*24*60</f>
         <v>4.600000079954043</v>
       </c>
-      <c r="H73" s="94" t="str">
+      <c r="H73" s="89" t="str">
         <f t="shared" ref="H73:H82" si="15">HOUR(F73)&amp;IF(MINUTE(F73)&gt;=10, ":"&amp;MINUTE(F73), ":0"&amp;MINUTE(F73))</f>
         <v>21:42</v>
       </c>
@@ -11177,7 +11178,7 @@
         <f t="shared" ref="G74:G82" si="17">(F74-E74)*24*60</f>
         <v>2.649999896530062</v>
       </c>
-      <c r="H74" s="93" t="str">
+      <c r="H74" s="88" t="str">
         <f t="shared" si="15"/>
         <v>19:09</v>
       </c>
@@ -11204,7 +11205,7 @@
         <f t="shared" si="17"/>
         <v>3.1499998562503606</v>
       </c>
-      <c r="H75" s="92" t="str">
+      <c r="H75" s="87" t="str">
         <f t="shared" si="15"/>
         <v>19:20</v>
       </c>
@@ -11231,7 +11232,7 @@
         <f t="shared" si="17"/>
         <v>8.4500000684056431</v>
       </c>
-      <c r="H76" s="93" t="str">
+      <c r="H76" s="88" t="str">
         <f t="shared" si="15"/>
         <v>20:07</v>
       </c>
@@ -11258,7 +11259,7 @@
         <f t="shared" si="17"/>
         <v>17.466666768305004</v>
       </c>
-      <c r="H77" s="92" t="str">
+      <c r="H77" s="87" t="str">
         <f t="shared" si="15"/>
         <v>20:13</v>
       </c>
@@ -11285,7 +11286,7 @@
         <f t="shared" si="17"/>
         <v>28.566666576080024</v>
       </c>
-      <c r="H78" s="93" t="str">
+      <c r="H78" s="88" t="str">
         <f t="shared" si="15"/>
         <v>20:26</v>
       </c>
@@ -11312,7 +11313,7 @@
         <f t="shared" si="17"/>
         <v>36.033333406085148</v>
       </c>
-      <c r="H79" s="92" t="str">
+      <c r="H79" s="87" t="str">
         <f t="shared" si="15"/>
         <v>20:35</v>
       </c>
@@ -11339,7 +11340,7 @@
         <f t="shared" si="17"/>
         <v>40.999999976484105</v>
       </c>
-      <c r="H80" s="93" t="str">
+      <c r="H80" s="88" t="str">
         <f t="shared" si="15"/>
         <v>20:40</v>
       </c>
@@ -11366,7 +11367,7 @@
         <f t="shared" si="17"/>
         <v>44.883333358447999</v>
       </c>
-      <c r="H81" s="92" t="str">
+      <c r="H81" s="87" t="str">
         <f t="shared" si="15"/>
         <v>21:17</v>
       </c>
@@ -11393,29 +11394,29 @@
         <f t="shared" si="17"/>
         <v>36.316666658967733</v>
       </c>
-      <c r="H82" s="93" t="str">
+      <c r="H82" s="88" t="str">
         <f t="shared" si="15"/>
         <v>21:26</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="98" t="s">
+      <c r="A83" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="B83" s="98">
+      <c r="B83" s="93">
         <v>0</v>
       </c>
-      <c r="C83" s="103">
+      <c r="C83" s="98">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D83" s="97" t="s">
+      <c r="D83" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E83" s="104"/>
-      <c r="F83" s="104"/>
-      <c r="G83" s="104"/>
-      <c r="H83" s="105"/>
+      <c r="E83" s="99"/>
+      <c r="F83" s="99"/>
+      <c r="G83" s="99"/>
+      <c r="H83" s="100"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -11442,7 +11443,7 @@
         <v>68</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H87" s="60" t="str">
         <f>$H$2</f>
@@ -11471,7 +11472,7 @@
         <f>(F88-E88)*24*60</f>
         <v>1.0500000463798642</v>
       </c>
-      <c r="H88" s="92" t="str">
+      <c r="H88" s="87" t="str">
         <f t="shared" ref="H88:H97" si="18">HOUR(F88)&amp;IF(MINUTE(F88)&gt;=10, ":"&amp;MINUTE(F88), ":0"&amp;MINUTE(F88))</f>
         <v>20:02</v>
       </c>
@@ -11498,7 +11499,7 @@
         <f t="shared" ref="G89:G97" si="20">(F89-E89)*24*60</f>
         <v>13.966666704509407</v>
       </c>
-      <c r="H89" s="93" t="str">
+      <c r="H89" s="88" t="str">
         <f t="shared" si="18"/>
         <v>20:14</v>
       </c>
@@ -11525,7 +11526,7 @@
         <f t="shared" si="20"/>
         <v>40.983333410695195</v>
       </c>
-      <c r="H90" s="92" t="str">
+      <c r="H90" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:41</v>
       </c>
@@ -11552,7 +11553,7 @@
         <f t="shared" si="20"/>
         <v>2.3666666331700981</v>
       </c>
-      <c r="H91" s="93" t="str">
+      <c r="H91" s="88" t="str">
         <f t="shared" si="18"/>
         <v>20:42</v>
       </c>
@@ -11581,7 +11582,7 @@
         <f t="shared" si="20"/>
         <v>0.61666675843298435</v>
       </c>
-      <c r="H92" s="95" t="str">
+      <c r="H92" s="90" t="str">
         <f t="shared" si="18"/>
         <v>20:43</v>
       </c>
@@ -11608,7 +11609,7 @@
         <f t="shared" si="20"/>
         <v>49.81666665058583</v>
       </c>
-      <c r="H93" s="93" t="str">
+      <c r="H93" s="88" t="str">
         <f t="shared" si="18"/>
         <v>20:50</v>
       </c>
@@ -11635,7 +11636,7 @@
         <f t="shared" si="20"/>
         <v>49.333333246177062</v>
       </c>
-      <c r="H94" s="92" t="str">
+      <c r="H94" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:50</v>
       </c>
@@ -11662,7 +11663,7 @@
         <f t="shared" si="20"/>
         <v>90.133333343546838</v>
       </c>
-      <c r="H95" s="93" t="str">
+      <c r="H95" s="88" t="str">
         <f t="shared" si="18"/>
         <v>20:56</v>
       </c>
@@ -11689,7 +11690,7 @@
         <f t="shared" si="20"/>
         <v>86.583333309972659</v>
       </c>
-      <c r="H96" s="92" t="str">
+      <c r="H96" s="87" t="str">
         <f t="shared" si="18"/>
         <v>21:20</v>
       </c>
@@ -11716,29 +11717,29 @@
         <f t="shared" si="20"/>
         <v>76.93333343253471</v>
       </c>
-      <c r="H97" s="93" t="str">
+      <c r="H97" s="88" t="str">
         <f t="shared" si="18"/>
         <v>21:20</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="98" t="s">
+      <c r="A98" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="B98" s="98">
+      <c r="B98" s="93">
         <v>0</v>
       </c>
-      <c r="C98" s="103">
+      <c r="C98" s="98">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="D98" s="97" t="s">
+      <c r="D98" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E98" s="104"/>
-      <c r="F98" s="104"/>
-      <c r="G98" s="104"/>
-      <c r="H98" s="105"/>
+      <c r="E98" s="99"/>
+      <c r="F98" s="99"/>
+      <c r="G98" s="99"/>
+      <c r="H98" s="100"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
@@ -11765,7 +11766,7 @@
         <v>68</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H102" s="60" t="str">
         <f>$H$2</f>
@@ -11794,7 +11795,7 @@
         <f>(F103-E103)*24*60</f>
         <v>53.033333325292915</v>
       </c>
-      <c r="H103" s="92" t="str">
+      <c r="H103" s="87" t="str">
         <f t="shared" ref="H103:H111" si="21">HOUR(F103)&amp;IF(MINUTE(F103)&gt;=10, ":"&amp;MINUTE(F103), ":0"&amp;MINUTE(F103))</f>
         <v>19:08</v>
       </c>
@@ -11821,7 +11822,7 @@
         <f t="shared" ref="G104:G111" si="23">(F104-E104)*24*60</f>
         <v>2.416666749631986</v>
       </c>
-      <c r="H104" s="93" t="str">
+      <c r="H104" s="88" t="str">
         <f t="shared" si="21"/>
         <v>20:06</v>
       </c>
@@ -11848,7 +11849,7 @@
         <f t="shared" si="23"/>
         <v>3.1999999727122486</v>
       </c>
-      <c r="H105" s="92" t="str">
+      <c r="H105" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:07</v>
       </c>
@@ -11875,7 +11876,7 @@
         <f t="shared" si="23"/>
         <v>1.9333333452232182</v>
       </c>
-      <c r="H106" s="93" t="str">
+      <c r="H106" s="88" t="str">
         <f t="shared" si="21"/>
         <v>20:07</v>
       </c>
@@ -11902,7 +11903,7 @@
         <f t="shared" si="23"/>
         <v>18.433333294233307</v>
       </c>
-      <c r="H107" s="92" t="str">
+      <c r="H107" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:22</v>
       </c>
@@ -11929,7 +11930,7 @@
         <f t="shared" si="23"/>
         <v>60.26666673598811</v>
       </c>
-      <c r="H108" s="93" t="str">
+      <c r="H108" s="88" t="str">
         <f t="shared" si="21"/>
         <v>20:24</v>
       </c>
@@ -11956,7 +11957,7 @@
         <f t="shared" si="23"/>
         <v>8.2333333406131715</v>
       </c>
-      <c r="H109" s="92" t="str">
+      <c r="H109" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:35</v>
       </c>
@@ -11983,7 +11984,7 @@
         <f t="shared" si="23"/>
         <v>38.300000110175461</v>
       </c>
-      <c r="H110" s="93" t="str">
+      <c r="H110" s="88" t="str">
         <f t="shared" si="21"/>
         <v>20:42</v>
       </c>
@@ -12010,29 +12011,29 @@
         <f t="shared" si="23"/>
         <v>1.7833334463648498</v>
       </c>
-      <c r="H111" s="92" t="str">
+      <c r="H111" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:44</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="97" t="s">
+      <c r="A112" s="92" t="s">
         <v>696</v>
       </c>
-      <c r="B112" s="97">
+      <c r="B112" s="92">
         <v>0</v>
       </c>
-      <c r="C112" s="100">
+      <c r="C112" s="95">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="D112" s="97" t="s">
+      <c r="D112" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E112" s="101"/>
-      <c r="F112" s="101"/>
-      <c r="G112" s="102"/>
-      <c r="H112" s="102"/>
+      <c r="E112" s="96"/>
+      <c r="F112" s="96"/>
+      <c r="G112" s="97"/>
+      <c r="H112" s="97"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
@@ -12059,7 +12060,7 @@
         <v>68</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H116" s="60" t="str">
         <f>$H$2</f>
@@ -12088,7 +12089,7 @@
         <f>(F117-E117)*24*60</f>
         <v>2.8666666033677757</v>
       </c>
-      <c r="H117" s="92" t="str">
+      <c r="H117" s="87" t="str">
         <f t="shared" ref="H117:H124" si="24">HOUR(F117)&amp;IF(MINUTE(F117)&gt;=10, ":"&amp;MINUTE(F117), ":0"&amp;MINUTE(F117))</f>
         <v>19:04</v>
       </c>
@@ -12115,7 +12116,7 @@
         <f t="shared" ref="G118:G124" si="26">(F118-E118)*24*60</f>
         <v>2.1500000625383109</v>
       </c>
-      <c r="H118" s="93" t="str">
+      <c r="H118" s="88" t="str">
         <f t="shared" si="24"/>
         <v>19:30</v>
       </c>
@@ -12142,7 +12143,7 @@
         <f t="shared" si="26"/>
         <v>1.8833333754446357</v>
       </c>
-      <c r="H119" s="92" t="str">
+      <c r="H119" s="87" t="str">
         <f t="shared" si="24"/>
         <v>20:03</v>
       </c>
@@ -12169,7 +12170,7 @@
         <f t="shared" si="26"/>
         <v>25.966666659805924</v>
       </c>
-      <c r="H120" s="93" t="str">
+      <c r="H120" s="88" t="str">
         <f t="shared" si="24"/>
         <v>20:04</v>
       </c>
@@ -12196,7 +12197,7 @@
         <f t="shared" si="26"/>
         <v>30.80000001238659</v>
       </c>
-      <c r="H121" s="92" t="str">
+      <c r="H121" s="87" t="str">
         <f t="shared" si="24"/>
         <v>20:07</v>
       </c>
@@ -12223,7 +12224,7 @@
         <f t="shared" si="26"/>
         <v>72.600000039674342</v>
       </c>
-      <c r="H122" s="93" t="str">
+      <c r="H122" s="88" t="str">
         <f t="shared" si="24"/>
         <v>21:17</v>
       </c>
@@ -12250,7 +12251,7 @@
         <f t="shared" si="26"/>
         <v>2.3333333758637309</v>
       </c>
-      <c r="H123" s="92" t="str">
+      <c r="H123" s="87" t="str">
         <f t="shared" si="24"/>
         <v>21:20</v>
       </c>
@@ -12279,48 +12280,48 @@
         <f t="shared" si="26"/>
         <v>3.6833332409150898</v>
       </c>
-      <c r="H124" s="99" t="str">
+      <c r="H124" s="94" t="str">
         <f t="shared" si="24"/>
         <v>19:09</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A125" s="98" t="s">
+      <c r="A125" s="93" t="s">
         <v>986</v>
       </c>
-      <c r="B125" s="98">
+      <c r="B125" s="93">
         <v>0</v>
       </c>
-      <c r="C125" s="103">
+      <c r="C125" s="98">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D125" s="97" t="s">
+      <c r="D125" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E125" s="104"/>
-      <c r="F125" s="104"/>
-      <c r="G125" s="101"/>
-      <c r="H125" s="105"/>
+      <c r="E125" s="99"/>
+      <c r="F125" s="99"/>
+      <c r="G125" s="96"/>
+      <c r="H125" s="100"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="97" t="s">
+      <c r="A126" s="92" t="s">
         <v>696</v>
       </c>
-      <c r="B126" s="97">
+      <c r="B126" s="92">
         <v>0</v>
       </c>
-      <c r="C126" s="100">
+      <c r="C126" s="95">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D126" s="97" t="s">
+      <c r="D126" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E126" s="101"/>
-      <c r="F126" s="101"/>
-      <c r="G126" s="101"/>
-      <c r="H126" s="102"/>
+      <c r="E126" s="96"/>
+      <c r="F126" s="96"/>
+      <c r="G126" s="96"/>
+      <c r="H126" s="97"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
@@ -12352,7 +12353,7 @@
         <v>68</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="H131" s="60" t="str">
         <f>$H$2</f>
@@ -12381,7 +12382,7 @@
         <f>(F132-E132)*24*60</f>
         <v>7.0833333651535213</v>
       </c>
-      <c r="H132" s="95" t="str">
+      <c r="H132" s="90" t="str">
         <f t="shared" ref="H132:H139" si="27">HOUR(F132)&amp;IF(MINUTE(F132)&gt;=10, ":"&amp;MINUTE(F132), ":0"&amp;MINUTE(F132))</f>
         <v>20:06</v>
       </c>
@@ -12408,7 +12409,7 @@
         <f t="shared" ref="G133:G139" si="29">(F133-E133)*24*60</f>
         <v>5.116666752146557</v>
       </c>
-      <c r="H133" s="93" t="str">
+      <c r="H133" s="88" t="str">
         <f t="shared" si="27"/>
         <v>20:12</v>
       </c>
@@ -12435,7 +12436,7 @@
         <f t="shared" si="29"/>
         <v>18.016666551120579</v>
       </c>
-      <c r="H134" s="92" t="str">
+      <c r="H134" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:18</v>
       </c>
@@ -12462,7 +12463,7 @@
         <f t="shared" si="29"/>
         <v>32.466666680993512</v>
       </c>
-      <c r="H135" s="93" t="str">
+      <c r="H135" s="88" t="str">
         <f t="shared" si="27"/>
         <v>20:31</v>
       </c>
@@ -12489,7 +12490,7 @@
         <f t="shared" si="29"/>
         <v>2.4999999767169356</v>
       </c>
-      <c r="H136" s="92" t="str">
+      <c r="H136" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:32</v>
       </c>
@@ -12516,7 +12517,7 @@
         <f t="shared" si="29"/>
         <v>3.3500000182539225</v>
       </c>
-      <c r="H137" s="93" t="str">
+      <c r="H137" s="88" t="str">
         <f t="shared" si="27"/>
         <v>20:33</v>
       </c>
@@ -12543,7 +12544,7 @@
         <f t="shared" si="29"/>
         <v>35.116666703252122</v>
       </c>
-      <c r="H138" s="92" t="str">
+      <c r="H138" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:33</v>
       </c>
@@ -12570,67 +12571,67 @@
         <f t="shared" si="29"/>
         <v>28.033333338098601</v>
       </c>
-      <c r="H139" s="93" t="str">
+      <c r="H139" s="88" t="str">
         <f t="shared" si="27"/>
         <v>20:56</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="114" t="s">
+      <c r="A140" s="109" t="s">
         <v>986</v>
       </c>
-      <c r="B140" s="97">
+      <c r="B140" s="92">
         <v>0</v>
       </c>
-      <c r="C140" s="103">
+      <c r="C140" s="98">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D140" s="97" t="s">
+      <c r="D140" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E140" s="104"/>
-      <c r="F140" s="104"/>
-      <c r="G140" s="104"/>
-      <c r="H140" s="105"/>
+      <c r="E140" s="99"/>
+      <c r="F140" s="99"/>
+      <c r="G140" s="99"/>
+      <c r="H140" s="100"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="97" t="s">
+      <c r="A141" s="92" t="s">
         <v>1081</v>
       </c>
-      <c r="B141" s="97">
+      <c r="B141" s="92">
         <v>0</v>
       </c>
-      <c r="C141" s="100">
+      <c r="C141" s="95">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D141" s="97" t="s">
+      <c r="D141" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E141" s="101"/>
-      <c r="F141" s="101"/>
-      <c r="G141" s="101"/>
-      <c r="H141" s="102"/>
+      <c r="E141" s="96"/>
+      <c r="F141" s="96"/>
+      <c r="G141" s="96"/>
+      <c r="H141" s="97"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="98" t="s">
+      <c r="A142" s="93" t="s">
         <v>1083</v>
       </c>
-      <c r="B142" s="97">
+      <c r="B142" s="92">
         <v>0</v>
       </c>
-      <c r="C142" s="103">
+      <c r="C142" s="98">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D142" s="97" t="s">
+      <c r="D142" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="E142" s="104"/>
-      <c r="F142" s="104"/>
-      <c r="G142" s="104"/>
-      <c r="H142" s="105"/>
+      <c r="E142" s="99"/>
+      <c r="F142" s="99"/>
+      <c r="G142" s="99"/>
+      <c r="H142" s="100"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18633,7 +18634,7 @@
       <c r="AX83" t="s">
         <v>1063</v>
       </c>
-      <c r="BA83" s="113">
+      <c r="BA83" s="108">
         <f>(13-4)/13</f>
         <v>0.69230769230769229</v>
       </c>
@@ -18696,7 +18697,7 @@
       <c r="AX84" t="s">
         <v>1073</v>
       </c>
-      <c r="BA84" s="113">
+      <c r="BA84" s="108">
         <f t="shared" ref="BA84:BA87" si="2">(13-4)/13</f>
         <v>0.69230769230769229</v>
       </c>
@@ -18759,7 +18760,7 @@
       <c r="AX85" t="s">
         <v>1046</v>
       </c>
-      <c r="BA85" s="113">
+      <c r="BA85" s="108">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -18822,7 +18823,7 @@
       <c r="AX86" t="s">
         <v>1046</v>
       </c>
-      <c r="BA86" s="113">
+      <c r="BA86" s="108">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -18885,7 +18886,7 @@
       <c r="AX87" t="s">
         <v>1063</v>
       </c>
-      <c r="BA87" s="113">
+      <c r="BA87" s="108">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -18911,7 +18912,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18934,7 +18935,7 @@
         <v>63</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C3" s="81" t="s">
         <v>988</v>
@@ -18945,10 +18946,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>1084</v>
+        <v>1099</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>1085</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -19026,9 +19027,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6358CC-62AD-AF43-A08A-FACC5983B0AF}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19037,15 +19040,15 @@
     <col min="3" max="14" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B1" s="22"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C2" s="59" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="D2" s="59" t="s">
         <v>16</v>
@@ -19063,7 +19066,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="59" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="J2" s="59" t="s">
         <v>21</v>
@@ -19078,677 +19081,718 @@
         <v>24</v>
       </c>
       <c r="N2" s="59" t="s">
+        <v>1091</v>
+      </c>
+      <c r="O2" s="59" t="s">
+        <v>1093</v>
+      </c>
+      <c r="P2" s="59" t="s">
         <v>1094</v>
       </c>
-      <c r="O2" s="59" t="s">
-        <v>1096</v>
-      </c>
-      <c r="P2" s="59" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B3" s="124" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C3" s="125">
+      <c r="Q2" s="121" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="119" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C3" s="120">
         <v>1</v>
       </c>
-      <c r="D3" s="125">
+      <c r="D3" s="120">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="E3" s="125">
+      <c r="E3" s="120">
         <f t="shared" ref="E3:N3" si="0">D3+1</f>
         <v>3</v>
       </c>
-      <c r="F3" s="125">
+      <c r="F3" s="120">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G3" s="125">
+      <c r="G3" s="120">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H3" s="125">
+      <c r="H3" s="120">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I3" s="125">
+      <c r="I3" s="120">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J3" s="125">
+      <c r="J3" s="120">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K3" s="125">
+      <c r="K3" s="120">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L3" s="125">
+      <c r="L3" s="120">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M3" s="125">
+      <c r="M3" s="120">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N3" s="125">
+      <c r="N3" s="120">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O3" s="125">
-        <f t="shared" ref="O3:P3" si="1">N3+1</f>
+      <c r="O3" s="120">
+        <f t="shared" ref="O3" si="1">N3+1</f>
         <v>13</v>
       </c>
-      <c r="P3" s="125">
-        <f t="shared" si="1"/>
+      <c r="P3" s="120">
+        <f t="shared" ref="P3" si="2">O3+1</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="122" t="s">
+      <c r="Q3" s="120">
+        <f t="shared" ref="Q3" si="3">P3+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="120">
+      <c r="C4" s="115">
         <v>44580</v>
       </c>
-      <c r="D4" s="120">
+      <c r="D4" s="115">
         <f>C4+7</f>
         <v>44587</v>
       </c>
-      <c r="E4" s="120">
-        <f t="shared" ref="E4:M4" si="2">D4+7</f>
+      <c r="E4" s="115">
+        <f t="shared" ref="E4:M4" si="4">D4+7</f>
         <v>44594</v>
       </c>
-      <c r="F4" s="120">
-        <f t="shared" si="2"/>
+      <c r="F4" s="115">
+        <f t="shared" si="4"/>
         <v>44601</v>
       </c>
-      <c r="G4" s="120">
-        <f t="shared" si="2"/>
+      <c r="G4" s="115">
+        <f t="shared" si="4"/>
         <v>44608</v>
       </c>
-      <c r="H4" s="120">
-        <f t="shared" si="2"/>
+      <c r="H4" s="115">
+        <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="I4" s="120">
-        <f t="shared" si="2"/>
+      <c r="I4" s="115">
+        <f t="shared" si="4"/>
         <v>44622</v>
       </c>
-      <c r="J4" s="120">
-        <f t="shared" si="2"/>
+      <c r="J4" s="115">
+        <f t="shared" si="4"/>
         <v>44629</v>
       </c>
-      <c r="K4" s="120">
-        <f t="shared" si="2"/>
+      <c r="K4" s="115">
+        <f t="shared" si="4"/>
         <v>44636</v>
       </c>
-      <c r="L4" s="120">
-        <f t="shared" si="2"/>
+      <c r="L4" s="115">
+        <f t="shared" si="4"/>
         <v>44643</v>
       </c>
-      <c r="M4" s="120">
-        <f t="shared" si="2"/>
+      <c r="M4" s="115">
+        <f t="shared" si="4"/>
         <v>44650</v>
       </c>
-      <c r="N4" s="120">
-        <f t="shared" ref="N4:O4" si="3">M4+7</f>
+      <c r="N4" s="115">
+        <f t="shared" ref="N4:O4" si="5">M4+7</f>
         <v>44657</v>
       </c>
-      <c r="O4" s="120">
-        <f t="shared" si="3"/>
+      <c r="O4" s="115">
+        <f t="shared" si="5"/>
         <v>44664</v>
       </c>
-      <c r="P4" s="120">
-        <f t="shared" ref="P4" si="4">O4+7</f>
+      <c r="P4" s="115">
+        <f t="shared" ref="P4:Q4" si="6">O4+7</f>
         <v>44671</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="123">
+      <c r="Q4" s="115">
+        <f t="shared" si="6"/>
+        <v>44678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="118">
         <v>220981245</v>
       </c>
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="121">
+      <c r="C5" s="116">
         <v>1</v>
       </c>
-      <c r="D5" s="121">
+      <c r="D5" s="116">
         <v>1</v>
       </c>
-      <c r="E5" s="121">
+      <c r="E5" s="116">
         <v>1</v>
       </c>
-      <c r="F5" s="121">
+      <c r="F5" s="116">
         <v>1</v>
       </c>
-      <c r="G5" s="121">
+      <c r="G5" s="116">
         <v>1</v>
       </c>
-      <c r="H5" s="121">
+      <c r="H5" s="116">
         <v>1</v>
       </c>
-      <c r="I5" s="121">
+      <c r="I5" s="116">
         <v>1</v>
       </c>
-      <c r="J5" s="121">
+      <c r="J5" s="116">
         <v>1</v>
       </c>
-      <c r="K5" s="121">
+      <c r="K5" s="116">
         <v>1</v>
       </c>
-      <c r="L5" s="121">
+      <c r="L5" s="116">
         <v>1</v>
       </c>
-      <c r="M5" s="121">
+      <c r="M5" s="116">
         <v>1</v>
       </c>
-      <c r="N5" s="121">
+      <c r="N5" s="116">
         <v>1</v>
       </c>
-      <c r="O5" s="121" t="s">
+      <c r="O5" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P5" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q5" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="118">
+        <v>399515449</v>
+      </c>
+      <c r="B6" s="118" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="116">
+        <v>1</v>
+      </c>
+      <c r="D6" s="116">
+        <v>1</v>
+      </c>
+      <c r="E6" s="116">
+        <v>1</v>
+      </c>
+      <c r="F6" s="116">
+        <v>1</v>
+      </c>
+      <c r="G6" s="116">
+        <v>1</v>
+      </c>
+      <c r="H6" s="116">
+        <v>1</v>
+      </c>
+      <c r="I6" s="116">
+        <v>1</v>
+      </c>
+      <c r="J6" s="116">
+        <v>1</v>
+      </c>
+      <c r="K6" s="116">
+        <v>1</v>
+      </c>
+      <c r="L6" s="116">
+        <v>1</v>
+      </c>
+      <c r="M6" s="116">
+        <v>1</v>
+      </c>
+      <c r="N6" s="116">
+        <v>1</v>
+      </c>
+      <c r="O6" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P6" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q6" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="118">
+        <v>207595964</v>
+      </c>
+      <c r="B7" s="118" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="116">
+        <v>1</v>
+      </c>
+      <c r="D7" s="116">
+        <v>1</v>
+      </c>
+      <c r="E7" s="116">
+        <v>1</v>
+      </c>
+      <c r="F7" s="116">
+        <v>1</v>
+      </c>
+      <c r="G7" s="116">
+        <v>1</v>
+      </c>
+      <c r="H7" s="116">
+        <v>1</v>
+      </c>
+      <c r="I7" s="116">
+        <v>1</v>
+      </c>
+      <c r="J7" s="116">
+        <v>1</v>
+      </c>
+      <c r="K7" s="116">
+        <v>1</v>
+      </c>
+      <c r="L7" s="116">
+        <v>1</v>
+      </c>
+      <c r="M7" s="116">
+        <v>1</v>
+      </c>
+      <c r="N7" s="116">
+        <v>1</v>
+      </c>
+      <c r="O7" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P7" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q7" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="118">
+        <v>211776124</v>
+      </c>
+      <c r="B8" s="118" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="116">
+        <v>1</v>
+      </c>
+      <c r="D8" s="116">
+        <v>1</v>
+      </c>
+      <c r="E8" s="116">
+        <v>1</v>
+      </c>
+      <c r="F8" s="116">
+        <v>1</v>
+      </c>
+      <c r="G8" s="116">
+        <v>1</v>
+      </c>
+      <c r="H8" s="116">
+        <v>1</v>
+      </c>
+      <c r="I8" s="116">
+        <v>1</v>
+      </c>
+      <c r="J8" s="116">
+        <v>1</v>
+      </c>
+      <c r="K8" s="116">
+        <v>1</v>
+      </c>
+      <c r="L8" s="116">
+        <v>1</v>
+      </c>
+      <c r="M8" s="116">
+        <v>1</v>
+      </c>
+      <c r="N8" s="116">
+        <v>1</v>
+      </c>
+      <c r="O8" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P8" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q8" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="118">
+        <v>220981202</v>
+      </c>
+      <c r="B9" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="116">
+        <v>1</v>
+      </c>
+      <c r="D9" s="116">
+        <v>1</v>
+      </c>
+      <c r="E9" s="116">
+        <v>1</v>
+      </c>
+      <c r="F9" s="116">
+        <v>1</v>
+      </c>
+      <c r="G9" s="116">
+        <v>1</v>
+      </c>
+      <c r="H9" s="116">
+        <v>1</v>
+      </c>
+      <c r="I9" s="116">
+        <v>1</v>
+      </c>
+      <c r="J9" s="116">
+        <v>0</v>
+      </c>
+      <c r="K9" s="116">
+        <v>0</v>
+      </c>
+      <c r="L9" s="116">
+        <v>1</v>
+      </c>
+      <c r="M9" s="116">
+        <v>1</v>
+      </c>
+      <c r="N9" s="116">
+        <v>1</v>
+      </c>
+      <c r="O9" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P9" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q9" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="118">
+        <v>398813438</v>
+      </c>
+      <c r="B10" s="118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="116">
+        <v>1</v>
+      </c>
+      <c r="D10" s="116">
+        <v>1</v>
+      </c>
+      <c r="E10" s="116">
+        <v>1</v>
+      </c>
+      <c r="F10" s="116">
+        <v>1</v>
+      </c>
+      <c r="G10" s="116">
+        <v>1</v>
+      </c>
+      <c r="H10" s="116">
+        <v>1</v>
+      </c>
+      <c r="I10" s="116">
+        <v>1</v>
+      </c>
+      <c r="J10" s="116">
+        <v>1</v>
+      </c>
+      <c r="K10" s="116">
+        <v>1</v>
+      </c>
+      <c r="L10" s="116">
+        <v>1</v>
+      </c>
+      <c r="M10" s="116">
+        <v>1</v>
+      </c>
+      <c r="N10" s="116">
+        <v>1</v>
+      </c>
+      <c r="O10" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P10" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q10" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="118">
+        <v>220981261</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="116">
+        <v>1</v>
+      </c>
+      <c r="D11" s="116">
+        <v>1</v>
+      </c>
+      <c r="E11" s="116">
+        <v>1</v>
+      </c>
+      <c r="F11" s="116">
+        <v>1</v>
+      </c>
+      <c r="G11" s="116">
+        <v>1</v>
+      </c>
+      <c r="H11" s="116">
+        <v>1</v>
+      </c>
+      <c r="I11" s="116">
+        <v>1</v>
+      </c>
+      <c r="J11" s="116">
+        <v>1</v>
+      </c>
+      <c r="K11" s="116">
+        <v>1</v>
+      </c>
+      <c r="L11" s="116">
+        <v>1</v>
+      </c>
+      <c r="M11" s="116">
+        <v>0</v>
+      </c>
+      <c r="N11" s="116">
+        <v>1</v>
+      </c>
+      <c r="O11" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P11" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q11" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="118">
+        <v>220981296</v>
+      </c>
+      <c r="B12" s="118" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="116">
+        <v>1</v>
+      </c>
+      <c r="D12" s="116">
+        <v>1</v>
+      </c>
+      <c r="E12" s="116">
+        <v>1</v>
+      </c>
+      <c r="F12" s="116">
+        <v>1</v>
+      </c>
+      <c r="G12" s="116">
+        <v>1</v>
+      </c>
+      <c r="H12" s="116">
+        <v>1</v>
+      </c>
+      <c r="I12" s="116">
+        <v>1</v>
+      </c>
+      <c r="J12" s="116">
+        <v>1</v>
+      </c>
+      <c r="K12" s="116">
+        <v>1</v>
+      </c>
+      <c r="L12" s="116">
+        <v>1</v>
+      </c>
+      <c r="M12" s="116">
+        <v>1</v>
+      </c>
+      <c r="N12" s="116">
+        <v>1</v>
+      </c>
+      <c r="O12" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P12" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q12" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="118">
+        <v>220981229</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="116">
+        <v>1</v>
+      </c>
+      <c r="D13" s="116">
+        <v>1</v>
+      </c>
+      <c r="E13" s="116">
+        <v>1</v>
+      </c>
+      <c r="F13" s="116">
+        <v>1</v>
+      </c>
+      <c r="G13" s="116">
+        <v>0</v>
+      </c>
+      <c r="H13" s="116">
+        <v>1</v>
+      </c>
+      <c r="I13" s="116">
+        <v>1</v>
+      </c>
+      <c r="J13" s="116">
+        <v>1</v>
+      </c>
+      <c r="K13" s="116">
+        <v>1</v>
+      </c>
+      <c r="L13" s="116">
+        <v>0</v>
+      </c>
+      <c r="M13" s="116">
+        <v>0</v>
+      </c>
+      <c r="N13" s="116">
+        <v>1</v>
+      </c>
+      <c r="O13" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P13" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q13" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="118">
+        <v>220981288</v>
+      </c>
+      <c r="B14" s="118" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="116">
+        <v>1</v>
+      </c>
+      <c r="D14" s="116">
+        <v>1</v>
+      </c>
+      <c r="E14" s="116">
+        <v>1</v>
+      </c>
+      <c r="F14" s="116">
+        <v>1</v>
+      </c>
+      <c r="G14" s="116">
+        <v>1</v>
+      </c>
+      <c r="H14" s="116">
+        <v>1</v>
+      </c>
+      <c r="I14" s="116">
+        <v>1</v>
+      </c>
+      <c r="J14" s="116">
+        <v>1</v>
+      </c>
+      <c r="K14" s="116">
+        <v>1</v>
+      </c>
+      <c r="L14" s="116">
+        <v>1</v>
+      </c>
+      <c r="M14" s="116">
+        <v>1</v>
+      </c>
+      <c r="N14" s="116">
+        <v>1</v>
+      </c>
+      <c r="O14" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="P14" s="116" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q14" s="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="113" t="s">
         <v>1095</v>
       </c>
-      <c r="P5" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="123">
-        <v>399515449</v>
-      </c>
-      <c r="B6" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="121">
-        <v>1</v>
-      </c>
-      <c r="D6" s="121">
-        <v>1</v>
-      </c>
-      <c r="E6" s="121">
-        <v>1</v>
-      </c>
-      <c r="F6" s="121">
-        <v>1</v>
-      </c>
-      <c r="G6" s="121">
-        <v>1</v>
-      </c>
-      <c r="H6" s="121">
-        <v>1</v>
-      </c>
-      <c r="I6" s="121">
-        <v>1</v>
-      </c>
-      <c r="J6" s="121">
-        <v>1</v>
-      </c>
-      <c r="K6" s="121">
-        <v>1</v>
-      </c>
-      <c r="L6" s="121">
-        <v>1</v>
-      </c>
-      <c r="M6" s="121">
-        <v>1</v>
-      </c>
-      <c r="N6" s="121">
-        <v>1</v>
-      </c>
-      <c r="O6" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P6" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="123">
-        <v>207595964</v>
-      </c>
-      <c r="B7" s="123" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="121">
-        <v>1</v>
-      </c>
-      <c r="D7" s="121">
-        <v>1</v>
-      </c>
-      <c r="E7" s="121">
-        <v>1</v>
-      </c>
-      <c r="F7" s="121">
-        <v>1</v>
-      </c>
-      <c r="G7" s="121">
-        <v>1</v>
-      </c>
-      <c r="H7" s="121">
-        <v>1</v>
-      </c>
-      <c r="I7" s="121">
-        <v>1</v>
-      </c>
-      <c r="J7" s="121">
-        <v>1</v>
-      </c>
-      <c r="K7" s="121">
-        <v>1</v>
-      </c>
-      <c r="L7" s="121">
-        <v>1</v>
-      </c>
-      <c r="M7" s="121">
-        <v>1</v>
-      </c>
-      <c r="N7" s="121">
-        <v>1</v>
-      </c>
-      <c r="O7" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P7" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="123">
-        <v>211776124</v>
-      </c>
-      <c r="B8" s="123" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="121">
-        <v>1</v>
-      </c>
-      <c r="D8" s="121">
-        <v>1</v>
-      </c>
-      <c r="E8" s="121">
-        <v>1</v>
-      </c>
-      <c r="F8" s="121">
-        <v>1</v>
-      </c>
-      <c r="G8" s="121">
-        <v>1</v>
-      </c>
-      <c r="H8" s="121">
-        <v>1</v>
-      </c>
-      <c r="I8" s="121">
-        <v>1</v>
-      </c>
-      <c r="J8" s="121">
-        <v>1</v>
-      </c>
-      <c r="K8" s="121">
-        <v>1</v>
-      </c>
-      <c r="L8" s="121">
-        <v>1</v>
-      </c>
-      <c r="M8" s="121">
-        <v>1</v>
-      </c>
-      <c r="N8" s="121">
-        <v>1</v>
-      </c>
-      <c r="O8" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P8" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="123">
-        <v>220981202</v>
-      </c>
-      <c r="B9" s="123" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="121">
-        <v>1</v>
-      </c>
-      <c r="D9" s="121">
-        <v>1</v>
-      </c>
-      <c r="E9" s="121">
-        <v>1</v>
-      </c>
-      <c r="F9" s="121">
-        <v>1</v>
-      </c>
-      <c r="G9" s="121">
-        <v>1</v>
-      </c>
-      <c r="H9" s="121">
-        <v>1</v>
-      </c>
-      <c r="I9" s="121">
-        <v>1</v>
-      </c>
-      <c r="J9" s="121">
-        <v>0</v>
-      </c>
-      <c r="K9" s="121">
-        <v>0</v>
-      </c>
-      <c r="L9" s="121">
-        <v>1</v>
-      </c>
-      <c r="M9" s="121">
-        <v>1</v>
-      </c>
-      <c r="N9" s="121">
-        <v>1</v>
-      </c>
-      <c r="O9" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P9" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="123">
-        <v>398813438</v>
-      </c>
-      <c r="B10" s="123" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="121">
-        <v>1</v>
-      </c>
-      <c r="D10" s="121">
-        <v>1</v>
-      </c>
-      <c r="E10" s="121">
-        <v>1</v>
-      </c>
-      <c r="F10" s="121">
-        <v>1</v>
-      </c>
-      <c r="G10" s="121">
-        <v>1</v>
-      </c>
-      <c r="H10" s="121">
-        <v>1</v>
-      </c>
-      <c r="I10" s="121">
-        <v>1</v>
-      </c>
-      <c r="J10" s="121">
-        <v>1</v>
-      </c>
-      <c r="K10" s="121">
-        <v>1</v>
-      </c>
-      <c r="L10" s="121">
-        <v>1</v>
-      </c>
-      <c r="M10" s="121">
-        <v>1</v>
-      </c>
-      <c r="N10" s="121">
-        <v>1</v>
-      </c>
-      <c r="O10" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P10" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="123">
-        <v>220981261</v>
-      </c>
-      <c r="B11" s="123" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="121">
-        <v>1</v>
-      </c>
-      <c r="D11" s="121">
-        <v>1</v>
-      </c>
-      <c r="E11" s="121">
-        <v>1</v>
-      </c>
-      <c r="F11" s="121">
-        <v>1</v>
-      </c>
-      <c r="G11" s="121">
-        <v>1</v>
-      </c>
-      <c r="H11" s="121">
-        <v>1</v>
-      </c>
-      <c r="I11" s="121">
-        <v>1</v>
-      </c>
-      <c r="J11" s="121">
-        <v>1</v>
-      </c>
-      <c r="K11" s="121">
-        <v>1</v>
-      </c>
-      <c r="L11" s="121">
-        <v>1</v>
-      </c>
-      <c r="M11" s="121">
-        <v>0</v>
-      </c>
-      <c r="N11" s="121">
-        <v>1</v>
-      </c>
-      <c r="O11" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P11" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="123">
-        <v>220981296</v>
-      </c>
-      <c r="B12" s="123" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="121">
-        <v>1</v>
-      </c>
-      <c r="D12" s="121">
-        <v>1</v>
-      </c>
-      <c r="E12" s="121">
-        <v>1</v>
-      </c>
-      <c r="F12" s="121">
-        <v>1</v>
-      </c>
-      <c r="G12" s="121">
-        <v>1</v>
-      </c>
-      <c r="H12" s="121">
-        <v>1</v>
-      </c>
-      <c r="I12" s="121">
-        <v>1</v>
-      </c>
-      <c r="J12" s="121">
-        <v>1</v>
-      </c>
-      <c r="K12" s="121">
-        <v>1</v>
-      </c>
-      <c r="L12" s="121">
-        <v>1</v>
-      </c>
-      <c r="M12" s="121">
-        <v>1</v>
-      </c>
-      <c r="N12" s="121">
-        <v>1</v>
-      </c>
-      <c r="O12" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P12" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="123">
-        <v>220981229</v>
-      </c>
-      <c r="B13" s="123" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="121">
-        <v>1</v>
-      </c>
-      <c r="D13" s="121">
-        <v>1</v>
-      </c>
-      <c r="E13" s="121">
-        <v>1</v>
-      </c>
-      <c r="F13" s="121">
-        <v>1</v>
-      </c>
-      <c r="G13" s="121">
-        <v>0</v>
-      </c>
-      <c r="H13" s="121">
-        <v>1</v>
-      </c>
-      <c r="I13" s="121">
-        <v>1</v>
-      </c>
-      <c r="J13" s="121">
-        <v>1</v>
-      </c>
-      <c r="K13" s="121">
-        <v>1</v>
-      </c>
-      <c r="L13" s="121">
-        <v>0</v>
-      </c>
-      <c r="M13" s="121">
-        <v>0</v>
-      </c>
-      <c r="N13" s="121">
-        <v>1</v>
-      </c>
-      <c r="O13" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P13" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="123">
-        <v>220981288</v>
-      </c>
-      <c r="B14" s="123" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="121">
-        <v>1</v>
-      </c>
-      <c r="D14" s="121">
-        <v>1</v>
-      </c>
-      <c r="E14" s="121">
-        <v>1</v>
-      </c>
-      <c r="F14" s="121">
-        <v>1</v>
-      </c>
-      <c r="G14" s="121">
-        <v>1</v>
-      </c>
-      <c r="H14" s="121">
-        <v>1</v>
-      </c>
-      <c r="I14" s="121">
-        <v>1</v>
-      </c>
-      <c r="J14" s="121">
-        <v>1</v>
-      </c>
-      <c r="K14" s="121">
-        <v>1</v>
-      </c>
-      <c r="L14" s="121">
-        <v>1</v>
-      </c>
-      <c r="M14" s="121">
-        <v>1</v>
-      </c>
-      <c r="N14" s="121">
-        <v>1</v>
-      </c>
-      <c r="O14" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P14" s="121" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="118" t="s">
-        <v>1098</v>
-      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="119"/>
+      <c r="C19" s="114"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="119"/>
+      <c r="C20" s="114"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="119"/>
+      <c r="C21" s="114"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="119"/>
+      <c r="C22" s="114"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="119"/>
+      <c r="C23" s="114"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="119"/>
+      <c r="C24" s="114"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="119"/>
+      <c r="C25" s="114"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="119"/>
+      <c r="C26" s="114"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="119"/>
+      <c r="C27" s="114"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="119"/>
+      <c r="C28" s="114"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Cambiar calificaciones por calif ponderada
</commit_message>
<xml_diff>
--- a/grades/Calificaciones.xlsx
+++ b/grades/Calificaciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/02_Studies/2022_MCD_UDG/03_Desarrollo_proyectos_II/2022-s1_Material_Vic/05_Calificaciones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/05_Projects_levic/Projects_git/UDG_MCD_Project_Dev_II/grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C440307C-9EAE-3A46-928A-C9FFCB72B25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57077510-84EB-8542-9E1F-8656FCBE4AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
   </bookViews>
@@ -3871,7 +3871,7 @@
     <t>Exposición en congreso, publicación</t>
   </si>
   <si>
-    <t>Puntos acumulados al 2022-04-27</t>
+    <t>2022-04-27</t>
   </si>
 </sst>
 </file>
@@ -4431,7 +4431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4573,7 +4573,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4609,7 +4608,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4653,6 +4651,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7514,15 +7525,15 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" style="23" customWidth="1"/>
     <col min="2" max="2" width="27" style="23" customWidth="1"/>
-    <col min="3" max="8" width="16.5" style="17" customWidth="1"/>
-    <col min="9" max="9" width="0" style="17" hidden="1" customWidth="1"/>
+    <col min="3" max="8" width="15.6640625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="140.5" style="17" hidden="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
@@ -7534,408 +7545,408 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="str">
-        <f>RESUMEN!A40</f>
+        <f>"Puntos acumulados al " &amp; RESUMEN!A40</f>
         <v>Puntos acumulados al 2022-04-27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I3" s="86" t="str">
+      <c r="I3" s="85" t="str">
         <f>"|"&amp;A4&amp;"|"&amp;B4&amp;"|"&amp;C4&amp;"|"&amp;D4&amp;"|"&amp;E4&amp;"|"&amp;F4&amp;"|"&amp;G4&amp;"|__"&amp;H4&amp;"__|"</f>
         <v>|Id. estudiante|Nombre|EXPOSICIONES (30%)|QUIZES (CONTROLES DE LECTURA, 30%)|TAREAS (20%)|EXAMEN FINAL (20%)|PUNTOS EXTRAS|__CALIF. FINAL__|</v>
       </c>
     </row>
-    <row r="4" spans="1:9" customFormat="1" ht="56" x14ac:dyDescent="0.2">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:9" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A4" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="122" t="s">
+      <c r="C4" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="121" t="s">
         <v>991</v>
       </c>
-      <c r="E4" s="124" t="s">
+      <c r="E4" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="123" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="126" t="s">
+      <c r="H4" s="124" t="s">
         <v>990</v>
       </c>
-      <c r="I4" s="110" t="str">
+      <c r="I4" s="108" t="str">
         <f>"|---|---|---|---|---|---|---|---|"</f>
         <v>|---|---|---|---|---|---|---|---|</v>
       </c>
     </row>
     <row r="5" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82">
+      <c r="A5" s="128">
         <v>220981245</v>
       </c>
       <c r="B5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="107">
-        <f>RESUMEN!F5</f>
-        <v>100</v>
-      </c>
-      <c r="D5" s="107">
-        <f>RESUMEN!Q5</f>
-        <v>100</v>
-      </c>
-      <c r="E5" s="107">
-        <f>RESUMEN!AC5</f>
-        <v>100</v>
-      </c>
-      <c r="F5" s="107">
-        <f>RESUMEN!AD5</f>
+      <c r="C5" s="126">
+        <f>RESUMEN!F5*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D5" s="126">
+        <f>RESUMEN!Q5*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="E5" s="126">
+        <f>RESUMEN!AC5*0.2</f>
+        <v>20</v>
+      </c>
+      <c r="F5" s="126">
+        <f>RESUMEN!AD5*0.2</f>
         <v>0</v>
       </c>
-      <c r="G5" s="107">
+      <c r="G5" s="126">
         <f>RESUMEN!C24</f>
         <v>10</v>
       </c>
-      <c r="H5" s="85">
-        <f t="shared" ref="H5:H14" si="0">C5*0.3+D5*0.3+E5*0.2+F5*0.2+G5</f>
+      <c r="H5" s="127">
+        <f>SUM(C5:G5)</f>
         <v>90</v>
       </c>
-      <c r="I5" s="86" t="str">
+      <c r="I5" s="85" t="str">
         <f>"|"&amp;A5&amp;"|"&amp;B5&amp;"|"&amp;ROUND(C5,1)&amp;"|"&amp;ROUND(D5,1)&amp;"|"&amp;ROUND(E5,1)&amp;"|"&amp;ROUND(F5,1)&amp;"|"&amp;ROUND(G5,1)&amp;"|__"&amp;ROUND(H5,1)&amp;"__|"</f>
-        <v>|220981245|José Raúl Castro Esparza|100|100|100|0|10|__90__|</v>
+        <v>|220981245|José Raúl Castro Esparza|30|30|20|0|10|__90__|</v>
       </c>
     </row>
     <row r="6" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="82">
+      <c r="A6" s="128">
         <v>399515449</v>
       </c>
       <c r="B6" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="107">
-        <f>RESUMEN!F6</f>
-        <v>100</v>
-      </c>
-      <c r="D6" s="107">
-        <f>RESUMEN!Q6</f>
-        <v>100</v>
-      </c>
-      <c r="E6" s="107">
-        <f>RESUMEN!AC6</f>
-        <v>100</v>
-      </c>
-      <c r="F6" s="107">
-        <f>RESUMEN!AD6</f>
+      <c r="C6" s="126">
+        <f>RESUMEN!F6*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D6" s="126">
+        <f>RESUMEN!Q6*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="E6" s="126">
+        <f>RESUMEN!AC6*0.2</f>
+        <v>20</v>
+      </c>
+      <c r="F6" s="126">
+        <f>RESUMEN!AD6*0.2</f>
         <v>0</v>
       </c>
-      <c r="G6" s="107">
+      <c r="G6" s="126">
         <f>RESUMEN!C25</f>
         <v>0</v>
       </c>
-      <c r="H6" s="85">
+      <c r="H6" s="127">
+        <f t="shared" ref="H6:H14" si="0">SUM(C6:G6)</f>
+        <v>80</v>
+      </c>
+      <c r="I6" s="85" t="str">
+        <f t="shared" ref="I6:I14" si="1">"|"&amp;A6&amp;"|"&amp;B6&amp;"|"&amp;ROUND(C6,1)&amp;"|"&amp;ROUND(D6,1)&amp;"|"&amp;ROUND(E6,1)&amp;"|"&amp;ROUND(F6,1)&amp;"|"&amp;ROUND(G6,1)&amp;"|__"&amp;ROUND(H6,1)&amp;"__|"</f>
+        <v>|399515449|Martha Olivia Ramos Lara|30|30|20|0|0|__80__|</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="128">
+        <v>207595964</v>
+      </c>
+      <c r="B7" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="126">
+        <f>RESUMEN!F7*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D7" s="126">
+        <f>RESUMEN!Q7*0.3</f>
+        <v>27.444444444444439</v>
+      </c>
+      <c r="E7" s="126">
+        <f>RESUMEN!AC7*0.2</f>
+        <v>17.72187878787879</v>
+      </c>
+      <c r="F7" s="126">
+        <f>RESUMEN!AD7*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="126">
+        <f>RESUMEN!C26</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="127">
+        <f t="shared" si="0"/>
+        <v>75.166323232323236</v>
+      </c>
+      <c r="I7" s="85" t="str">
+        <f t="shared" si="1"/>
+        <v>|207595964|Carol Desireé Ramírez Durán|30|27.4|17.7|0|0|__75.2__|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="128">
+        <v>211776124</v>
+      </c>
+      <c r="B8" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="126">
+        <f>RESUMEN!F8*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D8" s="126">
+        <f>RESUMEN!Q8*0.3</f>
+        <v>25.444555555555549</v>
+      </c>
+      <c r="E8" s="126">
+        <f>RESUMEN!AC8*0.2</f>
+        <v>17.72187878787879</v>
+      </c>
+      <c r="F8" s="126">
+        <f>RESUMEN!AD8*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="126">
+        <f>RESUMEN!C27</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="127">
+        <f t="shared" si="0"/>
+        <v>73.166434343434346</v>
+      </c>
+      <c r="I8" s="85" t="str">
+        <f t="shared" si="1"/>
+        <v>|211776124|César Iván Vargas López|30|25.4|17.7|0|0|__73.2__|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="128">
+        <v>220981202</v>
+      </c>
+      <c r="B9" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="126">
+        <f>RESUMEN!F9*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D9" s="126">
+        <f>RESUMEN!Q9*0.3</f>
+        <v>23.555499999999999</v>
+      </c>
+      <c r="E9" s="126">
+        <f>RESUMEN!AC9*0.2</f>
+        <v>20</v>
+      </c>
+      <c r="F9" s="126">
+        <f>RESUMEN!AD9*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="126">
+        <f>RESUMEN!C28</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="127">
+        <f t="shared" si="0"/>
+        <v>73.555499999999995</v>
+      </c>
+      <c r="I9" s="85" t="str">
+        <f t="shared" si="1"/>
+        <v>|220981202|Pedro Martínez Ayala|30|23.6|20|0|0|__73.6__|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="128">
+        <v>398813438</v>
+      </c>
+      <c r="B10" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="126">
+        <f>RESUMEN!F10*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D10" s="126">
+        <f>RESUMEN!Q10*0.3</f>
+        <v>30.000000000000004</v>
+      </c>
+      <c r="E10" s="126">
+        <f>RESUMEN!AC10*0.2</f>
+        <v>20</v>
+      </c>
+      <c r="F10" s="126">
+        <f>RESUMEN!AD10*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="126">
+        <f>RESUMEN!C29</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="127">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I6" s="86" t="str">
-        <f t="shared" ref="I6:I14" si="1">"|"&amp;A6&amp;"|"&amp;B6&amp;"|"&amp;ROUND(C6,1)&amp;"|"&amp;ROUND(D6,1)&amp;"|"&amp;ROUND(E6,1)&amp;"|"&amp;ROUND(F6,1)&amp;"|"&amp;ROUND(G6,1)&amp;"|__"&amp;ROUND(H6,1)&amp;"__|"</f>
-        <v>|399515449|Martha Olivia Ramos Lara|100|100|100|0|0|__80__|</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="82">
-        <v>207595964</v>
-      </c>
-      <c r="B7" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="107">
-        <f>RESUMEN!F7</f>
-        <v>100</v>
-      </c>
-      <c r="D7" s="107">
-        <f>RESUMEN!Q7</f>
-        <v>91.481481481481467</v>
-      </c>
-      <c r="E7" s="107">
-        <f>RESUMEN!AC7</f>
-        <v>88.609393939393939</v>
-      </c>
-      <c r="F7" s="107">
-        <f>RESUMEN!AD7</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="107">
-        <f>RESUMEN!C26</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="85">
-        <f t="shared" si="0"/>
-        <v>75.166323232323236</v>
-      </c>
-      <c r="I7" s="86" t="str">
+      <c r="I10" s="85" t="str">
         <f t="shared" si="1"/>
-        <v>|207595964|Carol Desireé Ramírez Durán|100|91.5|88.6|0|0|__75.2__|</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="82">
-        <v>211776124</v>
-      </c>
-      <c r="B8" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="107">
-        <f>RESUMEN!F8</f>
-        <v>100</v>
-      </c>
-      <c r="D8" s="107">
-        <f>RESUMEN!Q8</f>
-        <v>84.815185185185172</v>
-      </c>
-      <c r="E8" s="107">
-        <f>RESUMEN!AC8</f>
-        <v>88.609393939393939</v>
-      </c>
-      <c r="F8" s="107">
-        <f>RESUMEN!AD8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="107">
-        <f>RESUMEN!C27</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="85">
-        <f t="shared" si="0"/>
-        <v>73.166434343434346</v>
-      </c>
-      <c r="I8" s="86" t="str">
-        <f t="shared" si="1"/>
-        <v>|211776124|César Iván Vargas López|100|84.8|88.6|0|0|__73.2__|</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="82">
-        <v>220981202</v>
-      </c>
-      <c r="B9" s="82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="107">
-        <f>RESUMEN!F9</f>
-        <v>100</v>
-      </c>
-      <c r="D9" s="107">
-        <f>RESUMEN!Q9</f>
-        <v>78.518333333333331</v>
-      </c>
-      <c r="E9" s="107">
-        <f>RESUMEN!AC9</f>
-        <v>100</v>
-      </c>
-      <c r="F9" s="107">
-        <f>RESUMEN!AD9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="107">
-        <f>RESUMEN!C28</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="85">
-        <f t="shared" si="0"/>
-        <v>73.555499999999995</v>
-      </c>
-      <c r="I9" s="86" t="str">
-        <f t="shared" si="1"/>
-        <v>|220981202|Pedro Martínez Ayala|100|78.5|100|0|0|__73.6__|</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="82">
-        <v>398813438</v>
-      </c>
-      <c r="B10" s="82" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="107">
-        <f>RESUMEN!F10</f>
-        <v>100</v>
-      </c>
-      <c r="D10" s="107">
-        <f>RESUMEN!Q10</f>
-        <v>100.00000000000001</v>
-      </c>
-      <c r="E10" s="107">
-        <f>RESUMEN!AC10</f>
-        <v>100</v>
-      </c>
-      <c r="F10" s="107">
-        <f>RESUMEN!AD10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="107">
-        <f>RESUMEN!C29</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="85">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="I10" s="86" t="str">
-        <f t="shared" si="1"/>
-        <v>|398813438|Afra Julieta Lomelí Avila|100|100|100|0|0|__80__|</v>
+        <v>|398813438|Afra Julieta Lomelí Avila|30|30|20|0|0|__80__|</v>
       </c>
     </row>
     <row r="11" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="82">
+      <c r="A11" s="128">
         <v>220981261</v>
       </c>
       <c r="B11" s="82" t="s">
         <v>992</v>
       </c>
-      <c r="C11" s="107">
-        <f>RESUMEN!F11</f>
-        <v>100</v>
-      </c>
-      <c r="D11" s="107">
-        <f>RESUMEN!Q11</f>
-        <v>52.223703703703706</v>
-      </c>
-      <c r="E11" s="107">
-        <f>RESUMEN!AC11</f>
-        <v>91.612834224598927</v>
-      </c>
-      <c r="F11" s="107">
-        <f>RESUMEN!AD11</f>
+      <c r="C11" s="126">
+        <f>RESUMEN!F11*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D11" s="126">
+        <f>RESUMEN!Q11*0.3</f>
+        <v>15.667111111111112</v>
+      </c>
+      <c r="E11" s="126">
+        <f>RESUMEN!AC11*0.2</f>
+        <v>18.322566844919788</v>
+      </c>
+      <c r="F11" s="126">
+        <f>RESUMEN!AD11*0.2</f>
         <v>0</v>
       </c>
-      <c r="G11" s="107">
+      <c r="G11" s="126">
         <f>RESUMEN!C30</f>
         <v>0</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="127">
         <f t="shared" si="0"/>
         <v>63.989677956030903</v>
       </c>
-      <c r="I11" s="86" t="str">
+      <c r="I11" s="85" t="str">
         <f t="shared" si="1"/>
-        <v>|220981261|Mónica Alonso Soria|100|52.2|91.6|0|0|__64__|</v>
+        <v>|220981261|Mónica Alonso Soria|30|15.7|18.3|0|0|__64__|</v>
       </c>
     </row>
     <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="82">
+      <c r="A12" s="128">
         <v>220981296</v>
       </c>
       <c r="B12" s="82" t="s">
         <v>993</v>
       </c>
-      <c r="C12" s="107">
-        <f>RESUMEN!F12</f>
-        <v>100</v>
-      </c>
-      <c r="D12" s="107">
-        <f>RESUMEN!Q12</f>
-        <v>82.221851851851852</v>
-      </c>
-      <c r="E12" s="107">
-        <f>RESUMEN!AC12</f>
-        <v>91.612834224598927</v>
-      </c>
-      <c r="F12" s="107">
-        <f>RESUMEN!AD12</f>
+      <c r="C12" s="126">
+        <f>RESUMEN!F12*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D12" s="126">
+        <f>RESUMEN!Q12*0.3</f>
+        <v>24.666555555555554</v>
+      </c>
+      <c r="E12" s="126">
+        <f>RESUMEN!AC12*0.2</f>
+        <v>18.322566844919788</v>
+      </c>
+      <c r="F12" s="126">
+        <f>RESUMEN!AD12*0.2</f>
         <v>0</v>
       </c>
-      <c r="G12" s="107">
+      <c r="G12" s="126">
         <f>RESUMEN!C31</f>
         <v>0</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="127">
         <f t="shared" si="0"/>
         <v>72.989122400475338</v>
       </c>
-      <c r="I12" s="86" t="str">
+      <c r="I12" s="85" t="str">
         <f t="shared" si="1"/>
-        <v>|220981296|Mario Palomino Hernández|100|82.2|91.6|0|0|__73__|</v>
+        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|0|0|__73__|</v>
       </c>
     </row>
     <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82">
+      <c r="A13" s="128">
         <v>220981229</v>
       </c>
       <c r="B13" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="107">
-        <f>RESUMEN!F13</f>
-        <v>85</v>
-      </c>
-      <c r="D13" s="107">
-        <f>RESUMEN!Q13</f>
-        <v>64.258888888888876</v>
-      </c>
-      <c r="E13" s="107">
-        <f>RESUMEN!AC13</f>
-        <v>89.990909090909099</v>
-      </c>
-      <c r="F13" s="107">
-        <f>RESUMEN!AD13</f>
+      <c r="C13" s="126">
+        <f>RESUMEN!F13*0.3</f>
+        <v>25.5</v>
+      </c>
+      <c r="D13" s="126">
+        <f>RESUMEN!Q13*0.3</f>
+        <v>19.277666666666661</v>
+      </c>
+      <c r="E13" s="126">
+        <f>RESUMEN!AC13*0.2</f>
+        <v>17.99818181818182</v>
+      </c>
+      <c r="F13" s="126">
+        <f>RESUMEN!AD13*0.2</f>
         <v>0</v>
       </c>
-      <c r="G13" s="107">
+      <c r="G13" s="126">
         <f>RESUMEN!C32</f>
         <v>0</v>
       </c>
-      <c r="H13" s="85">
+      <c r="H13" s="127">
         <f t="shared" si="0"/>
         <v>62.775848484848481</v>
       </c>
-      <c r="I13" s="86" t="str">
+      <c r="I13" s="85" t="str">
         <f t="shared" si="1"/>
-        <v>|220981229|Luis Enrique Neri González|85|64.3|90|0|0|__62.8__|</v>
+        <v>|220981229|Luis Enrique Neri González|25.5|19.3|18|0|0|__62.8__|</v>
       </c>
     </row>
     <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82">
+      <c r="A14" s="128">
         <v>220981288</v>
       </c>
       <c r="B14" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="107">
-        <f>RESUMEN!F14</f>
-        <v>100</v>
-      </c>
-      <c r="D14" s="107">
-        <f>RESUMEN!Q14</f>
-        <v>87.777777777777771</v>
-      </c>
-      <c r="E14" s="107">
-        <f>RESUMEN!AC14</f>
-        <v>89.990909090909099</v>
-      </c>
-      <c r="F14" s="107">
-        <f>RESUMEN!AD14</f>
+      <c r="C14" s="126">
+        <f>RESUMEN!F14*0.3</f>
+        <v>30</v>
+      </c>
+      <c r="D14" s="126">
+        <f>RESUMEN!Q14*0.3</f>
+        <v>26.333333333333332</v>
+      </c>
+      <c r="E14" s="126">
+        <f>RESUMEN!AC14*0.2</f>
+        <v>17.99818181818182</v>
+      </c>
+      <c r="F14" s="126">
+        <f>RESUMEN!AD14*0.2</f>
         <v>0</v>
       </c>
-      <c r="G14" s="107">
+      <c r="G14" s="126">
         <f>RESUMEN!C33</f>
         <v>0</v>
       </c>
-      <c r="H14" s="85">
+      <c r="H14" s="127">
         <f t="shared" si="0"/>
         <v>74.331515151515148</v>
       </c>
-      <c r="I14" s="86" t="str">
+      <c r="I14" s="85" t="str">
         <f t="shared" si="1"/>
-        <v>|220981288|Carlos Samuel Cruz Mariscal|100|87.8|90|0|0|__74.3__|</v>
+        <v>|220981288|Carlos Samuel Cruz Mariscal|30|26.3|18|0|0|__74.3__|</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="86"/>
+      <c r="I15" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7946,9 +7957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB78B30B-85E1-8742-88C2-F69873755D79}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B24" sqref="B24"/>
+      <selection pane="topRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8129,34 +8140,34 @@
         <f>AVERAGE(D5:E5)</f>
         <v>100</v>
       </c>
-      <c r="G5" s="101">
+      <c r="G5" s="100">
         <v>100</v>
       </c>
-      <c r="H5" s="102">
+      <c r="H5" s="101">
         <v>100</v>
       </c>
-      <c r="I5" s="102">
+      <c r="I5" s="101">
         <v>100</v>
       </c>
-      <c r="J5" s="102">
+      <c r="J5" s="101">
         <v>100</v>
       </c>
-      <c r="K5" s="102">
+      <c r="K5" s="101">
         <v>100</v>
       </c>
-      <c r="L5" s="102">
+      <c r="L5" s="101">
         <v>100</v>
       </c>
-      <c r="M5" s="102">
+      <c r="M5" s="101">
         <v>100</v>
       </c>
-      <c r="N5" s="102">
+      <c r="N5" s="101">
         <v>100</v>
       </c>
-      <c r="O5" s="103">
+      <c r="O5" s="102">
         <v>100</v>
       </c>
-      <c r="P5" s="103">
+      <c r="P5" s="102">
         <v>90</v>
       </c>
       <c r="Q5" s="68">
@@ -8225,34 +8236,34 @@
         <f t="shared" ref="F6:F14" si="1">AVERAGE(D6:E6)</f>
         <v>100</v>
       </c>
-      <c r="G6" s="101">
+      <c r="G6" s="100">
         <v>100</v>
       </c>
-      <c r="H6" s="102">
+      <c r="H6" s="101">
         <v>100</v>
       </c>
-      <c r="I6" s="102">
+      <c r="I6" s="101">
         <v>100</v>
       </c>
-      <c r="J6" s="102">
+      <c r="J6" s="101">
         <v>100</v>
       </c>
-      <c r="K6" s="102">
+      <c r="K6" s="101">
         <v>100</v>
       </c>
-      <c r="L6" s="102">
+      <c r="L6" s="101">
         <v>100</v>
       </c>
-      <c r="M6" s="102">
+      <c r="M6" s="101">
         <v>100</v>
       </c>
-      <c r="N6" s="102">
+      <c r="N6" s="101">
         <v>100</v>
       </c>
-      <c r="O6" s="103">
+      <c r="O6" s="102">
         <v>100</v>
       </c>
-      <c r="P6" s="103">
+      <c r="P6" s="102">
         <v>0</v>
       </c>
       <c r="Q6" s="68">
@@ -8321,34 +8332,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G7" s="101">
+      <c r="G7" s="100">
         <v>93.33</v>
       </c>
-      <c r="H7" s="102">
+      <c r="H7" s="101">
         <v>80</v>
       </c>
-      <c r="I7" s="102">
+      <c r="I7" s="101">
         <v>86.67</v>
       </c>
-      <c r="J7" s="102">
+      <c r="J7" s="101">
         <v>100</v>
       </c>
-      <c r="K7" s="102">
+      <c r="K7" s="101">
         <v>93.33</v>
       </c>
-      <c r="L7" s="102">
+      <c r="L7" s="101">
         <v>93.333333333333329</v>
       </c>
-      <c r="M7" s="102">
+      <c r="M7" s="101">
         <v>86.67</v>
       </c>
-      <c r="N7" s="102">
+      <c r="N7" s="101">
         <v>93.33</v>
       </c>
-      <c r="O7" s="103">
+      <c r="O7" s="102">
         <v>86.67</v>
       </c>
-      <c r="P7" s="103">
+      <c r="P7" s="102">
         <v>90</v>
       </c>
       <c r="Q7" s="68">
@@ -8417,35 +8428,35 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G8" s="101">
+      <c r="G8" s="100">
         <v>93.33</v>
       </c>
-      <c r="H8" s="102">
+      <c r="H8" s="101">
         <v>73.33</v>
       </c>
-      <c r="I8" s="102">
+      <c r="I8" s="101">
         <f>QUIZES!C35</f>
         <v>86.67</v>
       </c>
-      <c r="J8" s="102">
+      <c r="J8" s="101">
         <v>100</v>
       </c>
-      <c r="K8" s="102">
+      <c r="K8" s="101">
         <v>80</v>
       </c>
-      <c r="L8" s="102">
+      <c r="L8" s="101">
         <v>86.666666666666671</v>
       </c>
-      <c r="M8" s="102">
+      <c r="M8" s="101">
         <v>86.67</v>
       </c>
-      <c r="N8" s="102">
+      <c r="N8" s="101">
         <v>66.67</v>
       </c>
-      <c r="O8" s="103">
+      <c r="O8" s="102">
         <v>66.67</v>
       </c>
-      <c r="P8" s="103">
+      <c r="P8" s="102">
         <v>90</v>
       </c>
       <c r="Q8" s="68">
@@ -8514,34 +8525,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G9" s="101">
+      <c r="G9" s="100">
         <v>36.664999999999999</v>
       </c>
-      <c r="H9" s="102">
+      <c r="H9" s="101">
         <v>100</v>
       </c>
-      <c r="I9" s="102">
+      <c r="I9" s="101">
         <v>100</v>
       </c>
-      <c r="J9" s="102">
+      <c r="J9" s="101">
         <v>93.33</v>
       </c>
-      <c r="K9" s="102">
+      <c r="K9" s="101">
         <v>100</v>
       </c>
-      <c r="L9" s="102">
+      <c r="L9" s="101">
         <v>0</v>
       </c>
-      <c r="M9" s="102">
+      <c r="M9" s="101">
         <v>0</v>
       </c>
-      <c r="N9" s="102">
+      <c r="N9" s="101">
         <v>86.67</v>
       </c>
-      <c r="O9" s="103">
+      <c r="O9" s="102">
         <v>100</v>
       </c>
-      <c r="P9" s="103">
+      <c r="P9" s="102">
         <v>90</v>
       </c>
       <c r="Q9" s="68">
@@ -8610,34 +8621,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G10" s="101">
+      <c r="G10" s="100">
         <v>86.67</v>
       </c>
-      <c r="H10" s="102">
+      <c r="H10" s="101">
         <v>100</v>
       </c>
-      <c r="I10" s="102">
+      <c r="I10" s="101">
         <v>100</v>
       </c>
-      <c r="J10" s="102">
+      <c r="J10" s="101">
         <v>100</v>
       </c>
-      <c r="K10" s="102">
+      <c r="K10" s="101">
         <v>100</v>
       </c>
-      <c r="L10" s="102">
+      <c r="L10" s="101">
         <v>100</v>
       </c>
-      <c r="M10" s="102">
+      <c r="M10" s="101">
         <v>100</v>
       </c>
-      <c r="N10" s="102">
+      <c r="N10" s="101">
         <v>100</v>
       </c>
-      <c r="O10" s="103">
+      <c r="O10" s="102">
         <v>100</v>
       </c>
-      <c r="P10" s="103">
+      <c r="P10" s="102">
         <v>100</v>
       </c>
       <c r="Q10" s="68">
@@ -8706,34 +8717,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G11" s="101">
+      <c r="G11" s="100">
         <v>80</v>
       </c>
-      <c r="H11" s="102">
+      <c r="H11" s="101">
         <v>43.335000000000001</v>
       </c>
-      <c r="I11" s="102">
+      <c r="I11" s="101">
         <v>80</v>
       </c>
-      <c r="J11" s="102">
+      <c r="J11" s="101">
         <v>66.67</v>
       </c>
-      <c r="K11" s="102">
+      <c r="K11" s="101">
         <v>33.335000000000001</v>
       </c>
-      <c r="L11" s="102">
+      <c r="L11" s="101">
         <v>73.333333333333329</v>
       </c>
-      <c r="M11" s="102">
+      <c r="M11" s="101">
         <v>46.67</v>
       </c>
-      <c r="N11" s="102">
+      <c r="N11" s="101">
         <v>46.67</v>
       </c>
-      <c r="O11" s="103">
+      <c r="O11" s="102">
         <v>0</v>
       </c>
-      <c r="P11" s="103">
+      <c r="P11" s="102">
         <v>0</v>
       </c>
       <c r="Q11" s="68">
@@ -8802,34 +8813,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G12" s="101">
+      <c r="G12" s="100">
         <v>86.67</v>
       </c>
-      <c r="H12" s="102">
+      <c r="H12" s="101">
         <v>93.33</v>
       </c>
-      <c r="I12" s="102">
+      <c r="I12" s="101">
         <v>100</v>
       </c>
-      <c r="J12" s="102">
+      <c r="J12" s="101">
         <v>73.33</v>
       </c>
-      <c r="K12" s="102">
+      <c r="K12" s="101">
         <v>86.67</v>
       </c>
-      <c r="L12" s="102">
+      <c r="L12" s="101">
         <v>66.666666666666657</v>
       </c>
-      <c r="M12" s="102">
+      <c r="M12" s="101">
         <v>73.33</v>
       </c>
-      <c r="N12" s="102">
+      <c r="N12" s="101">
         <v>80</v>
       </c>
-      <c r="O12" s="103">
+      <c r="O12" s="102">
         <v>80</v>
       </c>
-      <c r="P12" s="103">
+      <c r="P12" s="102">
         <v>0</v>
       </c>
       <c r="Q12" s="68">
@@ -8898,34 +8909,34 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="100">
         <v>93.33</v>
       </c>
-      <c r="H13" s="102">
+      <c r="H13" s="101">
         <v>73.33</v>
       </c>
-      <c r="I13" s="102">
+      <c r="I13" s="101">
         <v>86.67</v>
       </c>
-      <c r="J13" s="102">
+      <c r="J13" s="101">
         <v>0</v>
       </c>
-      <c r="K13" s="102">
+      <c r="K13" s="101">
         <v>86.67</v>
       </c>
-      <c r="L13" s="102">
+      <c r="L13" s="101">
         <v>60</v>
       </c>
-      <c r="M13" s="102">
+      <c r="M13" s="101">
         <v>93.33</v>
       </c>
-      <c r="N13" s="102">
+      <c r="N13" s="101">
         <v>0</v>
       </c>
-      <c r="O13" s="103">
+      <c r="O13" s="102">
         <v>0</v>
       </c>
-      <c r="P13" s="103">
+      <c r="P13" s="102">
         <v>85</v>
       </c>
       <c r="Q13" s="68">
@@ -8994,34 +9005,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G14" s="104">
+      <c r="G14" s="103">
         <v>100</v>
       </c>
-      <c r="H14" s="105">
+      <c r="H14" s="104">
         <v>100</v>
       </c>
-      <c r="I14" s="105">
+      <c r="I14" s="104">
         <v>93.33</v>
       </c>
-      <c r="J14" s="105">
+      <c r="J14" s="104">
         <v>100</v>
       </c>
-      <c r="K14" s="105">
+      <c r="K14" s="104">
         <v>100</v>
       </c>
-      <c r="L14" s="105">
+      <c r="L14" s="104">
         <v>80</v>
       </c>
-      <c r="M14" s="105">
+      <c r="M14" s="104">
         <v>80</v>
       </c>
-      <c r="N14" s="105">
+      <c r="N14" s="104">
         <v>46.67</v>
       </c>
-      <c r="O14" s="106">
+      <c r="O14" s="105">
         <v>43.34</v>
       </c>
-      <c r="P14" s="106">
+      <c r="P14" s="105">
         <v>90</v>
       </c>
       <c r="Q14" s="71">
@@ -9102,7 +9113,7 @@
       <c r="H22" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="J22" s="111"/>
+      <c r="J22" s="109"/>
     </row>
     <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
@@ -9411,7 +9422,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="112" t="s">
+      <c r="A35" s="110" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -9422,7 +9433,7 @@
       <c r="B39" s="22"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="125" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -9641,7 +9652,7 @@
         <f>(F3-E3)*24*60</f>
         <v>1.8833332392387092</v>
       </c>
-      <c r="H3" s="87" t="str">
+      <c r="H3" s="86" t="str">
         <f>HOUR(F3)&amp;IF(MINUTE(F3)&gt;=10, ":"&amp;MINUTE(F3), ":0"&amp;MINUTE(F3))</f>
         <v>20:50</v>
       </c>
@@ -9668,7 +9679,7 @@
         <f t="shared" ref="G4:G12" si="1">(F4-E4)*24*60</f>
         <v>7.4833332491107285</v>
       </c>
-      <c r="H4" s="88" t="str">
+      <c r="H4" s="87" t="str">
         <f t="shared" ref="H4:H12" si="2">HOUR(F4)&amp;IF(MINUTE(F4)&gt;=10, ":"&amp;MINUTE(F4), ":0"&amp;MINUTE(F4))</f>
         <v>20:50</v>
       </c>
@@ -9695,7 +9706,7 @@
         <f t="shared" si="1"/>
         <v>61.233333261916414</v>
       </c>
-      <c r="H5" s="87" t="str">
+      <c r="H5" s="86" t="str">
         <f t="shared" si="2"/>
         <v>21:05</v>
       </c>
@@ -9722,7 +9733,7 @@
         <f t="shared" si="1"/>
         <v>68.300000071758404</v>
       </c>
-      <c r="H6" s="88" t="str">
+      <c r="H6" s="87" t="str">
         <f t="shared" si="2"/>
         <v>21:08</v>
       </c>
@@ -9749,7 +9760,7 @@
         <f t="shared" si="1"/>
         <v>79.10000006086193</v>
       </c>
-      <c r="H7" s="87" t="str">
+      <c r="H7" s="86" t="str">
         <f t="shared" si="2"/>
         <v>21:09</v>
       </c>
@@ -9776,7 +9787,7 @@
         <f t="shared" si="1"/>
         <v>34.200000000419095</v>
       </c>
-      <c r="H8" s="88" t="str">
+      <c r="H8" s="87" t="str">
         <f t="shared" si="2"/>
         <v>21:17</v>
       </c>
@@ -9803,7 +9814,7 @@
         <f t="shared" si="1"/>
         <v>18.366666622459888</v>
       </c>
-      <c r="H9" s="87" t="str">
+      <c r="H9" s="86" t="str">
         <f t="shared" si="2"/>
         <v>21:42</v>
       </c>
@@ -9830,7 +9841,7 @@
         <f t="shared" si="1"/>
         <v>57.050000061281025</v>
       </c>
-      <c r="H10" s="88" t="str">
+      <c r="H10" s="87" t="str">
         <f t="shared" si="2"/>
         <v>21:58</v>
       </c>
@@ -9857,7 +9868,7 @@
         <f t="shared" si="1"/>
         <v>85.250000021187589</v>
       </c>
-      <c r="H11" s="87" t="str">
+      <c r="H11" s="86" t="str">
         <f t="shared" si="2"/>
         <v>22:10</v>
       </c>
@@ -9886,7 +9897,7 @@
         <f t="shared" si="1"/>
         <v>34.449999985517934</v>
       </c>
-      <c r="H12" s="94" t="str">
+      <c r="H12" s="93" t="str">
         <f t="shared" si="2"/>
         <v>23:52</v>
       </c>
@@ -9945,7 +9956,7 @@
         <f>(F17-E17)*24*60</f>
         <v>0.36666662665084004</v>
       </c>
-      <c r="H17" s="87" t="str">
+      <c r="H17" s="86" t="str">
         <f t="shared" ref="H17:H26" si="3">HOUR(F17)&amp;IF(MINUTE(F17)&gt;=10, ":"&amp;MINUTE(F17), ":0"&amp;MINUTE(F17))</f>
         <v>19:46</v>
       </c>
@@ -9972,7 +9983,7 @@
         <f t="shared" ref="G18:G26" si="5">(F18-E18)*24*60</f>
         <v>10.10000002454035</v>
       </c>
-      <c r="H18" s="88" t="str">
+      <c r="H18" s="87" t="str">
         <f t="shared" si="3"/>
         <v>19:54</v>
       </c>
@@ -9999,7 +10010,7 @@
         <f t="shared" si="5"/>
         <v>23.700000102398917</v>
       </c>
-      <c r="H19" s="87" t="str">
+      <c r="H19" s="86" t="str">
         <f t="shared" si="3"/>
         <v>20:32</v>
       </c>
@@ -10026,7 +10037,7 @@
         <f t="shared" si="5"/>
         <v>53.783333280589432</v>
       </c>
-      <c r="H20" s="88" t="str">
+      <c r="H20" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:33</v>
       </c>
@@ -10053,7 +10064,7 @@
         <f t="shared" si="5"/>
         <v>25.850000018253922</v>
       </c>
-      <c r="H21" s="87" t="str">
+      <c r="H21" s="86" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10080,7 +10091,7 @@
         <f t="shared" si="5"/>
         <v>20.766666680574417</v>
       </c>
-      <c r="H22" s="88" t="str">
+      <c r="H22" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10107,7 +10118,7 @@
         <f t="shared" si="5"/>
         <v>26.416666806908324</v>
       </c>
-      <c r="H23" s="87" t="str">
+      <c r="H23" s="86" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10134,7 +10145,7 @@
         <f t="shared" si="5"/>
         <v>2.366666643647477</v>
       </c>
-      <c r="H24" s="88" t="str">
+      <c r="H24" s="87" t="str">
         <f t="shared" si="3"/>
         <v>20:48</v>
       </c>
@@ -10161,7 +10172,7 @@
         <f t="shared" si="5"/>
         <v>77.049999937880784</v>
       </c>
-      <c r="H25" s="87" t="str">
+      <c r="H25" s="86" t="str">
         <f t="shared" si="3"/>
         <v>20:59</v>
       </c>
@@ -10190,7 +10201,7 @@
         <f t="shared" si="5"/>
         <v>61.149999888148159</v>
       </c>
-      <c r="H26" s="94" t="str">
+      <c r="H26" s="93" t="str">
         <f t="shared" si="3"/>
         <v>21:14</v>
       </c>
@@ -10249,7 +10260,7 @@
         <f>(F31-E31)*24*60</f>
         <v>10.066666599595919</v>
       </c>
-      <c r="H31" s="87" t="str">
+      <c r="H31" s="86" t="str">
         <f t="shared" ref="H31:H40" si="6">HOUR(F31)&amp;IF(MINUTE(F31)&gt;=10, ":"&amp;MINUTE(F31), ":0"&amp;MINUTE(F31))</f>
         <v>18:38</v>
       </c>
@@ -10276,7 +10287,7 @@
         <f t="shared" ref="G32:G40" si="8">(F32-E32)*24*60</f>
         <v>1.2166666577104479</v>
       </c>
-      <c r="H32" s="88" t="str">
+      <c r="H32" s="87" t="str">
         <f t="shared" si="6"/>
         <v>19:29</v>
       </c>
@@ -10303,7 +10314,7 @@
         <f t="shared" si="8"/>
         <v>17.533333440078422</v>
       </c>
-      <c r="H33" s="87" t="str">
+      <c r="H33" s="86" t="str">
         <f t="shared" si="6"/>
         <v>20:24</v>
       </c>
@@ -10330,7 +10341,7 @@
         <f t="shared" si="8"/>
         <v>22.833333358867094</v>
       </c>
-      <c r="H34" s="88" t="str">
+      <c r="H34" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:29</v>
       </c>
@@ -10357,7 +10368,7 @@
         <f t="shared" si="8"/>
         <v>27.583333348156884</v>
       </c>
-      <c r="H35" s="87" t="str">
+      <c r="H35" s="86" t="str">
         <f t="shared" si="6"/>
         <v>20:36</v>
       </c>
@@ -10384,7 +10395,7 @@
         <f t="shared" si="8"/>
         <v>34.833333303686231</v>
       </c>
-      <c r="H36" s="88" t="str">
+      <c r="H36" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:40</v>
       </c>
@@ -10411,7 +10422,7 @@
         <f t="shared" si="8"/>
         <v>34.049999944400042</v>
       </c>
-      <c r="H37" s="87" t="str">
+      <c r="H37" s="86" t="str">
         <f t="shared" si="6"/>
         <v>20:41</v>
       </c>
@@ -10438,7 +10449,7 @@
         <f t="shared" si="8"/>
         <v>23.449999970616773</v>
       </c>
-      <c r="H38" s="88" t="str">
+      <c r="H38" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:42</v>
       </c>
@@ -10465,7 +10476,7 @@
         <f t="shared" si="8"/>
         <v>24.316666703671217</v>
       </c>
-      <c r="H39" s="87" t="str">
+      <c r="H39" s="86" t="str">
         <f t="shared" si="6"/>
         <v>20:44</v>
       </c>
@@ -10492,7 +10503,7 @@
         <f t="shared" si="8"/>
         <v>1.6333333903457969</v>
       </c>
-      <c r="H40" s="88" t="str">
+      <c r="H40" s="87" t="str">
         <f t="shared" si="6"/>
         <v>20:57</v>
       </c>
@@ -10551,7 +10562,7 @@
         <f>(F45-E45)*24*60</f>
         <v>2.9000000073574483</v>
       </c>
-      <c r="H45" s="87" t="str">
+      <c r="H45" s="86" t="str">
         <f t="shared" ref="H45:H53" si="9">HOUR(F45)&amp;IF(MINUTE(F45)&gt;=10, ":"&amp;MINUTE(F45), ":0"&amp;MINUTE(F45))</f>
         <v>19:01</v>
       </c>
@@ -10578,7 +10589,7 @@
         <f t="shared" ref="G46:G53" si="11">(F46-E46)*24*60</f>
         <v>3.4500001044943929</v>
       </c>
-      <c r="H46" s="88" t="str">
+      <c r="H46" s="87" t="str">
         <f t="shared" si="9"/>
         <v>19:36</v>
       </c>
@@ -10605,7 +10616,7 @@
         <f t="shared" si="11"/>
         <v>12.300000046379864</v>
       </c>
-      <c r="H47" s="87" t="str">
+      <c r="H47" s="86" t="str">
         <f t="shared" si="9"/>
         <v>20:25</v>
       </c>
@@ -10632,7 +10643,7 @@
         <f t="shared" si="11"/>
         <v>14.150000017834827</v>
       </c>
-      <c r="H48" s="88" t="str">
+      <c r="H48" s="87" t="str">
         <f t="shared" si="9"/>
         <v>20:29</v>
       </c>
@@ -10659,7 +10670,7 @@
         <f t="shared" si="11"/>
         <v>98.449999921722338</v>
       </c>
-      <c r="H49" s="87" t="str">
+      <c r="H49" s="86" t="str">
         <f t="shared" si="9"/>
         <v>20:37</v>
       </c>
@@ -10686,7 +10697,7 @@
         <f t="shared" si="11"/>
         <v>2.0666666887700558</v>
       </c>
-      <c r="H50" s="88" t="str">
+      <c r="H50" s="87" t="str">
         <f t="shared" si="9"/>
         <v>20:41</v>
       </c>
@@ -10713,7 +10724,7 @@
         <f t="shared" si="11"/>
         <v>69.46666675969027</v>
       </c>
-      <c r="H51" s="87" t="str">
+      <c r="H51" s="86" t="str">
         <f t="shared" si="9"/>
         <v>20:41</v>
       </c>
@@ -10740,7 +10751,7 @@
         <f t="shared" si="11"/>
         <v>28.866666677640751</v>
       </c>
-      <c r="H52" s="88" t="str">
+      <c r="H52" s="87" t="str">
         <f t="shared" si="9"/>
         <v>20:42</v>
       </c>
@@ -10767,29 +10778,29 @@
         <f t="shared" si="11"/>
         <v>3.8833333924412727</v>
       </c>
-      <c r="H53" s="87" t="str">
+      <c r="H53" s="86" t="str">
         <f t="shared" si="9"/>
         <v>21:08</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="92" t="s">
+      <c r="A54" s="91" t="s">
         <v>696</v>
       </c>
-      <c r="B54" s="92">
+      <c r="B54" s="91">
         <v>0</v>
       </c>
-      <c r="C54" s="95">
+      <c r="C54" s="94">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="D54" s="92" t="s">
+      <c r="D54" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E54" s="96"/>
-      <c r="F54" s="96"/>
-      <c r="G54" s="96"/>
-      <c r="H54" s="97"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
+      <c r="H54" s="96"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -10845,7 +10856,7 @@
         <f>(F59-E59)*24*60</f>
         <v>1.3500000012572855</v>
       </c>
-      <c r="H59" s="87" t="str">
+      <c r="H59" s="86" t="str">
         <f t="shared" ref="H59:H68" si="12">HOUR(F59)&amp;IF(MINUTE(F59)&gt;=10, ":"&amp;MINUTE(F59), ":0"&amp;MINUTE(F59))</f>
         <v>19:20</v>
       </c>
@@ -10872,7 +10883,7 @@
         <f t="shared" ref="G60:G68" si="14">(F60-E60)*24*60</f>
         <v>1.2500000617001206</v>
       </c>
-      <c r="H60" s="88" t="str">
+      <c r="H60" s="87" t="str">
         <f t="shared" si="12"/>
         <v>19:27</v>
       </c>
@@ -10899,7 +10910,7 @@
         <f t="shared" si="14"/>
         <v>18.716666536638513</v>
       </c>
-      <c r="H61" s="87" t="str">
+      <c r="H61" s="86" t="str">
         <f t="shared" si="12"/>
         <v>20:19</v>
       </c>
@@ -10926,7 +10937,7 @@
         <f t="shared" si="14"/>
         <v>27.316666661063209</v>
       </c>
-      <c r="H62" s="88" t="str">
+      <c r="H62" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:29</v>
       </c>
@@ -10953,7 +10964,7 @@
         <f t="shared" si="14"/>
         <v>61.666666707023978</v>
       </c>
-      <c r="H63" s="87" t="str">
+      <c r="H63" s="86" t="str">
         <f t="shared" si="12"/>
         <v>20:32</v>
       </c>
@@ -10980,7 +10991,7 @@
         <f t="shared" si="14"/>
         <v>29.033333425177261</v>
       </c>
-      <c r="H64" s="88" t="str">
+      <c r="H64" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:33</v>
       </c>
@@ -11007,7 +11018,7 @@
         <f t="shared" si="14"/>
         <v>35.316666582366452</v>
       </c>
-      <c r="H65" s="87" t="str">
+      <c r="H65" s="86" t="str">
         <f t="shared" si="12"/>
         <v>20:36</v>
       </c>
@@ -11034,7 +11045,7 @@
         <f t="shared" si="14"/>
         <v>4.2999999783933163</v>
       </c>
-      <c r="H66" s="88" t="str">
+      <c r="H66" s="87" t="str">
         <f t="shared" si="12"/>
         <v>20:37</v>
       </c>
@@ -11061,7 +11072,7 @@
         <f t="shared" si="14"/>
         <v>62.583333409857005</v>
       </c>
-      <c r="H67" s="87" t="str">
+      <c r="H67" s="86" t="str">
         <f t="shared" si="12"/>
         <v>20:37</v>
       </c>
@@ -11086,11 +11097,11 @@
       <c r="F68" s="41">
         <v>44619.626990740697</v>
       </c>
-      <c r="G68" s="91">
+      <c r="G68" s="90">
         <f t="shared" si="14"/>
         <v>83.099999948171899</v>
       </c>
-      <c r="H68" s="94" t="str">
+      <c r="H68" s="93" t="str">
         <f t="shared" si="12"/>
         <v>15:02</v>
       </c>
@@ -11151,7 +11162,7 @@
         <f>(F73-E73)*24*60</f>
         <v>4.600000079954043</v>
       </c>
-      <c r="H73" s="89" t="str">
+      <c r="H73" s="88" t="str">
         <f t="shared" ref="H73:H82" si="15">HOUR(F73)&amp;IF(MINUTE(F73)&gt;=10, ":"&amp;MINUTE(F73), ":0"&amp;MINUTE(F73))</f>
         <v>21:42</v>
       </c>
@@ -11178,7 +11189,7 @@
         <f t="shared" ref="G74:G82" si="17">(F74-E74)*24*60</f>
         <v>2.649999896530062</v>
       </c>
-      <c r="H74" s="88" t="str">
+      <c r="H74" s="87" t="str">
         <f t="shared" si="15"/>
         <v>19:09</v>
       </c>
@@ -11205,7 +11216,7 @@
         <f t="shared" si="17"/>
         <v>3.1499998562503606</v>
       </c>
-      <c r="H75" s="87" t="str">
+      <c r="H75" s="86" t="str">
         <f t="shared" si="15"/>
         <v>19:20</v>
       </c>
@@ -11232,7 +11243,7 @@
         <f t="shared" si="17"/>
         <v>8.4500000684056431</v>
       </c>
-      <c r="H76" s="88" t="str">
+      <c r="H76" s="87" t="str">
         <f t="shared" si="15"/>
         <v>20:07</v>
       </c>
@@ -11259,7 +11270,7 @@
         <f t="shared" si="17"/>
         <v>17.466666768305004</v>
       </c>
-      <c r="H77" s="87" t="str">
+      <c r="H77" s="86" t="str">
         <f t="shared" si="15"/>
         <v>20:13</v>
       </c>
@@ -11286,7 +11297,7 @@
         <f t="shared" si="17"/>
         <v>28.566666576080024</v>
       </c>
-      <c r="H78" s="88" t="str">
+      <c r="H78" s="87" t="str">
         <f t="shared" si="15"/>
         <v>20:26</v>
       </c>
@@ -11313,7 +11324,7 @@
         <f t="shared" si="17"/>
         <v>36.033333406085148</v>
       </c>
-      <c r="H79" s="87" t="str">
+      <c r="H79" s="86" t="str">
         <f t="shared" si="15"/>
         <v>20:35</v>
       </c>
@@ -11340,7 +11351,7 @@
         <f t="shared" si="17"/>
         <v>40.999999976484105</v>
       </c>
-      <c r="H80" s="88" t="str">
+      <c r="H80" s="87" t="str">
         <f t="shared" si="15"/>
         <v>20:40</v>
       </c>
@@ -11367,7 +11378,7 @@
         <f t="shared" si="17"/>
         <v>44.883333358447999</v>
       </c>
-      <c r="H81" s="87" t="str">
+      <c r="H81" s="86" t="str">
         <f t="shared" si="15"/>
         <v>21:17</v>
       </c>
@@ -11394,29 +11405,29 @@
         <f t="shared" si="17"/>
         <v>36.316666658967733</v>
       </c>
-      <c r="H82" s="88" t="str">
+      <c r="H82" s="87" t="str">
         <f t="shared" si="15"/>
         <v>21:26</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="93" t="s">
+      <c r="A83" s="92" t="s">
         <v>687</v>
       </c>
-      <c r="B83" s="93">
+      <c r="B83" s="92">
         <v>0</v>
       </c>
-      <c r="C83" s="98">
+      <c r="C83" s="97">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D83" s="92" t="s">
+      <c r="D83" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E83" s="99"/>
-      <c r="F83" s="99"/>
-      <c r="G83" s="99"/>
-      <c r="H83" s="100"/>
+      <c r="E83" s="98"/>
+      <c r="F83" s="98"/>
+      <c r="G83" s="98"/>
+      <c r="H83" s="99"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -11472,7 +11483,7 @@
         <f>(F88-E88)*24*60</f>
         <v>1.0500000463798642</v>
       </c>
-      <c r="H88" s="87" t="str">
+      <c r="H88" s="86" t="str">
         <f t="shared" ref="H88:H97" si="18">HOUR(F88)&amp;IF(MINUTE(F88)&gt;=10, ":"&amp;MINUTE(F88), ":0"&amp;MINUTE(F88))</f>
         <v>20:02</v>
       </c>
@@ -11499,7 +11510,7 @@
         <f t="shared" ref="G89:G97" si="20">(F89-E89)*24*60</f>
         <v>13.966666704509407</v>
       </c>
-      <c r="H89" s="88" t="str">
+      <c r="H89" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:14</v>
       </c>
@@ -11526,7 +11537,7 @@
         <f t="shared" si="20"/>
         <v>40.983333410695195</v>
       </c>
-      <c r="H90" s="87" t="str">
+      <c r="H90" s="86" t="str">
         <f t="shared" si="18"/>
         <v>20:41</v>
       </c>
@@ -11553,7 +11564,7 @@
         <f t="shared" si="20"/>
         <v>2.3666666331700981</v>
       </c>
-      <c r="H91" s="88" t="str">
+      <c r="H91" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:42</v>
       </c>
@@ -11582,7 +11593,7 @@
         <f t="shared" si="20"/>
         <v>0.61666675843298435</v>
       </c>
-      <c r="H92" s="90" t="str">
+      <c r="H92" s="89" t="str">
         <f t="shared" si="18"/>
         <v>20:43</v>
       </c>
@@ -11609,7 +11620,7 @@
         <f t="shared" si="20"/>
         <v>49.81666665058583</v>
       </c>
-      <c r="H93" s="88" t="str">
+      <c r="H93" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:50</v>
       </c>
@@ -11636,7 +11647,7 @@
         <f t="shared" si="20"/>
         <v>49.333333246177062</v>
       </c>
-      <c r="H94" s="87" t="str">
+      <c r="H94" s="86" t="str">
         <f t="shared" si="18"/>
         <v>20:50</v>
       </c>
@@ -11663,7 +11674,7 @@
         <f t="shared" si="20"/>
         <v>90.133333343546838</v>
       </c>
-      <c r="H95" s="88" t="str">
+      <c r="H95" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:56</v>
       </c>
@@ -11690,7 +11701,7 @@
         <f t="shared" si="20"/>
         <v>86.583333309972659</v>
       </c>
-      <c r="H96" s="87" t="str">
+      <c r="H96" s="86" t="str">
         <f t="shared" si="18"/>
         <v>21:20</v>
       </c>
@@ -11717,29 +11728,29 @@
         <f t="shared" si="20"/>
         <v>76.93333343253471</v>
       </c>
-      <c r="H97" s="88" t="str">
+      <c r="H97" s="87" t="str">
         <f t="shared" si="18"/>
         <v>21:20</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="93" t="s">
+      <c r="A98" s="92" t="s">
         <v>687</v>
       </c>
-      <c r="B98" s="93">
+      <c r="B98" s="92">
         <v>0</v>
       </c>
-      <c r="C98" s="98">
+      <c r="C98" s="97">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="D98" s="92" t="s">
+      <c r="D98" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E98" s="99"/>
-      <c r="F98" s="99"/>
-      <c r="G98" s="99"/>
-      <c r="H98" s="100"/>
+      <c r="E98" s="98"/>
+      <c r="F98" s="98"/>
+      <c r="G98" s="98"/>
+      <c r="H98" s="99"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
@@ -11795,7 +11806,7 @@
         <f>(F103-E103)*24*60</f>
         <v>53.033333325292915</v>
       </c>
-      <c r="H103" s="87" t="str">
+      <c r="H103" s="86" t="str">
         <f t="shared" ref="H103:H111" si="21">HOUR(F103)&amp;IF(MINUTE(F103)&gt;=10, ":"&amp;MINUTE(F103), ":0"&amp;MINUTE(F103))</f>
         <v>19:08</v>
       </c>
@@ -11822,7 +11833,7 @@
         <f t="shared" ref="G104:G111" si="23">(F104-E104)*24*60</f>
         <v>2.416666749631986</v>
       </c>
-      <c r="H104" s="88" t="str">
+      <c r="H104" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:06</v>
       </c>
@@ -11849,7 +11860,7 @@
         <f t="shared" si="23"/>
         <v>3.1999999727122486</v>
       </c>
-      <c r="H105" s="87" t="str">
+      <c r="H105" s="86" t="str">
         <f t="shared" si="21"/>
         <v>20:07</v>
       </c>
@@ -11876,7 +11887,7 @@
         <f t="shared" si="23"/>
         <v>1.9333333452232182</v>
       </c>
-      <c r="H106" s="88" t="str">
+      <c r="H106" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:07</v>
       </c>
@@ -11903,7 +11914,7 @@
         <f t="shared" si="23"/>
         <v>18.433333294233307</v>
       </c>
-      <c r="H107" s="87" t="str">
+      <c r="H107" s="86" t="str">
         <f t="shared" si="21"/>
         <v>20:22</v>
       </c>
@@ -11930,7 +11941,7 @@
         <f t="shared" si="23"/>
         <v>60.26666673598811</v>
       </c>
-      <c r="H108" s="88" t="str">
+      <c r="H108" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:24</v>
       </c>
@@ -11957,7 +11968,7 @@
         <f t="shared" si="23"/>
         <v>8.2333333406131715</v>
       </c>
-      <c r="H109" s="87" t="str">
+      <c r="H109" s="86" t="str">
         <f t="shared" si="21"/>
         <v>20:35</v>
       </c>
@@ -11984,7 +11995,7 @@
         <f t="shared" si="23"/>
         <v>38.300000110175461</v>
       </c>
-      <c r="H110" s="88" t="str">
+      <c r="H110" s="87" t="str">
         <f t="shared" si="21"/>
         <v>20:42</v>
       </c>
@@ -12011,29 +12022,29 @@
         <f t="shared" si="23"/>
         <v>1.7833334463648498</v>
       </c>
-      <c r="H111" s="87" t="str">
+      <c r="H111" s="86" t="str">
         <f t="shared" si="21"/>
         <v>20:44</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="92" t="s">
+      <c r="A112" s="91" t="s">
         <v>696</v>
       </c>
-      <c r="B112" s="92">
+      <c r="B112" s="91">
         <v>0</v>
       </c>
-      <c r="C112" s="95">
+      <c r="C112" s="94">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="D112" s="92" t="s">
+      <c r="D112" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E112" s="96"/>
-      <c r="F112" s="96"/>
-      <c r="G112" s="97"/>
-      <c r="H112" s="97"/>
+      <c r="E112" s="95"/>
+      <c r="F112" s="95"/>
+      <c r="G112" s="96"/>
+      <c r="H112" s="96"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
@@ -12089,7 +12100,7 @@
         <f>(F117-E117)*24*60</f>
         <v>2.8666666033677757</v>
       </c>
-      <c r="H117" s="87" t="str">
+      <c r="H117" s="86" t="str">
         <f t="shared" ref="H117:H124" si="24">HOUR(F117)&amp;IF(MINUTE(F117)&gt;=10, ":"&amp;MINUTE(F117), ":0"&amp;MINUTE(F117))</f>
         <v>19:04</v>
       </c>
@@ -12116,7 +12127,7 @@
         <f t="shared" ref="G118:G124" si="26">(F118-E118)*24*60</f>
         <v>2.1500000625383109</v>
       </c>
-      <c r="H118" s="88" t="str">
+      <c r="H118" s="87" t="str">
         <f t="shared" si="24"/>
         <v>19:30</v>
       </c>
@@ -12143,7 +12154,7 @@
         <f t="shared" si="26"/>
         <v>1.8833333754446357</v>
       </c>
-      <c r="H119" s="87" t="str">
+      <c r="H119" s="86" t="str">
         <f t="shared" si="24"/>
         <v>20:03</v>
       </c>
@@ -12170,7 +12181,7 @@
         <f t="shared" si="26"/>
         <v>25.966666659805924</v>
       </c>
-      <c r="H120" s="88" t="str">
+      <c r="H120" s="87" t="str">
         <f t="shared" si="24"/>
         <v>20:04</v>
       </c>
@@ -12197,7 +12208,7 @@
         <f t="shared" si="26"/>
         <v>30.80000001238659</v>
       </c>
-      <c r="H121" s="87" t="str">
+      <c r="H121" s="86" t="str">
         <f t="shared" si="24"/>
         <v>20:07</v>
       </c>
@@ -12224,7 +12235,7 @@
         <f t="shared" si="26"/>
         <v>72.600000039674342</v>
       </c>
-      <c r="H122" s="88" t="str">
+      <c r="H122" s="87" t="str">
         <f t="shared" si="24"/>
         <v>21:17</v>
       </c>
@@ -12251,7 +12262,7 @@
         <f t="shared" si="26"/>
         <v>2.3333333758637309</v>
       </c>
-      <c r="H123" s="87" t="str">
+      <c r="H123" s="86" t="str">
         <f t="shared" si="24"/>
         <v>21:20</v>
       </c>
@@ -12280,48 +12291,48 @@
         <f t="shared" si="26"/>
         <v>3.6833332409150898</v>
       </c>
-      <c r="H124" s="94" t="str">
+      <c r="H124" s="93" t="str">
         <f t="shared" si="24"/>
         <v>19:09</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A125" s="93" t="s">
+      <c r="A125" s="92" t="s">
         <v>986</v>
       </c>
-      <c r="B125" s="93">
+      <c r="B125" s="92">
         <v>0</v>
       </c>
-      <c r="C125" s="98">
+      <c r="C125" s="97">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D125" s="92" t="s">
+      <c r="D125" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E125" s="99"/>
-      <c r="F125" s="99"/>
-      <c r="G125" s="96"/>
-      <c r="H125" s="100"/>
+      <c r="E125" s="98"/>
+      <c r="F125" s="98"/>
+      <c r="G125" s="95"/>
+      <c r="H125" s="99"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="92" t="s">
+      <c r="A126" s="91" t="s">
         <v>696</v>
       </c>
-      <c r="B126" s="92">
+      <c r="B126" s="91">
         <v>0</v>
       </c>
-      <c r="C126" s="95">
+      <c r="C126" s="94">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D126" s="92" t="s">
+      <c r="D126" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E126" s="96"/>
-      <c r="F126" s="96"/>
-      <c r="G126" s="96"/>
-      <c r="H126" s="97"/>
+      <c r="E126" s="95"/>
+      <c r="F126" s="95"/>
+      <c r="G126" s="95"/>
+      <c r="H126" s="96"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
@@ -12382,7 +12393,7 @@
         <f>(F132-E132)*24*60</f>
         <v>7.0833333651535213</v>
       </c>
-      <c r="H132" s="90" t="str">
+      <c r="H132" s="89" t="str">
         <f t="shared" ref="H132:H139" si="27">HOUR(F132)&amp;IF(MINUTE(F132)&gt;=10, ":"&amp;MINUTE(F132), ":0"&amp;MINUTE(F132))</f>
         <v>20:06</v>
       </c>
@@ -12409,7 +12420,7 @@
         <f t="shared" ref="G133:G139" si="29">(F133-E133)*24*60</f>
         <v>5.116666752146557</v>
       </c>
-      <c r="H133" s="88" t="str">
+      <c r="H133" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:12</v>
       </c>
@@ -12436,7 +12447,7 @@
         <f t="shared" si="29"/>
         <v>18.016666551120579</v>
       </c>
-      <c r="H134" s="87" t="str">
+      <c r="H134" s="86" t="str">
         <f t="shared" si="27"/>
         <v>20:18</v>
       </c>
@@ -12463,7 +12474,7 @@
         <f t="shared" si="29"/>
         <v>32.466666680993512</v>
       </c>
-      <c r="H135" s="88" t="str">
+      <c r="H135" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:31</v>
       </c>
@@ -12490,7 +12501,7 @@
         <f t="shared" si="29"/>
         <v>2.4999999767169356</v>
       </c>
-      <c r="H136" s="87" t="str">
+      <c r="H136" s="86" t="str">
         <f t="shared" si="27"/>
         <v>20:32</v>
       </c>
@@ -12517,7 +12528,7 @@
         <f t="shared" si="29"/>
         <v>3.3500000182539225</v>
       </c>
-      <c r="H137" s="88" t="str">
+      <c r="H137" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:33</v>
       </c>
@@ -12544,7 +12555,7 @@
         <f t="shared" si="29"/>
         <v>35.116666703252122</v>
       </c>
-      <c r="H138" s="87" t="str">
+      <c r="H138" s="86" t="str">
         <f t="shared" si="27"/>
         <v>20:33</v>
       </c>
@@ -12571,67 +12582,67 @@
         <f t="shared" si="29"/>
         <v>28.033333338098601</v>
       </c>
-      <c r="H139" s="88" t="str">
+      <c r="H139" s="87" t="str">
         <f t="shared" si="27"/>
         <v>20:56</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="109" t="s">
+      <c r="A140" s="107" t="s">
         <v>986</v>
       </c>
-      <c r="B140" s="92">
+      <c r="B140" s="91">
         <v>0</v>
       </c>
-      <c r="C140" s="98">
+      <c r="C140" s="97">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D140" s="92" t="s">
+      <c r="D140" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E140" s="99"/>
-      <c r="F140" s="99"/>
-      <c r="G140" s="99"/>
-      <c r="H140" s="100"/>
+      <c r="E140" s="98"/>
+      <c r="F140" s="98"/>
+      <c r="G140" s="98"/>
+      <c r="H140" s="99"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="92" t="s">
+      <c r="A141" s="91" t="s">
         <v>1081</v>
       </c>
-      <c r="B141" s="92">
+      <c r="B141" s="91">
         <v>0</v>
       </c>
-      <c r="C141" s="95">
+      <c r="C141" s="94">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D141" s="92" t="s">
+      <c r="D141" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E141" s="96"/>
-      <c r="F141" s="96"/>
-      <c r="G141" s="96"/>
-      <c r="H141" s="97"/>
+      <c r="E141" s="95"/>
+      <c r="F141" s="95"/>
+      <c r="G141" s="95"/>
+      <c r="H141" s="96"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="93" t="s">
+      <c r="A142" s="92" t="s">
         <v>1083</v>
       </c>
-      <c r="B142" s="92">
+      <c r="B142" s="91">
         <v>0</v>
       </c>
-      <c r="C142" s="98">
+      <c r="C142" s="97">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D142" s="92" t="s">
+      <c r="D142" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="E142" s="99"/>
-      <c r="F142" s="99"/>
-      <c r="G142" s="99"/>
-      <c r="H142" s="100"/>
+      <c r="E142" s="98"/>
+      <c r="F142" s="98"/>
+      <c r="G142" s="98"/>
+      <c r="H142" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18634,7 +18645,7 @@
       <c r="AX83" t="s">
         <v>1063</v>
       </c>
-      <c r="BA83" s="108">
+      <c r="BA83" s="106">
         <f>(13-4)/13</f>
         <v>0.69230769230769229</v>
       </c>
@@ -18697,7 +18708,7 @@
       <c r="AX84" t="s">
         <v>1073</v>
       </c>
-      <c r="BA84" s="108">
+      <c r="BA84" s="106">
         <f t="shared" ref="BA84:BA87" si="2">(13-4)/13</f>
         <v>0.69230769230769229</v>
       </c>
@@ -18760,7 +18771,7 @@
       <c r="AX85" t="s">
         <v>1046</v>
       </c>
-      <c r="BA85" s="108">
+      <c r="BA85" s="106">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -18823,7 +18834,7 @@
       <c r="AX86" t="s">
         <v>1046</v>
       </c>
-      <c r="BA86" s="108">
+      <c r="BA86" s="106">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -18886,7 +18897,7 @@
       <c r="AX87" t="s">
         <v>1063</v>
       </c>
-      <c r="BA87" s="108">
+      <c r="BA87" s="106">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -19089,668 +19100,668 @@
       <c r="P2" s="59" t="s">
         <v>1094</v>
       </c>
-      <c r="Q2" s="121" t="s">
+      <c r="Q2" s="119" t="s">
         <v>1098</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="117" t="s">
         <v>1088</v>
       </c>
-      <c r="C3" s="120">
+      <c r="C3" s="118">
         <v>1</v>
       </c>
-      <c r="D3" s="120">
+      <c r="D3" s="118">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="E3" s="120">
+      <c r="E3" s="118">
         <f t="shared" ref="E3:N3" si="0">D3+1</f>
         <v>3</v>
       </c>
-      <c r="F3" s="120">
+      <c r="F3" s="118">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G3" s="120">
+      <c r="G3" s="118">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H3" s="120">
+      <c r="H3" s="118">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I3" s="120">
+      <c r="I3" s="118">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J3" s="120">
+      <c r="J3" s="118">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K3" s="120">
+      <c r="K3" s="118">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L3" s="120">
+      <c r="L3" s="118">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M3" s="120">
+      <c r="M3" s="118">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N3" s="120">
+      <c r="N3" s="118">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O3" s="120">
+      <c r="O3" s="118">
         <f t="shared" ref="O3" si="1">N3+1</f>
         <v>13</v>
       </c>
-      <c r="P3" s="120">
+      <c r="P3" s="118">
         <f t="shared" ref="P3" si="2">O3+1</f>
         <v>14</v>
       </c>
-      <c r="Q3" s="120">
+      <c r="Q3" s="118">
         <f t="shared" ref="Q3" si="3">P3+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="115">
+      <c r="C4" s="113">
         <v>44580</v>
       </c>
-      <c r="D4" s="115">
+      <c r="D4" s="113">
         <f>C4+7</f>
         <v>44587</v>
       </c>
-      <c r="E4" s="115">
+      <c r="E4" s="113">
         <f t="shared" ref="E4:M4" si="4">D4+7</f>
         <v>44594</v>
       </c>
-      <c r="F4" s="115">
+      <c r="F4" s="113">
         <f t="shared" si="4"/>
         <v>44601</v>
       </c>
-      <c r="G4" s="115">
+      <c r="G4" s="113">
         <f t="shared" si="4"/>
         <v>44608</v>
       </c>
-      <c r="H4" s="115">
+      <c r="H4" s="113">
         <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="I4" s="115">
+      <c r="I4" s="113">
         <f t="shared" si="4"/>
         <v>44622</v>
       </c>
-      <c r="J4" s="115">
+      <c r="J4" s="113">
         <f t="shared" si="4"/>
         <v>44629</v>
       </c>
-      <c r="K4" s="115">
+      <c r="K4" s="113">
         <f t="shared" si="4"/>
         <v>44636</v>
       </c>
-      <c r="L4" s="115">
+      <c r="L4" s="113">
         <f t="shared" si="4"/>
         <v>44643</v>
       </c>
-      <c r="M4" s="115">
+      <c r="M4" s="113">
         <f t="shared" si="4"/>
         <v>44650</v>
       </c>
-      <c r="N4" s="115">
+      <c r="N4" s="113">
         <f t="shared" ref="N4:O4" si="5">M4+7</f>
         <v>44657</v>
       </c>
-      <c r="O4" s="115">
+      <c r="O4" s="113">
         <f t="shared" si="5"/>
         <v>44664</v>
       </c>
-      <c r="P4" s="115">
+      <c r="P4" s="113">
         <f t="shared" ref="P4:Q4" si="6">O4+7</f>
         <v>44671</v>
       </c>
-      <c r="Q4" s="115">
+      <c r="Q4" s="113">
         <f t="shared" si="6"/>
         <v>44678</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="118">
+      <c r="A5" s="116">
         <v>220981245</v>
       </c>
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="116">
+      <c r="C5" s="114">
         <v>1</v>
       </c>
-      <c r="D5" s="116">
+      <c r="D5" s="114">
         <v>1</v>
       </c>
-      <c r="E5" s="116">
+      <c r="E5" s="114">
         <v>1</v>
       </c>
-      <c r="F5" s="116">
+      <c r="F5" s="114">
         <v>1</v>
       </c>
-      <c r="G5" s="116">
+      <c r="G5" s="114">
         <v>1</v>
       </c>
-      <c r="H5" s="116">
+      <c r="H5" s="114">
         <v>1</v>
       </c>
-      <c r="I5" s="116">
+      <c r="I5" s="114">
         <v>1</v>
       </c>
-      <c r="J5" s="116">
+      <c r="J5" s="114">
         <v>1</v>
       </c>
-      <c r="K5" s="116">
+      <c r="K5" s="114">
         <v>1</v>
       </c>
-      <c r="L5" s="116">
+      <c r="L5" s="114">
         <v>1</v>
       </c>
-      <c r="M5" s="116">
+      <c r="M5" s="114">
         <v>1</v>
       </c>
-      <c r="N5" s="116">
+      <c r="N5" s="114">
         <v>1</v>
       </c>
-      <c r="O5" s="116" t="s">
+      <c r="O5" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P5" s="116" t="s">
+      <c r="P5" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q5" s="116">
+      <c r="Q5" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="118">
+      <c r="A6" s="116">
         <v>399515449</v>
       </c>
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="116">
+      <c r="C6" s="114">
         <v>1</v>
       </c>
-      <c r="D6" s="116">
+      <c r="D6" s="114">
         <v>1</v>
       </c>
-      <c r="E6" s="116">
+      <c r="E6" s="114">
         <v>1</v>
       </c>
-      <c r="F6" s="116">
+      <c r="F6" s="114">
         <v>1</v>
       </c>
-      <c r="G6" s="116">
+      <c r="G6" s="114">
         <v>1</v>
       </c>
-      <c r="H6" s="116">
+      <c r="H6" s="114">
         <v>1</v>
       </c>
-      <c r="I6" s="116">
+      <c r="I6" s="114">
         <v>1</v>
       </c>
-      <c r="J6" s="116">
+      <c r="J6" s="114">
         <v>1</v>
       </c>
-      <c r="K6" s="116">
+      <c r="K6" s="114">
         <v>1</v>
       </c>
-      <c r="L6" s="116">
+      <c r="L6" s="114">
         <v>1</v>
       </c>
-      <c r="M6" s="116">
+      <c r="M6" s="114">
         <v>1</v>
       </c>
-      <c r="N6" s="116">
+      <c r="N6" s="114">
         <v>1</v>
       </c>
-      <c r="O6" s="116" t="s">
+      <c r="O6" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P6" s="116" t="s">
+      <c r="P6" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q6" s="116">
+      <c r="Q6" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="118">
+      <c r="A7" s="116">
         <v>207595964</v>
       </c>
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="116">
+      <c r="C7" s="114">
         <v>1</v>
       </c>
-      <c r="D7" s="116">
+      <c r="D7" s="114">
         <v>1</v>
       </c>
-      <c r="E7" s="116">
+      <c r="E7" s="114">
         <v>1</v>
       </c>
-      <c r="F7" s="116">
+      <c r="F7" s="114">
         <v>1</v>
       </c>
-      <c r="G7" s="116">
+      <c r="G7" s="114">
         <v>1</v>
       </c>
-      <c r="H7" s="116">
+      <c r="H7" s="114">
         <v>1</v>
       </c>
-      <c r="I7" s="116">
+      <c r="I7" s="114">
         <v>1</v>
       </c>
-      <c r="J7" s="116">
+      <c r="J7" s="114">
         <v>1</v>
       </c>
-      <c r="K7" s="116">
+      <c r="K7" s="114">
         <v>1</v>
       </c>
-      <c r="L7" s="116">
+      <c r="L7" s="114">
         <v>1</v>
       </c>
-      <c r="M7" s="116">
+      <c r="M7" s="114">
         <v>1</v>
       </c>
-      <c r="N7" s="116">
+      <c r="N7" s="114">
         <v>1</v>
       </c>
-      <c r="O7" s="116" t="s">
+      <c r="O7" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P7" s="116" t="s">
+      <c r="P7" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q7" s="116">
+      <c r="Q7" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="118">
+      <c r="A8" s="116">
         <v>211776124</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="116">
+      <c r="C8" s="114">
         <v>1</v>
       </c>
-      <c r="D8" s="116">
+      <c r="D8" s="114">
         <v>1</v>
       </c>
-      <c r="E8" s="116">
+      <c r="E8" s="114">
         <v>1</v>
       </c>
-      <c r="F8" s="116">
+      <c r="F8" s="114">
         <v>1</v>
       </c>
-      <c r="G8" s="116">
+      <c r="G8" s="114">
         <v>1</v>
       </c>
-      <c r="H8" s="116">
+      <c r="H8" s="114">
         <v>1</v>
       </c>
-      <c r="I8" s="116">
+      <c r="I8" s="114">
         <v>1</v>
       </c>
-      <c r="J8" s="116">
+      <c r="J8" s="114">
         <v>1</v>
       </c>
-      <c r="K8" s="116">
+      <c r="K8" s="114">
         <v>1</v>
       </c>
-      <c r="L8" s="116">
+      <c r="L8" s="114">
         <v>1</v>
       </c>
-      <c r="M8" s="116">
+      <c r="M8" s="114">
         <v>1</v>
       </c>
-      <c r="N8" s="116">
+      <c r="N8" s="114">
         <v>1</v>
       </c>
-      <c r="O8" s="116" t="s">
+      <c r="O8" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P8" s="116" t="s">
+      <c r="P8" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q8" s="116">
+      <c r="Q8" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="118">
+      <c r="A9" s="116">
         <v>220981202</v>
       </c>
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="116">
+      <c r="C9" s="114">
         <v>1</v>
       </c>
-      <c r="D9" s="116">
+      <c r="D9" s="114">
         <v>1</v>
       </c>
-      <c r="E9" s="116">
+      <c r="E9" s="114">
         <v>1</v>
       </c>
-      <c r="F9" s="116">
+      <c r="F9" s="114">
         <v>1</v>
       </c>
-      <c r="G9" s="116">
+      <c r="G9" s="114">
         <v>1</v>
       </c>
-      <c r="H9" s="116">
+      <c r="H9" s="114">
         <v>1</v>
       </c>
-      <c r="I9" s="116">
+      <c r="I9" s="114">
         <v>1</v>
       </c>
-      <c r="J9" s="116">
+      <c r="J9" s="114">
         <v>0</v>
       </c>
-      <c r="K9" s="116">
+      <c r="K9" s="114">
         <v>0</v>
       </c>
-      <c r="L9" s="116">
+      <c r="L9" s="114">
         <v>1</v>
       </c>
-      <c r="M9" s="116">
+      <c r="M9" s="114">
         <v>1</v>
       </c>
-      <c r="N9" s="116">
+      <c r="N9" s="114">
         <v>1</v>
       </c>
-      <c r="O9" s="116" t="s">
+      <c r="O9" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P9" s="116" t="s">
+      <c r="P9" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q9" s="116">
+      <c r="Q9" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="118">
+      <c r="A10" s="116">
         <v>398813438</v>
       </c>
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="116">
+      <c r="C10" s="114">
         <v>1</v>
       </c>
-      <c r="D10" s="116">
+      <c r="D10" s="114">
         <v>1</v>
       </c>
-      <c r="E10" s="116">
+      <c r="E10" s="114">
         <v>1</v>
       </c>
-      <c r="F10" s="116">
+      <c r="F10" s="114">
         <v>1</v>
       </c>
-      <c r="G10" s="116">
+      <c r="G10" s="114">
         <v>1</v>
       </c>
-      <c r="H10" s="116">
+      <c r="H10" s="114">
         <v>1</v>
       </c>
-      <c r="I10" s="116">
+      <c r="I10" s="114">
         <v>1</v>
       </c>
-      <c r="J10" s="116">
+      <c r="J10" s="114">
         <v>1</v>
       </c>
-      <c r="K10" s="116">
+      <c r="K10" s="114">
         <v>1</v>
       </c>
-      <c r="L10" s="116">
+      <c r="L10" s="114">
         <v>1</v>
       </c>
-      <c r="M10" s="116">
+      <c r="M10" s="114">
         <v>1</v>
       </c>
-      <c r="N10" s="116">
+      <c r="N10" s="114">
         <v>1</v>
       </c>
-      <c r="O10" s="116" t="s">
+      <c r="O10" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P10" s="116" t="s">
+      <c r="P10" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q10" s="116">
+      <c r="Q10" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="118">
+      <c r="A11" s="116">
         <v>220981261</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="116">
+      <c r="C11" s="114">
         <v>1</v>
       </c>
-      <c r="D11" s="116">
+      <c r="D11" s="114">
         <v>1</v>
       </c>
-      <c r="E11" s="116">
+      <c r="E11" s="114">
         <v>1</v>
       </c>
-      <c r="F11" s="116">
+      <c r="F11" s="114">
         <v>1</v>
       </c>
-      <c r="G11" s="116">
+      <c r="G11" s="114">
         <v>1</v>
       </c>
-      <c r="H11" s="116">
+      <c r="H11" s="114">
         <v>1</v>
       </c>
-      <c r="I11" s="116">
+      <c r="I11" s="114">
         <v>1</v>
       </c>
-      <c r="J11" s="116">
+      <c r="J11" s="114">
         <v>1</v>
       </c>
-      <c r="K11" s="116">
+      <c r="K11" s="114">
         <v>1</v>
       </c>
-      <c r="L11" s="116">
+      <c r="L11" s="114">
         <v>1</v>
       </c>
-      <c r="M11" s="116">
+      <c r="M11" s="114">
         <v>0</v>
       </c>
-      <c r="N11" s="116">
+      <c r="N11" s="114">
         <v>1</v>
       </c>
-      <c r="O11" s="116" t="s">
+      <c r="O11" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P11" s="116" t="s">
+      <c r="P11" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q11" s="116">
+      <c r="Q11" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="118">
+      <c r="A12" s="116">
         <v>220981296</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="116">
+      <c r="C12" s="114">
         <v>1</v>
       </c>
-      <c r="D12" s="116">
+      <c r="D12" s="114">
         <v>1</v>
       </c>
-      <c r="E12" s="116">
+      <c r="E12" s="114">
         <v>1</v>
       </c>
-      <c r="F12" s="116">
+      <c r="F12" s="114">
         <v>1</v>
       </c>
-      <c r="G12" s="116">
+      <c r="G12" s="114">
         <v>1</v>
       </c>
-      <c r="H12" s="116">
+      <c r="H12" s="114">
         <v>1</v>
       </c>
-      <c r="I12" s="116">
+      <c r="I12" s="114">
         <v>1</v>
       </c>
-      <c r="J12" s="116">
+      <c r="J12" s="114">
         <v>1</v>
       </c>
-      <c r="K12" s="116">
+      <c r="K12" s="114">
         <v>1</v>
       </c>
-      <c r="L12" s="116">
+      <c r="L12" s="114">
         <v>1</v>
       </c>
-      <c r="M12" s="116">
+      <c r="M12" s="114">
         <v>1</v>
       </c>
-      <c r="N12" s="116">
+      <c r="N12" s="114">
         <v>1</v>
       </c>
-      <c r="O12" s="116" t="s">
+      <c r="O12" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P12" s="116" t="s">
+      <c r="P12" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q12" s="116">
+      <c r="Q12" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="118">
+      <c r="A13" s="116">
         <v>220981229</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="116">
+      <c r="C13" s="114">
         <v>1</v>
       </c>
-      <c r="D13" s="116">
+      <c r="D13" s="114">
         <v>1</v>
       </c>
-      <c r="E13" s="116">
+      <c r="E13" s="114">
         <v>1</v>
       </c>
-      <c r="F13" s="116">
+      <c r="F13" s="114">
         <v>1</v>
       </c>
-      <c r="G13" s="116">
+      <c r="G13" s="114">
         <v>0</v>
       </c>
-      <c r="H13" s="116">
+      <c r="H13" s="114">
         <v>1</v>
       </c>
-      <c r="I13" s="116">
+      <c r="I13" s="114">
         <v>1</v>
       </c>
-      <c r="J13" s="116">
+      <c r="J13" s="114">
         <v>1</v>
       </c>
-      <c r="K13" s="116">
+      <c r="K13" s="114">
         <v>1</v>
       </c>
-      <c r="L13" s="116">
+      <c r="L13" s="114">
         <v>0</v>
       </c>
-      <c r="M13" s="116">
+      <c r="M13" s="114">
         <v>0</v>
       </c>
-      <c r="N13" s="116">
+      <c r="N13" s="114">
         <v>1</v>
       </c>
-      <c r="O13" s="116" t="s">
+      <c r="O13" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P13" s="116" t="s">
+      <c r="P13" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q13" s="116">
+      <c r="Q13" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="118">
+      <c r="A14" s="116">
         <v>220981288</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="116">
+      <c r="C14" s="114">
         <v>1</v>
       </c>
-      <c r="D14" s="116">
+      <c r="D14" s="114">
         <v>1</v>
       </c>
-      <c r="E14" s="116">
+      <c r="E14" s="114">
         <v>1</v>
       </c>
-      <c r="F14" s="116">
+      <c r="F14" s="114">
         <v>1</v>
       </c>
-      <c r="G14" s="116">
+      <c r="G14" s="114">
         <v>1</v>
       </c>
-      <c r="H14" s="116">
+      <c r="H14" s="114">
         <v>1</v>
       </c>
-      <c r="I14" s="116">
+      <c r="I14" s="114">
         <v>1</v>
       </c>
-      <c r="J14" s="116">
+      <c r="J14" s="114">
         <v>1</v>
       </c>
-      <c r="K14" s="116">
+      <c r="K14" s="114">
         <v>1</v>
       </c>
-      <c r="L14" s="116">
+      <c r="L14" s="114">
         <v>1</v>
       </c>
-      <c r="M14" s="116">
+      <c r="M14" s="114">
         <v>1</v>
       </c>
-      <c r="N14" s="116">
+      <c r="N14" s="114">
         <v>1</v>
       </c>
-      <c r="O14" s="116" t="s">
+      <c r="O14" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="P14" s="116" t="s">
+      <c r="P14" s="114" t="s">
         <v>1092</v>
       </c>
-      <c r="Q14" s="116">
+      <c r="Q14" s="114">
         <v>1</v>
       </c>
     </row>
@@ -19760,39 +19771,39 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="111" t="s">
         <v>1095</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="114"/>
+      <c r="C19" s="112"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="114"/>
+      <c r="C20" s="112"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="114"/>
+      <c r="C21" s="112"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="114"/>
+      <c r="C22" s="112"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="114"/>
+      <c r="C23" s="112"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="114"/>
+      <c r="C24" s="112"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="114"/>
+      <c r="C25" s="112"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="114"/>
+      <c r="C26" s="112"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="114"/>
+      <c r="C27" s="112"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="114"/>
+      <c r="C28" s="112"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Añadir grupos de trabajo
</commit_message>
<xml_diff>
--- a/grades/Calificaciones.xlsx
+++ b/grades/Calificaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/05_Projects_levic/Projects_git/UDG_MCD_Project_Dev_II/grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57077510-84EB-8542-9E1F-8656FCBE4AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9928D484-F860-0B42-8F79-5DD9C2AFD6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="TAREAS" sheetId="3" r:id="rId4"/>
     <sheet name="PTOS EXTRAS" sheetId="4" r:id="rId5"/>
     <sheet name="ASISTENCIA" sheetId="6" r:id="rId6"/>
+    <sheet name="EQUIPOS" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="1106">
   <si>
     <t>Id. estudiante</t>
   </si>
@@ -3872,6 +3873,18 @@
   </si>
   <si>
     <t>2022-04-27</t>
+  </si>
+  <si>
+    <t>EQUIPOS DE TRABAJO</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>No. de Equipo</t>
+  </si>
+  <si>
+    <t>Alumnos</t>
   </si>
 </sst>
 </file>
@@ -4115,7 +4128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -4426,12 +4439,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4665,6 +4715,24 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -19809,4 +19877,120 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB27F55-7D0E-A846-97B5-EF9A7FB358DD}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="23"/>
+    </row>
+    <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="81" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B3" s="130" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C3" s="131"/>
+      <c r="D3" s="132"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="134" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D4" s="135" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="82" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="133" t="s">
+        <v>992</v>
+      </c>
+      <c r="C5" s="134" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D5" s="135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="82" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="133" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="134" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D6" s="135" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="82" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="133" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="134" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D7" s="135" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="82" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="133" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="134" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D8" s="135" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D8">
+    <sortCondition ref="A4:A8"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizar califs con ptos extra Mario
</commit_message>
<xml_diff>
--- a/grades/Calificaciones.xlsx
+++ b/grades/Calificaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/05_Projects_levic/Projects_git/UDG_MCD_Project_Dev_II/grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EC0366-7A39-7C43-8C99-FFC2D3C802F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A17341-2090-4C4F-A6E1-271B7E79002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN FINAL" sheetId="5" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="1120">
   <si>
     <t>Id. estudiante</t>
   </si>
@@ -3863,9 +3863,6 @@
     <t>@Risk+Project</t>
   </si>
   <si>
-    <t>2 actividades</t>
-  </si>
-  <si>
     <t>EQUIPOS DE TRABAJO</t>
   </si>
   <si>
@@ -3881,9 +3878,6 @@
     <t>Publicación</t>
   </si>
   <si>
-    <t>Exposición en congreso "Application of Data Mining Techniques to Characterize Students under the Effect of COVID-19", publicación en curso "Comparative Study of Monte Carlo Simulation and the Deterministic Model to Analyze the Thermal Insulation Cost"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Publicación "Organización y acceso a la información", </t>
   </si>
   <si>
@@ -3903,6 +3897,36 @@
   </si>
   <si>
     <t>2022-05-11</t>
+  </si>
+  <si>
+    <t>Proyecto personal</t>
+  </si>
+  <si>
+    <t>Exposición en congreso "Application of Data Mining Techniques to Characterize Students under the Effect of COVID-19"</t>
+  </si>
+  <si>
+    <t>Publicación en curso "Comparative Study of Monte Carlo Simulation and the Deterministic Model to Analyze the Thermal Insulation Cost"</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Terminología: n/a se refiere a "no aplica"</t>
+  </si>
+  <si>
+    <t>https://github.com/marioph2022/heartbeat_analysis</t>
+  </si>
+  <si>
+    <t>Proyecto personal "Analysis of synthetic heartbeat data"</t>
+  </si>
+  <si>
+    <t>https://github.com/marioph2022/ibm_iot_simulation</t>
+  </si>
+  <si>
+    <t>Proyecto personal "IBM IoT simulation"</t>
+  </si>
+  <si>
+    <t>Otra</t>
   </si>
 </sst>
 </file>
@@ -4154,7 +4178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -4513,13 +4537,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4762,6 +4812,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4772,16 +4828,46 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7643,7 +7729,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7980,15 +8066,15 @@
       </c>
       <c r="G12" s="125">
         <f>RESUMEN!C31</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H12" s="126">
         <f t="shared" si="0"/>
-        <v>72.989122400475338</v>
+        <v>82.989122400475338</v>
       </c>
       <c r="I12" s="84" t="str">
         <f t="shared" si="1"/>
-        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|0|0|__73__|</v>
+        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|0|10|__83__|</v>
       </c>
     </row>
     <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8077,7 +8163,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A40" sqref="A40"/>
+      <selection pane="topRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9242,7 +9328,7 @@
         <v>56</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="G23" s="29" t="s">
         <v>57</v>
@@ -9456,14 +9542,14 @@
       </c>
       <c r="C31" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E31" s="36">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F31" s="34">
         <v>0</v>
@@ -9544,7 +9630,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="124" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -9656,7 +9742,7 @@
       </c>
       <c r="C50" s="16">
         <f t="shared" si="6"/>
-        <v>72.989122400475338</v>
+        <v>82.989122400475338</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -19030,29 +19116,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56003B35-B20E-7E41-B8AA-8807D2B14A4C}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="95" customWidth="1"/>
-    <col min="4" max="4" width="55.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="147" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="147" customWidth="1"/>
+    <col min="3" max="3" width="76.1640625" style="147" customWidth="1"/>
+    <col min="4" max="4" width="83.6640625" style="149" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="147"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="146" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-    </row>
-    <row r="3" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="148"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="81" t="s">
         <v>62</v>
       </c>
@@ -19062,141 +19149,182 @@
       <c r="C3" s="81" t="s">
         <v>987</v>
       </c>
-      <c r="D3" s="137" t="s">
+      <c r="D3" s="133" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="137" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C4" s="141" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D4" s="150" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E4" s="147" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="135" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C4" s="136" t="s">
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="142"/>
+      <c r="B5" s="137" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C5" s="141" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D5" s="141" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="143" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="137"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="137"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="143" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="137"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="143" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="137"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="143" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="137"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="137"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="144" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="137" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C12" s="140" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D12" s="150" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E12" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="145"/>
+      <c r="B13" s="137" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C13" s="140" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D13" s="150" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="143" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="137"/>
+      <c r="C14" s="140"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="143" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="137" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C15" s="140" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D15" s="150" t="s">
         <v>1104</v>
       </c>
-      <c r="D4" s="138" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="135"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="135"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="135"/>
-      <c r="C7" s="135"/>
-      <c r="D7" s="135"/>
-      <c r="E7" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="135"/>
-      <c r="D8" s="135"/>
-      <c r="E8" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="82" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="135"/>
-      <c r="D9" s="135"/>
-      <c r="E9" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="135"/>
-      <c r="E10" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="135"/>
-      <c r="C11" s="135"/>
-      <c r="D11" s="135"/>
-      <c r="E11" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="82" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="135"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="135"/>
-      <c r="E12" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="135" t="s">
-        <v>1103</v>
-      </c>
-      <c r="C13" s="135" t="s">
-        <v>1105</v>
-      </c>
-      <c r="D13" s="138" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1109</v>
+      <c r="E15" s="147" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="138" t="s">
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B13" xr:uid="{056D01C0-61E5-EE48-96CE-68F5E7E36218}">
-      <formula1>"Proyecto personal, Publicación, Voluntariado, Hackathon, 2 actividades, 3 actividades, 4 o + actividades"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B15" xr:uid="{056D01C0-61E5-EE48-96CE-68F5E7E36218}">
+      <formula1>"Proyecto personal, Publicación, Voluntariado, Hackathon, Otra"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" xr:uid="{A22C7851-AA9B-3647-AB35-981668C8A869}"/>
+    <hyperlink ref="D15" r:id="rId1" xr:uid="{A22C7851-AA9B-3647-AB35-981668C8A869}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{CE298372-D79F-9644-BCDA-83ADF8BE8EAA}"/>
+    <hyperlink ref="D12" r:id="rId3" xr:uid="{7C23D744-7619-8E44-B373-DF5473B7BDE3}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{79F6FADB-05E6-D046-BCE4-9874A5879F96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19207,7 +19335,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19995,7 +20123,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -20003,13 +20131,13 @@
     </row>
     <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="81" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B3" s="134" t="s">
         <v>1101</v>
       </c>
-      <c r="B3" s="132" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C3" s="133"/>
-      <c r="D3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="136"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="82" t="s">
@@ -20019,7 +20147,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="130" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D4" s="131" t="s">
         <v>3</v>
@@ -20033,7 +20161,7 @@
         <v>991</v>
       </c>
       <c r="C5" s="130" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D5" s="131" t="s">
         <v>9</v>
@@ -20047,7 +20175,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="130" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D6" s="131" t="s">
         <v>11</v>
@@ -20061,7 +20189,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="130" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D7" s="131" t="s">
         <v>7</v>
@@ -20075,7 +20203,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="130" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D8" s="131" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Calificación considerando examen final
</commit_message>
<xml_diff>
--- a/grades/Calificaciones.xlsx
+++ b/grades/Calificaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/05_Projects_levic/Projects_git/UDG_MCD_Project_Dev_II/grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A17341-2090-4C4F-A6E1-271B7E79002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF16484-67F0-7544-A959-011672DDE32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="PTOS EXTRAS" sheetId="4" r:id="rId5"/>
     <sheet name="ASISTENCIA" sheetId="6" r:id="rId6"/>
     <sheet name="EQUIPOS" sheetId="7" r:id="rId7"/>
+    <sheet name="EXAMEN FINAL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -100,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="1134">
   <si>
     <t>Id. estudiante</t>
   </si>
@@ -3896,9 +3897,6 @@
     <t>PUBLIC.</t>
   </si>
   <si>
-    <t>2022-05-11</t>
-  </si>
-  <si>
     <t>Proyecto personal</t>
   </si>
   <si>
@@ -3927,18 +3925,121 @@
   </si>
   <si>
     <t>Otra</t>
+  </si>
+  <si>
+    <t>EXAMEN FINAL</t>
+  </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Gantt (en Project o PDF)</t>
+  </si>
+  <si>
+    <t>Reporte de resultados</t>
+  </si>
+  <si>
+    <t>Calificación</t>
+  </si>
+  <si>
+    <t>2022-05-18</t>
+  </si>
+  <si>
+    <t>Reporte detallado en Word</t>
+  </si>
+  <si>
+    <t>Archivo de Excel</t>
+  </si>
+  <si>
+    <t>https://github.com/vcuspinera/UDG_MCD_Project_Dev_II/tree/main/final_exam</t>
+  </si>
+  <si>
+    <t>Link a instrucciones y detalle del examen final:</t>
+  </si>
+  <si>
+    <t>Punto a calificar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GITHUB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Subir reporte a GitHub</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CORREO ELECTRONICO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Envío de archivos entregables</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>RESPUESTAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Veracidad y claridad de respuestas</t>
+    </r>
+  </si>
+  <si>
+    <t>Cada punto a calificar se le asignará 0 si no se entregó, 0.5 si se entregó con errores y 1 si es correcto. La calificación del examen final es el promedio de todas las actividades del examen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0\ &quot;%&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4085,8 +4186,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4175,6 +4290,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2C4C84"/>
         <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4569,7 +4690,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4700,7 +4821,6 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4818,23 +4938,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4842,17 +4950,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4869,6 +4968,45 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="16" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -6716,6 +6854,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFABD090"/>
+      <color rgb="FFFF8687"/>
       <color rgb="FF2C4C84"/>
       <color rgb="FF4F85E6"/>
       <color rgb="FF4C80DC"/>
@@ -6734,6 +6874,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>115608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>368299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F2F40D-3E81-F8C6-914E-4EB9B550AB1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8813800" y="1131608"/>
+          <a:ext cx="5664200" cy="2919691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7729,7 +7923,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7750,407 +7944,407 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="str">
         <f>"Puntos acumulados al " &amp; RESUMEN!A40</f>
-        <v>Puntos acumulados al 2022-05-11</v>
+        <v>Puntos acumulados al 2022-05-18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I3" s="84" t="str">
+      <c r="I3" s="83" t="str">
         <f>"|"&amp;A4&amp;"|"&amp;B4&amp;"|"&amp;C4&amp;"|"&amp;D4&amp;"|"&amp;E4&amp;"|"&amp;F4&amp;"|"&amp;G4&amp;"|__"&amp;H4&amp;"__|"</f>
         <v>|Id. estudiante|Nombre|EXPOSICIONES (30%)|QUIZES (CONTROLES DE LECTURA, 30%)|TAREAS (20%)|EXAMEN FINAL (20%)|PUNTOS EXTRAS|__CALIF. FINAL__|</v>
       </c>
     </row>
     <row r="4" spans="1:9" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="119" t="s">
         <v>990</v>
       </c>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="122" t="s">
+      <c r="F4" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="123" t="s">
+      <c r="H4" s="122" t="s">
         <v>989</v>
       </c>
-      <c r="I4" s="107" t="str">
+      <c r="I4" s="106" t="str">
         <f>"|---|---|---|---|---|---|---|---|"</f>
         <v>|---|---|---|---|---|---|---|---|</v>
       </c>
     </row>
     <row r="5" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="127">
+      <c r="A5" s="126">
         <v>220981245</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="125">
+      <c r="C5" s="124">
         <f>RESUMEN!F5*0.3</f>
         <v>30</v>
       </c>
-      <c r="D5" s="125">
+      <c r="D5" s="124">
         <f>RESUMEN!Q5*0.3</f>
         <v>30</v>
       </c>
-      <c r="E5" s="125">
+      <c r="E5" s="124">
         <f>RESUMEN!AC5*0.2</f>
         <v>20</v>
       </c>
-      <c r="F5" s="125">
+      <c r="F5" s="124">
         <f>RESUMEN!AD5*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="125">
+        <v>20</v>
+      </c>
+      <c r="G5" s="124">
         <f>RESUMEN!C24</f>
         <v>10</v>
       </c>
-      <c r="H5" s="126">
-        <f>SUM(C5:G5)</f>
-        <v>90</v>
-      </c>
-      <c r="I5" s="84" t="str">
+      <c r="H5" s="125">
+        <f>IF(SUM(C5:G5)&gt;100,100,SUM(C5:G5))</f>
+        <v>100</v>
+      </c>
+      <c r="I5" s="83" t="str">
         <f>"|"&amp;A5&amp;"|"&amp;B5&amp;"|"&amp;ROUND(C5,1)&amp;"|"&amp;ROUND(D5,1)&amp;"|"&amp;ROUND(E5,1)&amp;"|"&amp;ROUND(F5,1)&amp;"|"&amp;ROUND(G5,1)&amp;"|__"&amp;ROUND(H5,1)&amp;"__|"</f>
-        <v>|220981245|José Raúl Castro Esparza|30|30|20|0|10|__90__|</v>
+        <v>|220981245|José Raúl Castro Esparza|30|30|20|20|10|__100__|</v>
       </c>
     </row>
     <row r="6" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="127">
+      <c r="A6" s="126">
         <v>399515449</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="125">
+      <c r="C6" s="124">
         <f>RESUMEN!F6*0.3</f>
         <v>30</v>
       </c>
-      <c r="D6" s="125">
+      <c r="D6" s="124">
         <f>RESUMEN!Q6*0.3</f>
         <v>30</v>
       </c>
-      <c r="E6" s="125">
+      <c r="E6" s="124">
         <f>RESUMEN!AC6*0.2</f>
         <v>20</v>
       </c>
-      <c r="F6" s="125">
+      <c r="F6" s="124">
         <f>RESUMEN!AD6*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="125">
+        <v>20</v>
+      </c>
+      <c r="G6" s="124">
         <f>RESUMEN!C25</f>
         <v>0</v>
       </c>
-      <c r="H6" s="126">
-        <f t="shared" ref="H6:H14" si="0">SUM(C6:G6)</f>
-        <v>80</v>
-      </c>
-      <c r="I6" s="84" t="str">
+      <c r="H6" s="125">
+        <f t="shared" ref="H6:H14" si="0">IF(SUM(C6:G6)&gt;100,100,SUM(C6:G6))</f>
+        <v>100</v>
+      </c>
+      <c r="I6" s="83" t="str">
         <f t="shared" ref="I6:I14" si="1">"|"&amp;A6&amp;"|"&amp;B6&amp;"|"&amp;ROUND(C6,1)&amp;"|"&amp;ROUND(D6,1)&amp;"|"&amp;ROUND(E6,1)&amp;"|"&amp;ROUND(F6,1)&amp;"|"&amp;ROUND(G6,1)&amp;"|__"&amp;ROUND(H6,1)&amp;"__|"</f>
-        <v>|399515449|Martha Olivia Ramos Lara|30|30|20|0|0|__80__|</v>
+        <v>|399515449|Martha Olivia Ramos Lara|30|30|20|20|0|__100__|</v>
       </c>
     </row>
     <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="127">
+      <c r="A7" s="126">
         <v>207595964</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="125">
+      <c r="C7" s="124">
         <f>RESUMEN!F7*0.3</f>
         <v>30</v>
       </c>
-      <c r="D7" s="125">
+      <c r="D7" s="124">
         <f>RESUMEN!Q7*0.3</f>
         <v>27.444444444444439</v>
       </c>
-      <c r="E7" s="125">
+      <c r="E7" s="124">
         <f>RESUMEN!AC7*0.2</f>
         <v>17.72187878787879</v>
       </c>
-      <c r="F7" s="125">
+      <c r="F7" s="124">
         <f>RESUMEN!AD7*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="125">
+        <v>13</v>
+      </c>
+      <c r="G7" s="124">
         <f>RESUMEN!C26</f>
         <v>0</v>
       </c>
-      <c r="H7" s="126">
+      <c r="H7" s="125">
         <f t="shared" si="0"/>
-        <v>75.166323232323236</v>
-      </c>
-      <c r="I7" s="84" t="str">
+        <v>88.166323232323236</v>
+      </c>
+      <c r="I7" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|207595964|Carol Desireé Ramírez Durán|30|27.4|17.7|0|0|__75.2__|</v>
+        <v>|207595964|Carol Desireé Ramírez Durán|30|27.4|17.7|13|0|__88.2__|</v>
       </c>
     </row>
     <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127">
+      <c r="A8" s="126">
         <v>211776124</v>
       </c>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="125">
+      <c r="C8" s="124">
         <f>RESUMEN!F8*0.3</f>
         <v>30</v>
       </c>
-      <c r="D8" s="125">
+      <c r="D8" s="124">
         <f>RESUMEN!Q8*0.3</f>
         <v>25.444555555555549</v>
       </c>
-      <c r="E8" s="125">
+      <c r="E8" s="124">
         <f>RESUMEN!AC8*0.2</f>
         <v>17.72187878787879</v>
       </c>
-      <c r="F8" s="125">
+      <c r="F8" s="124">
         <f>RESUMEN!AD8*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="125">
+        <v>13</v>
+      </c>
+      <c r="G8" s="124">
         <f>RESUMEN!C27</f>
         <v>0</v>
       </c>
-      <c r="H8" s="126">
+      <c r="H8" s="125">
         <f t="shared" si="0"/>
-        <v>73.166434343434346</v>
-      </c>
-      <c r="I8" s="84" t="str">
+        <v>86.166434343434346</v>
+      </c>
+      <c r="I8" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|211776124|César Iván Vargas López|30|25.4|17.7|0|0|__73.2__|</v>
+        <v>|211776124|César Iván Vargas López|30|25.4|17.7|13|0|__86.2__|</v>
       </c>
     </row>
     <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127">
+      <c r="A9" s="126">
         <v>220981202</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="125">
+      <c r="C9" s="124">
         <f>RESUMEN!F9*0.3</f>
         <v>30</v>
       </c>
-      <c r="D9" s="125">
+      <c r="D9" s="124">
         <f>RESUMEN!Q9*0.3</f>
         <v>23.555499999999999</v>
       </c>
-      <c r="E9" s="125">
+      <c r="E9" s="124">
         <f>RESUMEN!AC9*0.2</f>
         <v>20</v>
       </c>
-      <c r="F9" s="125">
+      <c r="F9" s="124">
         <f>RESUMEN!AD9*0.2</f>
         <v>0</v>
       </c>
-      <c r="G9" s="125">
+      <c r="G9" s="124">
         <f>RESUMEN!C28</f>
         <v>0</v>
       </c>
-      <c r="H9" s="126">
+      <c r="H9" s="125">
         <f t="shared" si="0"/>
         <v>73.555499999999995</v>
       </c>
-      <c r="I9" s="84" t="str">
+      <c r="I9" s="83" t="str">
         <f t="shared" si="1"/>
         <v>|220981202|Pedro Martínez Ayala|30|23.6|20|0|0|__73.6__|</v>
       </c>
     </row>
     <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="127">
+      <c r="A10" s="126">
         <v>398813438</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="125">
+      <c r="C10" s="124">
         <f>RESUMEN!F10*0.3</f>
         <v>30</v>
       </c>
-      <c r="D10" s="125">
+      <c r="D10" s="124">
         <f>RESUMEN!Q10*0.3</f>
         <v>30.000000000000004</v>
       </c>
-      <c r="E10" s="125">
+      <c r="E10" s="124">
         <f>RESUMEN!AC10*0.2</f>
         <v>20</v>
       </c>
-      <c r="F10" s="125">
+      <c r="F10" s="124">
         <f>RESUMEN!AD10*0.2</f>
         <v>0</v>
       </c>
-      <c r="G10" s="125">
+      <c r="G10" s="124">
         <f>RESUMEN!C29</f>
         <v>0</v>
       </c>
-      <c r="H10" s="126">
+      <c r="H10" s="125">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I10" s="84" t="str">
+      <c r="I10" s="83" t="str">
         <f t="shared" si="1"/>
         <v>|398813438|Afra Julieta Lomelí Avila|30|30|20|0|0|__80__|</v>
       </c>
     </row>
     <row r="11" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127">
+      <c r="A11" s="126">
         <v>220981261</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="81" t="s">
         <v>991</v>
       </c>
-      <c r="C11" s="125">
+      <c r="C11" s="124">
         <f>RESUMEN!F11*0.3</f>
         <v>30</v>
       </c>
-      <c r="D11" s="125">
+      <c r="D11" s="124">
         <f>RESUMEN!Q11*0.3</f>
         <v>15.667111111111112</v>
       </c>
-      <c r="E11" s="125">
+      <c r="E11" s="124">
         <f>RESUMEN!AC11*0.2</f>
         <v>18.322566844919788</v>
       </c>
-      <c r="F11" s="125">
+      <c r="F11" s="124">
         <f>RESUMEN!AD11*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="125">
+        <v>15</v>
+      </c>
+      <c r="G11" s="124">
         <f>RESUMEN!C30</f>
         <v>0</v>
       </c>
-      <c r="H11" s="126">
+      <c r="H11" s="125">
         <f t="shared" si="0"/>
-        <v>63.989677956030903</v>
-      </c>
-      <c r="I11" s="84" t="str">
+        <v>78.989677956030903</v>
+      </c>
+      <c r="I11" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|220981261|Mónica Alonso Soria|30|15.7|18.3|0|0|__64__|</v>
+        <v>|220981261|Mónica Alonso Soria|30|15.7|18.3|15|0|__79__|</v>
       </c>
     </row>
     <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="127">
+      <c r="A12" s="126">
         <v>220981296</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="81" t="s">
         <v>992</v>
       </c>
-      <c r="C12" s="125">
+      <c r="C12" s="124">
         <f>RESUMEN!F12*0.3</f>
         <v>30</v>
       </c>
-      <c r="D12" s="125">
+      <c r="D12" s="124">
         <f>RESUMEN!Q12*0.3</f>
         <v>24.666555555555554</v>
       </c>
-      <c r="E12" s="125">
+      <c r="E12" s="124">
         <f>RESUMEN!AC12*0.2</f>
         <v>18.322566844919788</v>
       </c>
-      <c r="F12" s="125">
+      <c r="F12" s="124">
         <f>RESUMEN!AD12*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="125">
+        <v>15</v>
+      </c>
+      <c r="G12" s="124">
         <f>RESUMEN!C31</f>
         <v>10</v>
       </c>
-      <c r="H12" s="126">
+      <c r="H12" s="125">
         <f t="shared" si="0"/>
-        <v>82.989122400475338</v>
-      </c>
-      <c r="I12" s="84" t="str">
+        <v>97.989122400475338</v>
+      </c>
+      <c r="I12" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|0|10|__83__|</v>
+        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|15|10|__98__|</v>
       </c>
     </row>
     <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="127">
+      <c r="A13" s="126">
         <v>220981229</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="C13" s="125">
+      <c r="C13" s="124">
         <f>RESUMEN!F13*0.3</f>
         <v>25.5</v>
       </c>
-      <c r="D13" s="125">
+      <c r="D13" s="124">
         <f>RESUMEN!Q13*0.3</f>
         <v>19.277666666666661</v>
       </c>
-      <c r="E13" s="125">
+      <c r="E13" s="124">
         <f>RESUMEN!AC13*0.2</f>
         <v>17.99818181818182</v>
       </c>
-      <c r="F13" s="125">
+      <c r="F13" s="124">
         <f>RESUMEN!AD13*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="125">
+        <v>20</v>
+      </c>
+      <c r="G13" s="124">
         <f>RESUMEN!C32</f>
         <v>0</v>
       </c>
-      <c r="H13" s="126">
+      <c r="H13" s="125">
         <f t="shared" si="0"/>
-        <v>62.775848484848481</v>
-      </c>
-      <c r="I13" s="84" t="str">
+        <v>82.775848484848481</v>
+      </c>
+      <c r="I13" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|220981229|Luis Enrique Neri González|25.5|19.3|18|0|0|__62.8__|</v>
+        <v>|220981229|Luis Enrique Neri González|25.5|19.3|18|20|0|__82.8__|</v>
       </c>
     </row>
     <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="127">
+      <c r="A14" s="126">
         <v>220981288</v>
       </c>
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="125">
+      <c r="C14" s="124">
         <f>RESUMEN!F14*0.3</f>
         <v>30</v>
       </c>
-      <c r="D14" s="125">
+      <c r="D14" s="124">
         <f>RESUMEN!Q14*0.3</f>
         <v>26.333333333333332</v>
       </c>
-      <c r="E14" s="125">
+      <c r="E14" s="124">
         <f>RESUMEN!AC14*0.2</f>
         <v>17.99818181818182</v>
       </c>
-      <c r="F14" s="125">
+      <c r="F14" s="124">
         <f>RESUMEN!AD14*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="125">
+        <v>20</v>
+      </c>
+      <c r="G14" s="124">
         <f>RESUMEN!C33</f>
         <v>5</v>
       </c>
-      <c r="H14" s="126">
+      <c r="H14" s="125">
         <f t="shared" si="0"/>
-        <v>79.331515151515148</v>
-      </c>
-      <c r="I14" s="84" t="str">
+        <v>99.331515151515148</v>
+      </c>
+      <c r="I14" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|220981288|Carlos Samuel Cruz Mariscal|30|26.3|18|0|5|__79.3__|</v>
+        <v>|220981288|Carlos Samuel Cruz Mariscal|30|26.3|18|20|5|__99.3__|</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="84"/>
+      <c r="I15" s="83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8161,9 +8355,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB78B30B-85E1-8742-88C2-F69873755D79}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A31" sqref="A31"/>
+      <selection pane="topRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8332,7 +8526,7 @@
       </c>
       <c r="C5" s="16">
         <f>F5*0.3+Q5*0.3+AC5*0.2+AD5*0.2</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D5" s="67">
         <v>100</v>
@@ -8344,34 +8538,34 @@
         <f>AVERAGE(D5:E5)</f>
         <v>100</v>
       </c>
-      <c r="G5" s="99">
+      <c r="G5" s="98">
         <v>100</v>
       </c>
-      <c r="H5" s="100">
+      <c r="H5" s="99">
         <v>100</v>
       </c>
-      <c r="I5" s="100">
+      <c r="I5" s="99">
         <v>100</v>
       </c>
-      <c r="J5" s="100">
+      <c r="J5" s="99">
         <v>100</v>
       </c>
-      <c r="K5" s="100">
+      <c r="K5" s="99">
         <v>100</v>
       </c>
-      <c r="L5" s="100">
+      <c r="L5" s="99">
         <v>100</v>
       </c>
-      <c r="M5" s="100">
+      <c r="M5" s="99">
         <v>100</v>
       </c>
-      <c r="N5" s="100">
+      <c r="N5" s="99">
         <v>100</v>
       </c>
-      <c r="O5" s="101">
+      <c r="O5" s="100">
         <v>100</v>
       </c>
-      <c r="P5" s="101">
+      <c r="P5" s="100">
         <v>90</v>
       </c>
       <c r="Q5" s="68">
@@ -8415,8 +8609,9 @@
         <f>AVERAGE(R5:AB5)</f>
         <v>100</v>
       </c>
-      <c r="AD5" s="34">
-        <v>0</v>
+      <c r="AD5" s="68">
+        <f>'EXAMEN FINAL'!$C$16</f>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -8428,7 +8623,7 @@
       </c>
       <c r="C6" s="16">
         <f t="shared" ref="C6:C14" si="0">F6*0.3+Q6*0.3+AC6*0.2+AD6*0.2</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D6" s="67">
         <v>100</v>
@@ -8440,34 +8635,34 @@
         <f t="shared" ref="F6:F14" si="1">AVERAGE(D6:E6)</f>
         <v>100</v>
       </c>
-      <c r="G6" s="99">
+      <c r="G6" s="98">
         <v>100</v>
       </c>
-      <c r="H6" s="100">
+      <c r="H6" s="99">
         <v>100</v>
       </c>
-      <c r="I6" s="100">
+      <c r="I6" s="99">
         <v>100</v>
       </c>
-      <c r="J6" s="100">
+      <c r="J6" s="99">
         <v>100</v>
       </c>
-      <c r="K6" s="100">
+      <c r="K6" s="99">
         <v>100</v>
       </c>
-      <c r="L6" s="100">
+      <c r="L6" s="99">
         <v>100</v>
       </c>
-      <c r="M6" s="100">
+      <c r="M6" s="99">
         <v>100</v>
       </c>
-      <c r="N6" s="100">
+      <c r="N6" s="99">
         <v>100</v>
       </c>
-      <c r="O6" s="101">
+      <c r="O6" s="100">
         <v>100</v>
       </c>
-      <c r="P6" s="101">
+      <c r="P6" s="100">
         <v>0</v>
       </c>
       <c r="Q6" s="68">
@@ -8511,8 +8706,9 @@
         <f t="shared" ref="AC6:AC14" si="3">AVERAGE(R6:AB6)</f>
         <v>100</v>
       </c>
-      <c r="AD6" s="34">
-        <v>0</v>
+      <c r="AD6" s="68">
+        <f>'EXAMEN FINAL'!$C$16</f>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -8524,7 +8720,7 @@
       </c>
       <c r="C7" s="16">
         <f t="shared" si="0"/>
-        <v>75.166323232323236</v>
+        <v>88.166323232323236</v>
       </c>
       <c r="D7" s="67">
         <v>100</v>
@@ -8536,34 +8732,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G7" s="99">
+      <c r="G7" s="98">
         <v>93.33</v>
       </c>
-      <c r="H7" s="100">
+      <c r="H7" s="99">
         <v>80</v>
       </c>
-      <c r="I7" s="100">
+      <c r="I7" s="99">
         <v>86.67</v>
       </c>
-      <c r="J7" s="100">
+      <c r="J7" s="99">
         <v>100</v>
       </c>
-      <c r="K7" s="100">
+      <c r="K7" s="99">
         <v>93.33</v>
       </c>
-      <c r="L7" s="100">
+      <c r="L7" s="99">
         <v>93.333333333333329</v>
       </c>
-      <c r="M7" s="100">
+      <c r="M7" s="99">
         <v>86.67</v>
       </c>
-      <c r="N7" s="100">
+      <c r="N7" s="99">
         <v>93.33</v>
       </c>
-      <c r="O7" s="101">
+      <c r="O7" s="100">
         <v>86.67</v>
       </c>
-      <c r="P7" s="101">
+      <c r="P7" s="100">
         <v>90</v>
       </c>
       <c r="Q7" s="68">
@@ -8607,8 +8803,9 @@
         <f t="shared" si="3"/>
         <v>88.609393939393939</v>
       </c>
-      <c r="AD7" s="34">
-        <v>0</v>
+      <c r="AD7" s="68">
+        <f>'EXAMEN FINAL'!$G$16</f>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -8620,7 +8817,7 @@
       </c>
       <c r="C8" s="16">
         <f t="shared" si="0"/>
-        <v>73.166434343434346</v>
+        <v>86.166434343434346</v>
       </c>
       <c r="D8" s="67">
         <v>100</v>
@@ -8632,35 +8829,35 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G8" s="99">
+      <c r="G8" s="98">
         <v>93.33</v>
       </c>
-      <c r="H8" s="100">
+      <c r="H8" s="99">
         <v>73.33</v>
       </c>
-      <c r="I8" s="100">
+      <c r="I8" s="99">
         <f>QUIZES!C35</f>
         <v>86.67</v>
       </c>
-      <c r="J8" s="100">
+      <c r="J8" s="99">
         <v>100</v>
       </c>
-      <c r="K8" s="100">
+      <c r="K8" s="99">
         <v>80</v>
       </c>
-      <c r="L8" s="100">
+      <c r="L8" s="99">
         <v>86.666666666666671</v>
       </c>
-      <c r="M8" s="100">
+      <c r="M8" s="99">
         <v>86.67</v>
       </c>
-      <c r="N8" s="100">
+      <c r="N8" s="99">
         <v>66.67</v>
       </c>
-      <c r="O8" s="101">
+      <c r="O8" s="100">
         <v>66.67</v>
       </c>
-      <c r="P8" s="101">
+      <c r="P8" s="100">
         <v>90</v>
       </c>
       <c r="Q8" s="68">
@@ -8704,8 +8901,9 @@
         <f t="shared" si="3"/>
         <v>88.609393939393939</v>
       </c>
-      <c r="AD8" s="34">
-        <v>0</v>
+      <c r="AD8" s="68">
+        <f>'EXAMEN FINAL'!$G$16</f>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -8729,34 +8927,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G9" s="99">
+      <c r="G9" s="98">
         <v>36.664999999999999</v>
       </c>
-      <c r="H9" s="100">
+      <c r="H9" s="99">
         <v>100</v>
       </c>
-      <c r="I9" s="100">
+      <c r="I9" s="99">
         <v>100</v>
       </c>
-      <c r="J9" s="100">
+      <c r="J9" s="99">
         <v>93.33</v>
       </c>
-      <c r="K9" s="100">
+      <c r="K9" s="99">
         <v>100</v>
       </c>
-      <c r="L9" s="100">
+      <c r="L9" s="99">
         <v>0</v>
       </c>
-      <c r="M9" s="100">
+      <c r="M9" s="99">
         <v>0</v>
       </c>
-      <c r="N9" s="100">
+      <c r="N9" s="99">
         <v>86.67</v>
       </c>
-      <c r="O9" s="101">
+      <c r="O9" s="100">
         <v>100</v>
       </c>
-      <c r="P9" s="101">
+      <c r="P9" s="100">
         <v>90</v>
       </c>
       <c r="Q9" s="68">
@@ -8800,7 +8998,8 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="AD9" s="34">
+      <c r="AD9" s="68">
+        <f>'EXAMEN FINAL'!$F$16</f>
         <v>0</v>
       </c>
     </row>
@@ -8825,34 +9024,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G10" s="99">
+      <c r="G10" s="98">
         <v>86.67</v>
       </c>
-      <c r="H10" s="100">
+      <c r="H10" s="99">
         <v>100</v>
       </c>
-      <c r="I10" s="100">
+      <c r="I10" s="99">
         <v>100</v>
       </c>
-      <c r="J10" s="100">
+      <c r="J10" s="99">
         <v>100</v>
       </c>
-      <c r="K10" s="100">
+      <c r="K10" s="99">
         <v>100</v>
       </c>
-      <c r="L10" s="100">
+      <c r="L10" s="99">
         <v>100</v>
       </c>
-      <c r="M10" s="100">
+      <c r="M10" s="99">
         <v>100</v>
       </c>
-      <c r="N10" s="100">
+      <c r="N10" s="99">
         <v>100</v>
       </c>
-      <c r="O10" s="101">
+      <c r="O10" s="100">
         <v>100</v>
       </c>
-      <c r="P10" s="101">
+      <c r="P10" s="100">
         <v>100</v>
       </c>
       <c r="Q10" s="68">
@@ -8896,7 +9095,8 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="AD10" s="34">
+      <c r="AD10" s="68">
+        <f>'EXAMEN FINAL'!$F$16</f>
         <v>0</v>
       </c>
     </row>
@@ -8909,7 +9109,7 @@
       </c>
       <c r="C11" s="16">
         <f t="shared" si="0"/>
-        <v>63.989677956030903</v>
+        <v>78.989677956030903</v>
       </c>
       <c r="D11" s="67">
         <v>100</v>
@@ -8921,34 +9121,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G11" s="99">
+      <c r="G11" s="98">
         <v>80</v>
       </c>
-      <c r="H11" s="100">
+      <c r="H11" s="99">
         <v>43.335000000000001</v>
       </c>
-      <c r="I11" s="100">
+      <c r="I11" s="99">
         <v>80</v>
       </c>
-      <c r="J11" s="100">
+      <c r="J11" s="99">
         <v>66.67</v>
       </c>
-      <c r="K11" s="100">
+      <c r="K11" s="99">
         <v>33.335000000000001</v>
       </c>
-      <c r="L11" s="100">
+      <c r="L11" s="99">
         <v>73.333333333333329</v>
       </c>
-      <c r="M11" s="100">
+      <c r="M11" s="99">
         <v>46.67</v>
       </c>
-      <c r="N11" s="100">
+      <c r="N11" s="99">
         <v>46.67</v>
       </c>
-      <c r="O11" s="101">
+      <c r="O11" s="100">
         <v>0</v>
       </c>
-      <c r="P11" s="101">
+      <c r="P11" s="100">
         <v>0</v>
       </c>
       <c r="Q11" s="68">
@@ -8992,8 +9192,9 @@
         <f t="shared" si="3"/>
         <v>91.612834224598927</v>
       </c>
-      <c r="AD11" s="34">
-        <v>0</v>
+      <c r="AD11" s="68">
+        <f>'EXAMEN FINAL'!$D$16</f>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -9005,7 +9206,7 @@
       </c>
       <c r="C12" s="16">
         <f t="shared" si="0"/>
-        <v>72.989122400475338</v>
+        <v>87.989122400475338</v>
       </c>
       <c r="D12" s="67">
         <v>100</v>
@@ -9017,34 +9218,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G12" s="99">
+      <c r="G12" s="98">
         <v>86.67</v>
       </c>
-      <c r="H12" s="100">
+      <c r="H12" s="99">
         <v>93.33</v>
       </c>
-      <c r="I12" s="100">
+      <c r="I12" s="99">
         <v>100</v>
       </c>
-      <c r="J12" s="100">
+      <c r="J12" s="99">
         <v>73.33</v>
       </c>
-      <c r="K12" s="100">
+      <c r="K12" s="99">
         <v>86.67</v>
       </c>
-      <c r="L12" s="100">
+      <c r="L12" s="99">
         <v>66.666666666666657</v>
       </c>
-      <c r="M12" s="100">
+      <c r="M12" s="99">
         <v>73.33</v>
       </c>
-      <c r="N12" s="100">
+      <c r="N12" s="99">
         <v>80</v>
       </c>
-      <c r="O12" s="101">
+      <c r="O12" s="100">
         <v>80</v>
       </c>
-      <c r="P12" s="101">
+      <c r="P12" s="100">
         <v>0</v>
       </c>
       <c r="Q12" s="68">
@@ -9088,8 +9289,9 @@
         <f t="shared" si="3"/>
         <v>91.612834224598927</v>
       </c>
-      <c r="AD12" s="34">
-        <v>0</v>
+      <c r="AD12" s="68">
+        <f>'EXAMEN FINAL'!$D$16</f>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -9100,8 +9302,8 @@
         <v>10</v>
       </c>
       <c r="C13" s="16">
-        <f t="shared" si="0"/>
-        <v>62.775848484848481</v>
+        <f>F13*0.3+Q13*0.3+AC13*0.2+AD13*0.2</f>
+        <v>82.775848484848481</v>
       </c>
       <c r="D13" s="67">
         <v>85</v>
@@ -9113,34 +9315,34 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G13" s="99">
+      <c r="G13" s="98">
         <v>93.33</v>
       </c>
-      <c r="H13" s="100">
+      <c r="H13" s="99">
         <v>73.33</v>
       </c>
-      <c r="I13" s="100">
+      <c r="I13" s="99">
         <v>86.67</v>
       </c>
-      <c r="J13" s="100">
+      <c r="J13" s="99">
         <v>0</v>
       </c>
-      <c r="K13" s="100">
+      <c r="K13" s="99">
         <v>86.67</v>
       </c>
-      <c r="L13" s="100">
+      <c r="L13" s="99">
         <v>60</v>
       </c>
-      <c r="M13" s="100">
+      <c r="M13" s="99">
         <v>93.33</v>
       </c>
-      <c r="N13" s="100">
+      <c r="N13" s="99">
         <v>0</v>
       </c>
-      <c r="O13" s="101">
+      <c r="O13" s="100">
         <v>0</v>
       </c>
-      <c r="P13" s="101">
+      <c r="P13" s="100">
         <v>85</v>
       </c>
       <c r="Q13" s="68">
@@ -9184,8 +9386,9 @@
         <f t="shared" si="3"/>
         <v>89.990909090909099</v>
       </c>
-      <c r="AD13" s="34">
-        <v>0</v>
+      <c r="AD13" s="68">
+        <f>'EXAMEN FINAL'!$E$16</f>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
@@ -9197,7 +9400,7 @@
       </c>
       <c r="C14" s="62">
         <f t="shared" si="0"/>
-        <v>74.331515151515148</v>
+        <v>94.331515151515148</v>
       </c>
       <c r="D14" s="69">
         <v>100</v>
@@ -9209,34 +9412,34 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G14" s="102">
+      <c r="G14" s="101">
         <v>100</v>
       </c>
-      <c r="H14" s="103">
+      <c r="H14" s="102">
         <v>100</v>
       </c>
-      <c r="I14" s="103">
+      <c r="I14" s="102">
         <v>93.33</v>
       </c>
-      <c r="J14" s="103">
+      <c r="J14" s="102">
         <v>100</v>
       </c>
-      <c r="K14" s="103">
+      <c r="K14" s="102">
         <v>100</v>
       </c>
-      <c r="L14" s="103">
+      <c r="L14" s="102">
         <v>80</v>
       </c>
-      <c r="M14" s="103">
+      <c r="M14" s="102">
         <v>80</v>
       </c>
-      <c r="N14" s="103">
+      <c r="N14" s="102">
         <v>46.67</v>
       </c>
-      <c r="O14" s="104">
+      <c r="O14" s="103">
         <v>43.34</v>
       </c>
-      <c r="P14" s="104">
+      <c r="P14" s="103">
         <v>90</v>
       </c>
       <c r="Q14" s="71">
@@ -9280,8 +9483,9 @@
         <f t="shared" si="3"/>
         <v>89.990909090909099</v>
       </c>
-      <c r="AD14" s="80">
-        <v>0</v>
+      <c r="AD14" s="68">
+        <f>'EXAMEN FINAL'!$E$16</f>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -9309,7 +9513,7 @@
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="32"/>
-      <c r="J22" s="108"/>
+      <c r="J22" s="107"/>
     </row>
     <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
@@ -9518,7 +9722,7 @@
       </c>
       <c r="D30" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="36">
         <v>0</v>
@@ -9574,7 +9778,7 @@
       </c>
       <c r="D32" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="36">
         <v>0</v>
@@ -9618,7 +9822,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="109" t="s">
+      <c r="A35" s="108" t="s">
         <v>1086</v>
       </c>
     </row>
@@ -9629,8 +9833,8 @@
       <c r="B39" s="22"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="124" t="s">
-        <v>1109</v>
+      <c r="A40" s="123" t="s">
+        <v>1124</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -9658,7 +9862,7 @@
       </c>
       <c r="C43" s="16">
         <f>MIN(100,C5+C24)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -9670,7 +9874,7 @@
       </c>
       <c r="C44" s="16">
         <f t="shared" ref="C44:C52" si="6">MIN(100,C6+C25)</f>
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -9682,7 +9886,7 @@
       </c>
       <c r="C45" s="16">
         <f t="shared" si="6"/>
-        <v>75.166323232323236</v>
+        <v>88.166323232323236</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -9694,7 +9898,7 @@
       </c>
       <c r="C46" s="16">
         <f t="shared" si="6"/>
-        <v>73.166434343434346</v>
+        <v>86.166434343434346</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -9730,7 +9934,7 @@
       </c>
       <c r="C49" s="16">
         <f t="shared" si="6"/>
-        <v>63.989677956030903</v>
+        <v>78.989677956030903</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -9742,7 +9946,7 @@
       </c>
       <c r="C50" s="16">
         <f t="shared" si="6"/>
-        <v>82.989122400475338</v>
+        <v>97.989122400475338</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -9754,7 +9958,7 @@
       </c>
       <c r="C51" s="16">
         <f t="shared" si="6"/>
-        <v>62.775848484848481</v>
+        <v>82.775848484848481</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -9766,7 +9970,7 @@
       </c>
       <c r="C52" s="16">
         <f t="shared" si="6"/>
-        <v>79.331515151515148</v>
+        <v>99.331515151515148</v>
       </c>
     </row>
   </sheetData>
@@ -9848,7 +10052,7 @@
         <f>(F3-E3)*24*60</f>
         <v>1.8833332392387092</v>
       </c>
-      <c r="H3" s="85" t="str">
+      <c r="H3" s="84" t="str">
         <f>HOUR(F3)&amp;IF(MINUTE(F3)&gt;=10, ":"&amp;MINUTE(F3), ":0"&amp;MINUTE(F3))</f>
         <v>20:50</v>
       </c>
@@ -9875,7 +10079,7 @@
         <f t="shared" ref="G4:G12" si="1">(F4-E4)*24*60</f>
         <v>7.4833332491107285</v>
       </c>
-      <c r="H4" s="86" t="str">
+      <c r="H4" s="85" t="str">
         <f t="shared" ref="H4:H12" si="2">HOUR(F4)&amp;IF(MINUTE(F4)&gt;=10, ":"&amp;MINUTE(F4), ":0"&amp;MINUTE(F4))</f>
         <v>20:50</v>
       </c>
@@ -9902,7 +10106,7 @@
         <f t="shared" si="1"/>
         <v>61.233333261916414</v>
       </c>
-      <c r="H5" s="85" t="str">
+      <c r="H5" s="84" t="str">
         <f t="shared" si="2"/>
         <v>21:05</v>
       </c>
@@ -9929,7 +10133,7 @@
         <f t="shared" si="1"/>
         <v>68.300000071758404</v>
       </c>
-      <c r="H6" s="86" t="str">
+      <c r="H6" s="85" t="str">
         <f t="shared" si="2"/>
         <v>21:08</v>
       </c>
@@ -9956,7 +10160,7 @@
         <f t="shared" si="1"/>
         <v>79.10000006086193</v>
       </c>
-      <c r="H7" s="85" t="str">
+      <c r="H7" s="84" t="str">
         <f t="shared" si="2"/>
         <v>21:09</v>
       </c>
@@ -9983,7 +10187,7 @@
         <f t="shared" si="1"/>
         <v>34.200000000419095</v>
       </c>
-      <c r="H8" s="86" t="str">
+      <c r="H8" s="85" t="str">
         <f t="shared" si="2"/>
         <v>21:17</v>
       </c>
@@ -10010,7 +10214,7 @@
         <f t="shared" si="1"/>
         <v>18.366666622459888</v>
       </c>
-      <c r="H9" s="85" t="str">
+      <c r="H9" s="84" t="str">
         <f t="shared" si="2"/>
         <v>21:42</v>
       </c>
@@ -10037,7 +10241,7 @@
         <f t="shared" si="1"/>
         <v>57.050000061281025</v>
       </c>
-      <c r="H10" s="86" t="str">
+      <c r="H10" s="85" t="str">
         <f t="shared" si="2"/>
         <v>21:58</v>
       </c>
@@ -10064,7 +10268,7 @@
         <f t="shared" si="1"/>
         <v>85.250000021187589</v>
       </c>
-      <c r="H11" s="85" t="str">
+      <c r="H11" s="84" t="str">
         <f t="shared" si="2"/>
         <v>22:10</v>
       </c>
@@ -10093,7 +10297,7 @@
         <f t="shared" si="1"/>
         <v>34.449999985517934</v>
       </c>
-      <c r="H12" s="92" t="str">
+      <c r="H12" s="91" t="str">
         <f t="shared" si="2"/>
         <v>23:52</v>
       </c>
@@ -10152,7 +10356,7 @@
         <f>(F17-E17)*24*60</f>
         <v>0.36666662665084004</v>
       </c>
-      <c r="H17" s="85" t="str">
+      <c r="H17" s="84" t="str">
         <f t="shared" ref="H17:H26" si="3">HOUR(F17)&amp;IF(MINUTE(F17)&gt;=10, ":"&amp;MINUTE(F17), ":0"&amp;MINUTE(F17))</f>
         <v>19:46</v>
       </c>
@@ -10179,7 +10383,7 @@
         <f t="shared" ref="G18:G26" si="5">(F18-E18)*24*60</f>
         <v>10.10000002454035</v>
       </c>
-      <c r="H18" s="86" t="str">
+      <c r="H18" s="85" t="str">
         <f t="shared" si="3"/>
         <v>19:54</v>
       </c>
@@ -10206,7 +10410,7 @@
         <f t="shared" si="5"/>
         <v>23.700000102398917</v>
       </c>
-      <c r="H19" s="85" t="str">
+      <c r="H19" s="84" t="str">
         <f t="shared" si="3"/>
         <v>20:32</v>
       </c>
@@ -10233,7 +10437,7 @@
         <f t="shared" si="5"/>
         <v>53.783333280589432</v>
       </c>
-      <c r="H20" s="86" t="str">
+      <c r="H20" s="85" t="str">
         <f t="shared" si="3"/>
         <v>20:33</v>
       </c>
@@ -10260,7 +10464,7 @@
         <f t="shared" si="5"/>
         <v>25.850000018253922</v>
       </c>
-      <c r="H21" s="85" t="str">
+      <c r="H21" s="84" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10287,7 +10491,7 @@
         <f t="shared" si="5"/>
         <v>20.766666680574417</v>
       </c>
-      <c r="H22" s="86" t="str">
+      <c r="H22" s="85" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10314,7 +10518,7 @@
         <f t="shared" si="5"/>
         <v>26.416666806908324</v>
       </c>
-      <c r="H23" s="85" t="str">
+      <c r="H23" s="84" t="str">
         <f t="shared" si="3"/>
         <v>20:34</v>
       </c>
@@ -10341,7 +10545,7 @@
         <f t="shared" si="5"/>
         <v>2.366666643647477</v>
       </c>
-      <c r="H24" s="86" t="str">
+      <c r="H24" s="85" t="str">
         <f t="shared" si="3"/>
         <v>20:48</v>
       </c>
@@ -10368,7 +10572,7 @@
         <f t="shared" si="5"/>
         <v>77.049999937880784</v>
       </c>
-      <c r="H25" s="85" t="str">
+      <c r="H25" s="84" t="str">
         <f t="shared" si="3"/>
         <v>20:59</v>
       </c>
@@ -10397,7 +10601,7 @@
         <f t="shared" si="5"/>
         <v>61.149999888148159</v>
       </c>
-      <c r="H26" s="92" t="str">
+      <c r="H26" s="91" t="str">
         <f t="shared" si="3"/>
         <v>21:14</v>
       </c>
@@ -10456,7 +10660,7 @@
         <f>(F31-E31)*24*60</f>
         <v>10.066666599595919</v>
       </c>
-      <c r="H31" s="85" t="str">
+      <c r="H31" s="84" t="str">
         <f t="shared" ref="H31:H40" si="6">HOUR(F31)&amp;IF(MINUTE(F31)&gt;=10, ":"&amp;MINUTE(F31), ":0"&amp;MINUTE(F31))</f>
         <v>18:38</v>
       </c>
@@ -10483,7 +10687,7 @@
         <f t="shared" ref="G32:G40" si="8">(F32-E32)*24*60</f>
         <v>1.2166666577104479</v>
       </c>
-      <c r="H32" s="86" t="str">
+      <c r="H32" s="85" t="str">
         <f t="shared" si="6"/>
         <v>19:29</v>
       </c>
@@ -10510,7 +10714,7 @@
         <f t="shared" si="8"/>
         <v>17.533333440078422</v>
       </c>
-      <c r="H33" s="85" t="str">
+      <c r="H33" s="84" t="str">
         <f t="shared" si="6"/>
         <v>20:24</v>
       </c>
@@ -10537,7 +10741,7 @@
         <f t="shared" si="8"/>
         <v>22.833333358867094</v>
       </c>
-      <c r="H34" s="86" t="str">
+      <c r="H34" s="85" t="str">
         <f t="shared" si="6"/>
         <v>20:29</v>
       </c>
@@ -10564,7 +10768,7 @@
         <f t="shared" si="8"/>
         <v>27.583333348156884</v>
       </c>
-      <c r="H35" s="85" t="str">
+      <c r="H35" s="84" t="str">
         <f t="shared" si="6"/>
         <v>20:36</v>
       </c>
@@ -10591,7 +10795,7 @@
         <f t="shared" si="8"/>
         <v>34.833333303686231</v>
       </c>
-      <c r="H36" s="86" t="str">
+      <c r="H36" s="85" t="str">
         <f t="shared" si="6"/>
         <v>20:40</v>
       </c>
@@ -10618,7 +10822,7 @@
         <f t="shared" si="8"/>
         <v>34.049999944400042</v>
       </c>
-      <c r="H37" s="85" t="str">
+      <c r="H37" s="84" t="str">
         <f t="shared" si="6"/>
         <v>20:41</v>
       </c>
@@ -10645,7 +10849,7 @@
         <f t="shared" si="8"/>
         <v>23.449999970616773</v>
       </c>
-      <c r="H38" s="86" t="str">
+      <c r="H38" s="85" t="str">
         <f t="shared" si="6"/>
         <v>20:42</v>
       </c>
@@ -10672,7 +10876,7 @@
         <f t="shared" si="8"/>
         <v>24.316666703671217</v>
       </c>
-      <c r="H39" s="85" t="str">
+      <c r="H39" s="84" t="str">
         <f t="shared" si="6"/>
         <v>20:44</v>
       </c>
@@ -10699,7 +10903,7 @@
         <f t="shared" si="8"/>
         <v>1.6333333903457969</v>
       </c>
-      <c r="H40" s="86" t="str">
+      <c r="H40" s="85" t="str">
         <f t="shared" si="6"/>
         <v>20:57</v>
       </c>
@@ -10758,7 +10962,7 @@
         <f>(F45-E45)*24*60</f>
         <v>2.9000000073574483</v>
       </c>
-      <c r="H45" s="85" t="str">
+      <c r="H45" s="84" t="str">
         <f t="shared" ref="H45:H53" si="9">HOUR(F45)&amp;IF(MINUTE(F45)&gt;=10, ":"&amp;MINUTE(F45), ":0"&amp;MINUTE(F45))</f>
         <v>19:01</v>
       </c>
@@ -10785,7 +10989,7 @@
         <f t="shared" ref="G46:G53" si="11">(F46-E46)*24*60</f>
         <v>3.4500001044943929</v>
       </c>
-      <c r="H46" s="86" t="str">
+      <c r="H46" s="85" t="str">
         <f t="shared" si="9"/>
         <v>19:36</v>
       </c>
@@ -10812,7 +11016,7 @@
         <f t="shared" si="11"/>
         <v>12.300000046379864</v>
       </c>
-      <c r="H47" s="85" t="str">
+      <c r="H47" s="84" t="str">
         <f t="shared" si="9"/>
         <v>20:25</v>
       </c>
@@ -10839,7 +11043,7 @@
         <f t="shared" si="11"/>
         <v>14.150000017834827</v>
       </c>
-      <c r="H48" s="86" t="str">
+      <c r="H48" s="85" t="str">
         <f t="shared" si="9"/>
         <v>20:29</v>
       </c>
@@ -10866,7 +11070,7 @@
         <f t="shared" si="11"/>
         <v>98.449999921722338</v>
       </c>
-      <c r="H49" s="85" t="str">
+      <c r="H49" s="84" t="str">
         <f t="shared" si="9"/>
         <v>20:37</v>
       </c>
@@ -10893,7 +11097,7 @@
         <f t="shared" si="11"/>
         <v>2.0666666887700558</v>
       </c>
-      <c r="H50" s="86" t="str">
+      <c r="H50" s="85" t="str">
         <f t="shared" si="9"/>
         <v>20:41</v>
       </c>
@@ -10920,7 +11124,7 @@
         <f t="shared" si="11"/>
         <v>69.46666675969027</v>
       </c>
-      <c r="H51" s="85" t="str">
+      <c r="H51" s="84" t="str">
         <f t="shared" si="9"/>
         <v>20:41</v>
       </c>
@@ -10947,7 +11151,7 @@
         <f t="shared" si="11"/>
         <v>28.866666677640751</v>
       </c>
-      <c r="H52" s="86" t="str">
+      <c r="H52" s="85" t="str">
         <f t="shared" si="9"/>
         <v>20:42</v>
       </c>
@@ -10974,29 +11178,29 @@
         <f t="shared" si="11"/>
         <v>3.8833333924412727</v>
       </c>
-      <c r="H53" s="85" t="str">
+      <c r="H53" s="84" t="str">
         <f t="shared" si="9"/>
         <v>21:08</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="90" t="s">
+      <c r="A54" s="89" t="s">
         <v>695</v>
       </c>
-      <c r="B54" s="90">
+      <c r="B54" s="89">
         <v>0</v>
       </c>
-      <c r="C54" s="93">
+      <c r="C54" s="92">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="D54" s="90" t="s">
+      <c r="D54" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E54" s="94"/>
-      <c r="F54" s="94"/>
-      <c r="G54" s="94"/>
-      <c r="H54" s="95"/>
+      <c r="E54" s="93"/>
+      <c r="F54" s="93"/>
+      <c r="G54" s="93"/>
+      <c r="H54" s="94"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -11052,7 +11256,7 @@
         <f>(F59-E59)*24*60</f>
         <v>1.3500000012572855</v>
       </c>
-      <c r="H59" s="85" t="str">
+      <c r="H59" s="84" t="str">
         <f t="shared" ref="H59:H68" si="12">HOUR(F59)&amp;IF(MINUTE(F59)&gt;=10, ":"&amp;MINUTE(F59), ":0"&amp;MINUTE(F59))</f>
         <v>19:20</v>
       </c>
@@ -11079,7 +11283,7 @@
         <f t="shared" ref="G60:G68" si="14">(F60-E60)*24*60</f>
         <v>1.2500000617001206</v>
       </c>
-      <c r="H60" s="86" t="str">
+      <c r="H60" s="85" t="str">
         <f t="shared" si="12"/>
         <v>19:27</v>
       </c>
@@ -11106,7 +11310,7 @@
         <f t="shared" si="14"/>
         <v>18.716666536638513</v>
       </c>
-      <c r="H61" s="85" t="str">
+      <c r="H61" s="84" t="str">
         <f t="shared" si="12"/>
         <v>20:19</v>
       </c>
@@ -11133,7 +11337,7 @@
         <f t="shared" si="14"/>
         <v>27.316666661063209</v>
       </c>
-      <c r="H62" s="86" t="str">
+      <c r="H62" s="85" t="str">
         <f t="shared" si="12"/>
         <v>20:29</v>
       </c>
@@ -11160,7 +11364,7 @@
         <f t="shared" si="14"/>
         <v>61.666666707023978</v>
       </c>
-      <c r="H63" s="85" t="str">
+      <c r="H63" s="84" t="str">
         <f t="shared" si="12"/>
         <v>20:32</v>
       </c>
@@ -11187,7 +11391,7 @@
         <f t="shared" si="14"/>
         <v>29.033333425177261</v>
       </c>
-      <c r="H64" s="86" t="str">
+      <c r="H64" s="85" t="str">
         <f t="shared" si="12"/>
         <v>20:33</v>
       </c>
@@ -11214,7 +11418,7 @@
         <f t="shared" si="14"/>
         <v>35.316666582366452</v>
       </c>
-      <c r="H65" s="85" t="str">
+      <c r="H65" s="84" t="str">
         <f t="shared" si="12"/>
         <v>20:36</v>
       </c>
@@ -11241,7 +11445,7 @@
         <f t="shared" si="14"/>
         <v>4.2999999783933163</v>
       </c>
-      <c r="H66" s="86" t="str">
+      <c r="H66" s="85" t="str">
         <f t="shared" si="12"/>
         <v>20:37</v>
       </c>
@@ -11268,7 +11472,7 @@
         <f t="shared" si="14"/>
         <v>62.583333409857005</v>
       </c>
-      <c r="H67" s="85" t="str">
+      <c r="H67" s="84" t="str">
         <f t="shared" si="12"/>
         <v>20:37</v>
       </c>
@@ -11293,11 +11497,11 @@
       <c r="F68" s="41">
         <v>44619.626990740697</v>
       </c>
-      <c r="G68" s="89">
+      <c r="G68" s="88">
         <f t="shared" si="14"/>
         <v>83.099999948171899</v>
       </c>
-      <c r="H68" s="92" t="str">
+      <c r="H68" s="91" t="str">
         <f t="shared" si="12"/>
         <v>15:02</v>
       </c>
@@ -11358,7 +11562,7 @@
         <f>(F73-E73)*24*60</f>
         <v>4.600000079954043</v>
       </c>
-      <c r="H73" s="87" t="str">
+      <c r="H73" s="86" t="str">
         <f t="shared" ref="H73:H82" si="15">HOUR(F73)&amp;IF(MINUTE(F73)&gt;=10, ":"&amp;MINUTE(F73), ":0"&amp;MINUTE(F73))</f>
         <v>21:42</v>
       </c>
@@ -11385,7 +11589,7 @@
         <f t="shared" ref="G74:G82" si="17">(F74-E74)*24*60</f>
         <v>2.649999896530062</v>
       </c>
-      <c r="H74" s="86" t="str">
+      <c r="H74" s="85" t="str">
         <f t="shared" si="15"/>
         <v>19:09</v>
       </c>
@@ -11412,7 +11616,7 @@
         <f t="shared" si="17"/>
         <v>3.1499998562503606</v>
       </c>
-      <c r="H75" s="85" t="str">
+      <c r="H75" s="84" t="str">
         <f t="shared" si="15"/>
         <v>19:20</v>
       </c>
@@ -11439,7 +11643,7 @@
         <f t="shared" si="17"/>
         <v>8.4500000684056431</v>
       </c>
-      <c r="H76" s="86" t="str">
+      <c r="H76" s="85" t="str">
         <f t="shared" si="15"/>
         <v>20:07</v>
       </c>
@@ -11466,7 +11670,7 @@
         <f t="shared" si="17"/>
         <v>17.466666768305004</v>
       </c>
-      <c r="H77" s="85" t="str">
+      <c r="H77" s="84" t="str">
         <f t="shared" si="15"/>
         <v>20:13</v>
       </c>
@@ -11493,7 +11697,7 @@
         <f t="shared" si="17"/>
         <v>28.566666576080024</v>
       </c>
-      <c r="H78" s="86" t="str">
+      <c r="H78" s="85" t="str">
         <f t="shared" si="15"/>
         <v>20:26</v>
       </c>
@@ -11520,7 +11724,7 @@
         <f t="shared" si="17"/>
         <v>36.033333406085148</v>
       </c>
-      <c r="H79" s="85" t="str">
+      <c r="H79" s="84" t="str">
         <f t="shared" si="15"/>
         <v>20:35</v>
       </c>
@@ -11547,7 +11751,7 @@
         <f t="shared" si="17"/>
         <v>40.999999976484105</v>
       </c>
-      <c r="H80" s="86" t="str">
+      <c r="H80" s="85" t="str">
         <f t="shared" si="15"/>
         <v>20:40</v>
       </c>
@@ -11574,7 +11778,7 @@
         <f t="shared" si="17"/>
         <v>44.883333358447999</v>
       </c>
-      <c r="H81" s="85" t="str">
+      <c r="H81" s="84" t="str">
         <f t="shared" si="15"/>
         <v>21:17</v>
       </c>
@@ -11601,29 +11805,29 @@
         <f t="shared" si="17"/>
         <v>36.316666658967733</v>
       </c>
-      <c r="H82" s="86" t="str">
+      <c r="H82" s="85" t="str">
         <f t="shared" si="15"/>
         <v>21:26</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="91" t="s">
+      <c r="A83" s="90" t="s">
         <v>686</v>
       </c>
-      <c r="B83" s="91">
+      <c r="B83" s="90">
         <v>0</v>
       </c>
-      <c r="C83" s="96">
+      <c r="C83" s="95">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D83" s="90" t="s">
+      <c r="D83" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E83" s="97"/>
-      <c r="F83" s="97"/>
-      <c r="G83" s="97"/>
-      <c r="H83" s="98"/>
+      <c r="E83" s="96"/>
+      <c r="F83" s="96"/>
+      <c r="G83" s="96"/>
+      <c r="H83" s="97"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -11679,7 +11883,7 @@
         <f>(F88-E88)*24*60</f>
         <v>1.0500000463798642</v>
       </c>
-      <c r="H88" s="85" t="str">
+      <c r="H88" s="84" t="str">
         <f t="shared" ref="H88:H97" si="18">HOUR(F88)&amp;IF(MINUTE(F88)&gt;=10, ":"&amp;MINUTE(F88), ":0"&amp;MINUTE(F88))</f>
         <v>20:02</v>
       </c>
@@ -11706,7 +11910,7 @@
         <f t="shared" ref="G89:G97" si="20">(F89-E89)*24*60</f>
         <v>13.966666704509407</v>
       </c>
-      <c r="H89" s="86" t="str">
+      <c r="H89" s="85" t="str">
         <f t="shared" si="18"/>
         <v>20:14</v>
       </c>
@@ -11733,7 +11937,7 @@
         <f t="shared" si="20"/>
         <v>40.983333410695195</v>
       </c>
-      <c r="H90" s="85" t="str">
+      <c r="H90" s="84" t="str">
         <f t="shared" si="18"/>
         <v>20:41</v>
       </c>
@@ -11760,7 +11964,7 @@
         <f t="shared" si="20"/>
         <v>2.3666666331700981</v>
       </c>
-      <c r="H91" s="86" t="str">
+      <c r="H91" s="85" t="str">
         <f t="shared" si="18"/>
         <v>20:42</v>
       </c>
@@ -11789,7 +11993,7 @@
         <f t="shared" si="20"/>
         <v>0.61666675843298435</v>
       </c>
-      <c r="H92" s="88" t="str">
+      <c r="H92" s="87" t="str">
         <f t="shared" si="18"/>
         <v>20:43</v>
       </c>
@@ -11816,7 +12020,7 @@
         <f t="shared" si="20"/>
         <v>49.81666665058583</v>
       </c>
-      <c r="H93" s="86" t="str">
+      <c r="H93" s="85" t="str">
         <f t="shared" si="18"/>
         <v>20:50</v>
       </c>
@@ -11843,7 +12047,7 @@
         <f t="shared" si="20"/>
         <v>49.333333246177062</v>
       </c>
-      <c r="H94" s="85" t="str">
+      <c r="H94" s="84" t="str">
         <f t="shared" si="18"/>
         <v>20:50</v>
       </c>
@@ -11870,7 +12074,7 @@
         <f t="shared" si="20"/>
         <v>90.133333343546838</v>
       </c>
-      <c r="H95" s="86" t="str">
+      <c r="H95" s="85" t="str">
         <f t="shared" si="18"/>
         <v>20:56</v>
       </c>
@@ -11897,7 +12101,7 @@
         <f t="shared" si="20"/>
         <v>86.583333309972659</v>
       </c>
-      <c r="H96" s="85" t="str">
+      <c r="H96" s="84" t="str">
         <f t="shared" si="18"/>
         <v>21:20</v>
       </c>
@@ -11924,29 +12128,29 @@
         <f t="shared" si="20"/>
         <v>76.93333343253471</v>
       </c>
-      <c r="H97" s="86" t="str">
+      <c r="H97" s="85" t="str">
         <f t="shared" si="18"/>
         <v>21:20</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="91" t="s">
+      <c r="A98" s="90" t="s">
         <v>686</v>
       </c>
-      <c r="B98" s="91">
+      <c r="B98" s="90">
         <v>0</v>
       </c>
-      <c r="C98" s="96">
+      <c r="C98" s="95">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="D98" s="90" t="s">
+      <c r="D98" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E98" s="97"/>
-      <c r="F98" s="97"/>
-      <c r="G98" s="97"/>
-      <c r="H98" s="98"/>
+      <c r="E98" s="96"/>
+      <c r="F98" s="96"/>
+      <c r="G98" s="96"/>
+      <c r="H98" s="97"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
@@ -12002,7 +12206,7 @@
         <f>(F103-E103)*24*60</f>
         <v>53.033333325292915</v>
       </c>
-      <c r="H103" s="85" t="str">
+      <c r="H103" s="84" t="str">
         <f t="shared" ref="H103:H111" si="21">HOUR(F103)&amp;IF(MINUTE(F103)&gt;=10, ":"&amp;MINUTE(F103), ":0"&amp;MINUTE(F103))</f>
         <v>19:08</v>
       </c>
@@ -12029,7 +12233,7 @@
         <f t="shared" ref="G104:G111" si="23">(F104-E104)*24*60</f>
         <v>2.416666749631986</v>
       </c>
-      <c r="H104" s="86" t="str">
+      <c r="H104" s="85" t="str">
         <f t="shared" si="21"/>
         <v>20:06</v>
       </c>
@@ -12056,7 +12260,7 @@
         <f t="shared" si="23"/>
         <v>3.1999999727122486</v>
       </c>
-      <c r="H105" s="85" t="str">
+      <c r="H105" s="84" t="str">
         <f t="shared" si="21"/>
         <v>20:07</v>
       </c>
@@ -12083,7 +12287,7 @@
         <f t="shared" si="23"/>
         <v>1.9333333452232182</v>
       </c>
-      <c r="H106" s="86" t="str">
+      <c r="H106" s="85" t="str">
         <f t="shared" si="21"/>
         <v>20:07</v>
       </c>
@@ -12110,7 +12314,7 @@
         <f t="shared" si="23"/>
         <v>18.433333294233307</v>
       </c>
-      <c r="H107" s="85" t="str">
+      <c r="H107" s="84" t="str">
         <f t="shared" si="21"/>
         <v>20:22</v>
       </c>
@@ -12137,7 +12341,7 @@
         <f t="shared" si="23"/>
         <v>60.26666673598811</v>
       </c>
-      <c r="H108" s="86" t="str">
+      <c r="H108" s="85" t="str">
         <f t="shared" si="21"/>
         <v>20:24</v>
       </c>
@@ -12164,7 +12368,7 @@
         <f t="shared" si="23"/>
         <v>8.2333333406131715</v>
       </c>
-      <c r="H109" s="85" t="str">
+      <c r="H109" s="84" t="str">
         <f t="shared" si="21"/>
         <v>20:35</v>
       </c>
@@ -12191,7 +12395,7 @@
         <f t="shared" si="23"/>
         <v>38.300000110175461</v>
       </c>
-      <c r="H110" s="86" t="str">
+      <c r="H110" s="85" t="str">
         <f t="shared" si="21"/>
         <v>20:42</v>
       </c>
@@ -12218,29 +12422,29 @@
         <f t="shared" si="23"/>
         <v>1.7833334463648498</v>
       </c>
-      <c r="H111" s="85" t="str">
+      <c r="H111" s="84" t="str">
         <f t="shared" si="21"/>
         <v>20:44</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="90" t="s">
+      <c r="A112" s="89" t="s">
         <v>695</v>
       </c>
-      <c r="B112" s="90">
+      <c r="B112" s="89">
         <v>0</v>
       </c>
-      <c r="C112" s="93">
+      <c r="C112" s="92">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="D112" s="90" t="s">
+      <c r="D112" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E112" s="94"/>
-      <c r="F112" s="94"/>
-      <c r="G112" s="95"/>
-      <c r="H112" s="95"/>
+      <c r="E112" s="93"/>
+      <c r="F112" s="93"/>
+      <c r="G112" s="94"/>
+      <c r="H112" s="94"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
@@ -12296,7 +12500,7 @@
         <f>(F117-E117)*24*60</f>
         <v>2.8666666033677757</v>
       </c>
-      <c r="H117" s="85" t="str">
+      <c r="H117" s="84" t="str">
         <f t="shared" ref="H117:H124" si="24">HOUR(F117)&amp;IF(MINUTE(F117)&gt;=10, ":"&amp;MINUTE(F117), ":0"&amp;MINUTE(F117))</f>
         <v>19:04</v>
       </c>
@@ -12323,7 +12527,7 @@
         <f t="shared" ref="G118:G124" si="26">(F118-E118)*24*60</f>
         <v>2.1500000625383109</v>
       </c>
-      <c r="H118" s="86" t="str">
+      <c r="H118" s="85" t="str">
         <f t="shared" si="24"/>
         <v>19:30</v>
       </c>
@@ -12350,7 +12554,7 @@
         <f t="shared" si="26"/>
         <v>1.8833333754446357</v>
       </c>
-      <c r="H119" s="85" t="str">
+      <c r="H119" s="84" t="str">
         <f t="shared" si="24"/>
         <v>20:03</v>
       </c>
@@ -12377,7 +12581,7 @@
         <f t="shared" si="26"/>
         <v>25.966666659805924</v>
       </c>
-      <c r="H120" s="86" t="str">
+      <c r="H120" s="85" t="str">
         <f t="shared" si="24"/>
         <v>20:04</v>
       </c>
@@ -12404,7 +12608,7 @@
         <f t="shared" si="26"/>
         <v>30.80000001238659</v>
       </c>
-      <c r="H121" s="85" t="str">
+      <c r="H121" s="84" t="str">
         <f t="shared" si="24"/>
         <v>20:07</v>
       </c>
@@ -12431,7 +12635,7 @@
         <f t="shared" si="26"/>
         <v>72.600000039674342</v>
       </c>
-      <c r="H122" s="86" t="str">
+      <c r="H122" s="85" t="str">
         <f t="shared" si="24"/>
         <v>21:17</v>
       </c>
@@ -12458,7 +12662,7 @@
         <f t="shared" si="26"/>
         <v>2.3333333758637309</v>
       </c>
-      <c r="H123" s="85" t="str">
+      <c r="H123" s="84" t="str">
         <f t="shared" si="24"/>
         <v>21:20</v>
       </c>
@@ -12487,48 +12691,48 @@
         <f t="shared" si="26"/>
         <v>3.6833332409150898</v>
       </c>
-      <c r="H124" s="92" t="str">
+      <c r="H124" s="91" t="str">
         <f t="shared" si="24"/>
         <v>19:09</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A125" s="91" t="s">
+      <c r="A125" s="90" t="s">
         <v>985</v>
       </c>
-      <c r="B125" s="91">
+      <c r="B125" s="90">
         <v>0</v>
       </c>
-      <c r="C125" s="96">
+      <c r="C125" s="95">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D125" s="90" t="s">
+      <c r="D125" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E125" s="97"/>
-      <c r="F125" s="97"/>
-      <c r="G125" s="94"/>
-      <c r="H125" s="98"/>
+      <c r="E125" s="96"/>
+      <c r="F125" s="96"/>
+      <c r="G125" s="93"/>
+      <c r="H125" s="97"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="90" t="s">
+      <c r="A126" s="89" t="s">
         <v>695</v>
       </c>
-      <c r="B126" s="90">
+      <c r="B126" s="89">
         <v>0</v>
       </c>
-      <c r="C126" s="93">
+      <c r="C126" s="92">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D126" s="90" t="s">
+      <c r="D126" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E126" s="94"/>
-      <c r="F126" s="94"/>
-      <c r="G126" s="94"/>
-      <c r="H126" s="95"/>
+      <c r="E126" s="93"/>
+      <c r="F126" s="93"/>
+      <c r="G126" s="93"/>
+      <c r="H126" s="94"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
@@ -12589,7 +12793,7 @@
         <f>(F132-E132)*24*60</f>
         <v>7.0833333651535213</v>
       </c>
-      <c r="H132" s="88" t="str">
+      <c r="H132" s="87" t="str">
         <f t="shared" ref="H132:H139" si="27">HOUR(F132)&amp;IF(MINUTE(F132)&gt;=10, ":"&amp;MINUTE(F132), ":0"&amp;MINUTE(F132))</f>
         <v>20:06</v>
       </c>
@@ -12616,7 +12820,7 @@
         <f t="shared" ref="G133:G139" si="29">(F133-E133)*24*60</f>
         <v>5.116666752146557</v>
       </c>
-      <c r="H133" s="86" t="str">
+      <c r="H133" s="85" t="str">
         <f t="shared" si="27"/>
         <v>20:12</v>
       </c>
@@ -12643,7 +12847,7 @@
         <f t="shared" si="29"/>
         <v>18.016666551120579</v>
       </c>
-      <c r="H134" s="85" t="str">
+      <c r="H134" s="84" t="str">
         <f t="shared" si="27"/>
         <v>20:18</v>
       </c>
@@ -12670,7 +12874,7 @@
         <f t="shared" si="29"/>
         <v>32.466666680993512</v>
       </c>
-      <c r="H135" s="86" t="str">
+      <c r="H135" s="85" t="str">
         <f t="shared" si="27"/>
         <v>20:31</v>
       </c>
@@ -12697,7 +12901,7 @@
         <f t="shared" si="29"/>
         <v>2.4999999767169356</v>
       </c>
-      <c r="H136" s="85" t="str">
+      <c r="H136" s="84" t="str">
         <f t="shared" si="27"/>
         <v>20:32</v>
       </c>
@@ -12724,7 +12928,7 @@
         <f t="shared" si="29"/>
         <v>3.3500000182539225</v>
       </c>
-      <c r="H137" s="86" t="str">
+      <c r="H137" s="85" t="str">
         <f t="shared" si="27"/>
         <v>20:33</v>
       </c>
@@ -12751,7 +12955,7 @@
         <f t="shared" si="29"/>
         <v>35.116666703252122</v>
       </c>
-      <c r="H138" s="85" t="str">
+      <c r="H138" s="84" t="str">
         <f t="shared" si="27"/>
         <v>20:33</v>
       </c>
@@ -12778,67 +12982,67 @@
         <f t="shared" si="29"/>
         <v>28.033333338098601</v>
       </c>
-      <c r="H139" s="86" t="str">
+      <c r="H139" s="85" t="str">
         <f t="shared" si="27"/>
         <v>20:56</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="106" t="s">
+      <c r="A140" s="105" t="s">
         <v>985</v>
       </c>
-      <c r="B140" s="90">
+      <c r="B140" s="89">
         <v>0</v>
       </c>
-      <c r="C140" s="96">
+      <c r="C140" s="95">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D140" s="90" t="s">
+      <c r="D140" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E140" s="97"/>
-      <c r="F140" s="97"/>
-      <c r="G140" s="97"/>
-      <c r="H140" s="98"/>
+      <c r="E140" s="96"/>
+      <c r="F140" s="96"/>
+      <c r="G140" s="96"/>
+      <c r="H140" s="97"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="90" t="s">
+      <c r="A141" s="89" t="s">
         <v>1080</v>
       </c>
-      <c r="B141" s="90">
+      <c r="B141" s="89">
         <v>0</v>
       </c>
-      <c r="C141" s="93">
+      <c r="C141" s="92">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D141" s="90" t="s">
+      <c r="D141" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E141" s="94"/>
-      <c r="F141" s="94"/>
-      <c r="G141" s="94"/>
-      <c r="H141" s="95"/>
+      <c r="E141" s="93"/>
+      <c r="F141" s="93"/>
+      <c r="G141" s="93"/>
+      <c r="H141" s="94"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="91" t="s">
+      <c r="A142" s="90" t="s">
         <v>1082</v>
       </c>
-      <c r="B142" s="90">
+      <c r="B142" s="89">
         <v>0</v>
       </c>
-      <c r="C142" s="96">
+      <c r="C142" s="95">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="D142" s="90" t="s">
+      <c r="D142" s="89" t="s">
         <v>539</v>
       </c>
-      <c r="E142" s="97"/>
-      <c r="F142" s="97"/>
-      <c r="G142" s="97"/>
-      <c r="H142" s="98"/>
+      <c r="E142" s="96"/>
+      <c r="F142" s="96"/>
+      <c r="G142" s="96"/>
+      <c r="H142" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18841,7 +19045,7 @@
       <c r="AX83" t="s">
         <v>1062</v>
       </c>
-      <c r="BA83" s="105">
+      <c r="BA83" s="104">
         <f>(13-4)/13</f>
         <v>0.69230769230769229</v>
       </c>
@@ -18904,7 +19108,7 @@
       <c r="AX84" t="s">
         <v>1072</v>
       </c>
-      <c r="BA84" s="105">
+      <c r="BA84" s="104">
         <f t="shared" ref="BA84:BA87" si="2">(13-4)/13</f>
         <v>0.69230769230769229</v>
       </c>
@@ -18967,7 +19171,7 @@
       <c r="AX85" t="s">
         <v>1045</v>
       </c>
-      <c r="BA85" s="105">
+      <c r="BA85" s="104">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -19030,7 +19234,7 @@
       <c r="AX86" t="s">
         <v>1045</v>
       </c>
-      <c r="BA86" s="105">
+      <c r="BA86" s="104">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -19093,7 +19297,7 @@
       <c r="AX87" t="s">
         <v>1062</v>
       </c>
-      <c r="BA87" s="105">
+      <c r="BA87" s="104">
         <f t="shared" si="2"/>
         <v>0.69230769230769229</v>
       </c>
@@ -19124,190 +19328,190 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="147" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="147" customWidth="1"/>
-    <col min="3" max="3" width="76.1640625" style="147" customWidth="1"/>
-    <col min="4" max="4" width="83.6640625" style="149" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="147"/>
+    <col min="1" max="1" width="28.5" style="139" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="139" customWidth="1"/>
+    <col min="3" max="3" width="76.1640625" style="139" customWidth="1"/>
+    <col min="4" max="4" width="83.6640625" style="141" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="139"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="138" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="148"/>
+      <c r="A2" s="140"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="80" t="s">
         <v>1083</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="80" t="s">
         <v>987</v>
       </c>
-      <c r="D3" s="133" t="s">
+      <c r="D3" s="132" t="s">
         <v>1105</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="137" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C4" s="141" t="s">
+      <c r="B4" s="133" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C4" s="136" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D4" s="142" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E4" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="146"/>
+      <c r="B5" s="133" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C5" s="136" t="s">
         <v>1111</v>
       </c>
-      <c r="D4" s="150" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E4" s="147" t="s">
+      <c r="D5" s="136" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="133"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="139" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="142"/>
-      <c r="B5" s="137" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="137" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="133"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="137" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="133"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="137" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="133"/>
+      <c r="C9" s="135"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="133"/>
+      <c r="C10" s="135"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="137" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="133"/>
+      <c r="C11" s="135"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="143" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="133" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C12" s="135" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D12" s="142" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E12" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="144"/>
+      <c r="B13" s="133" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C13" s="135" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D13" s="142" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="137" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="133"/>
+      <c r="C14" s="135"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="133" t="s">
         <v>1102</v>
       </c>
-      <c r="C5" s="141" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D5" s="141" t="s">
+      <c r="C15" s="135" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D15" s="142" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E15" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="134" t="s">
         <v>1113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="143" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="137"/>
-      <c r="C6" s="140"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="143" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="137"/>
-      <c r="C7" s="140"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="143" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="137"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="143" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="137"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="143" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="137"/>
-      <c r="C10" s="140"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="143" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="137"/>
-      <c r="C11" s="140"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="144" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="137" t="s">
-        <v>1110</v>
-      </c>
-      <c r="C12" s="140" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D12" s="150" t="s">
-        <v>1115</v>
-      </c>
-      <c r="E12" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="145"/>
-      <c r="B13" s="137" t="s">
-        <v>1110</v>
-      </c>
-      <c r="C13" s="140" t="s">
-        <v>1118</v>
-      </c>
-      <c r="D13" s="150" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="143" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="140"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="143" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="137" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C15" s="140" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D15" s="150" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E15" s="147" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="138" t="s">
-        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -19334,7 +19538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6358CC-62AD-AF43-A08A-FACC5983B0AF}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -19394,668 +19598,668 @@
       <c r="P2" s="59" t="s">
         <v>1093</v>
       </c>
-      <c r="Q2" s="118" t="s">
+      <c r="Q2" s="117" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="115" t="s">
         <v>1087</v>
       </c>
-      <c r="C3" s="117">
+      <c r="C3" s="116">
         <v>1</v>
       </c>
-      <c r="D3" s="117">
+      <c r="D3" s="116">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="E3" s="117">
+      <c r="E3" s="116">
         <f t="shared" ref="E3:N3" si="0">D3+1</f>
         <v>3</v>
       </c>
-      <c r="F3" s="117">
+      <c r="F3" s="116">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G3" s="117">
+      <c r="G3" s="116">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H3" s="117">
+      <c r="H3" s="116">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I3" s="117">
+      <c r="I3" s="116">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J3" s="117">
+      <c r="J3" s="116">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K3" s="117">
+      <c r="K3" s="116">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L3" s="117">
+      <c r="L3" s="116">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M3" s="117">
+      <c r="M3" s="116">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N3" s="117">
+      <c r="N3" s="116">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O3" s="117">
+      <c r="O3" s="116">
         <f t="shared" ref="O3" si="1">N3+1</f>
         <v>13</v>
       </c>
-      <c r="P3" s="117">
+      <c r="P3" s="116">
         <f t="shared" ref="P3" si="2">O3+1</f>
         <v>14</v>
       </c>
-      <c r="Q3" s="117">
+      <c r="Q3" s="116">
         <f t="shared" ref="Q3" si="3">P3+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="112">
+      <c r="C4" s="111">
         <v>44580</v>
       </c>
-      <c r="D4" s="112">
+      <c r="D4" s="111">
         <f>C4+7</f>
         <v>44587</v>
       </c>
-      <c r="E4" s="112">
+      <c r="E4" s="111">
         <f t="shared" ref="E4:M4" si="4">D4+7</f>
         <v>44594</v>
       </c>
-      <c r="F4" s="112">
+      <c r="F4" s="111">
         <f t="shared" si="4"/>
         <v>44601</v>
       </c>
-      <c r="G4" s="112">
+      <c r="G4" s="111">
         <f t="shared" si="4"/>
         <v>44608</v>
       </c>
-      <c r="H4" s="112">
+      <c r="H4" s="111">
         <f t="shared" si="4"/>
         <v>44615</v>
       </c>
-      <c r="I4" s="112">
+      <c r="I4" s="111">
         <f t="shared" si="4"/>
         <v>44622</v>
       </c>
-      <c r="J4" s="112">
+      <c r="J4" s="111">
         <f t="shared" si="4"/>
         <v>44629</v>
       </c>
-      <c r="K4" s="112">
+      <c r="K4" s="111">
         <f t="shared" si="4"/>
         <v>44636</v>
       </c>
-      <c r="L4" s="112">
+      <c r="L4" s="111">
         <f t="shared" si="4"/>
         <v>44643</v>
       </c>
-      <c r="M4" s="112">
+      <c r="M4" s="111">
         <f t="shared" si="4"/>
         <v>44650</v>
       </c>
-      <c r="N4" s="112">
+      <c r="N4" s="111">
         <f t="shared" ref="N4:O4" si="5">M4+7</f>
         <v>44657</v>
       </c>
-      <c r="O4" s="112">
+      <c r="O4" s="111">
         <f t="shared" si="5"/>
         <v>44664</v>
       </c>
-      <c r="P4" s="112">
+      <c r="P4" s="111">
         <f t="shared" ref="P4:Q4" si="6">O4+7</f>
         <v>44671</v>
       </c>
-      <c r="Q4" s="112">
+      <c r="Q4" s="111">
         <f t="shared" si="6"/>
         <v>44678</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="115">
+      <c r="A5" s="114">
         <v>220981245</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="113">
+      <c r="C5" s="112">
         <v>1</v>
       </c>
-      <c r="D5" s="113">
+      <c r="D5" s="112">
         <v>1</v>
       </c>
-      <c r="E5" s="113">
+      <c r="E5" s="112">
         <v>1</v>
       </c>
-      <c r="F5" s="113">
+      <c r="F5" s="112">
         <v>1</v>
       </c>
-      <c r="G5" s="113">
+      <c r="G5" s="112">
         <v>1</v>
       </c>
-      <c r="H5" s="113">
+      <c r="H5" s="112">
         <v>1</v>
       </c>
-      <c r="I5" s="113">
+      <c r="I5" s="112">
         <v>1</v>
       </c>
-      <c r="J5" s="113">
+      <c r="J5" s="112">
         <v>1</v>
       </c>
-      <c r="K5" s="113">
+      <c r="K5" s="112">
         <v>1</v>
       </c>
-      <c r="L5" s="113">
+      <c r="L5" s="112">
         <v>1</v>
       </c>
-      <c r="M5" s="113">
+      <c r="M5" s="112">
         <v>1</v>
       </c>
-      <c r="N5" s="113">
+      <c r="N5" s="112">
         <v>1</v>
       </c>
-      <c r="O5" s="113" t="s">
+      <c r="O5" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P5" s="113" t="s">
+      <c r="P5" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q5" s="113">
+      <c r="Q5" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="115">
+      <c r="A6" s="114">
         <v>399515449</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="113">
+      <c r="C6" s="112">
         <v>1</v>
       </c>
-      <c r="D6" s="113">
+      <c r="D6" s="112">
         <v>1</v>
       </c>
-      <c r="E6" s="113">
+      <c r="E6" s="112">
         <v>1</v>
       </c>
-      <c r="F6" s="113">
+      <c r="F6" s="112">
         <v>1</v>
       </c>
-      <c r="G6" s="113">
+      <c r="G6" s="112">
         <v>1</v>
       </c>
-      <c r="H6" s="113">
+      <c r="H6" s="112">
         <v>1</v>
       </c>
-      <c r="I6" s="113">
+      <c r="I6" s="112">
         <v>1</v>
       </c>
-      <c r="J6" s="113">
+      <c r="J6" s="112">
         <v>1</v>
       </c>
-      <c r="K6" s="113">
+      <c r="K6" s="112">
         <v>1</v>
       </c>
-      <c r="L6" s="113">
+      <c r="L6" s="112">
         <v>1</v>
       </c>
-      <c r="M6" s="113">
+      <c r="M6" s="112">
         <v>1</v>
       </c>
-      <c r="N6" s="113">
+      <c r="N6" s="112">
         <v>1</v>
       </c>
-      <c r="O6" s="113" t="s">
+      <c r="O6" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P6" s="113" t="s">
+      <c r="P6" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q6" s="113">
+      <c r="Q6" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="115">
+      <c r="A7" s="114">
         <v>207595964</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="113">
+      <c r="C7" s="112">
         <v>1</v>
       </c>
-      <c r="D7" s="113">
+      <c r="D7" s="112">
         <v>1</v>
       </c>
-      <c r="E7" s="113">
+      <c r="E7" s="112">
         <v>1</v>
       </c>
-      <c r="F7" s="113">
+      <c r="F7" s="112">
         <v>1</v>
       </c>
-      <c r="G7" s="113">
+      <c r="G7" s="112">
         <v>1</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="112">
         <v>1</v>
       </c>
-      <c r="I7" s="113">
+      <c r="I7" s="112">
         <v>1</v>
       </c>
-      <c r="J7" s="113">
+      <c r="J7" s="112">
         <v>1</v>
       </c>
-      <c r="K7" s="113">
+      <c r="K7" s="112">
         <v>1</v>
       </c>
-      <c r="L7" s="113">
+      <c r="L7" s="112">
         <v>1</v>
       </c>
-      <c r="M7" s="113">
+      <c r="M7" s="112">
         <v>1</v>
       </c>
-      <c r="N7" s="113">
+      <c r="N7" s="112">
         <v>1</v>
       </c>
-      <c r="O7" s="113" t="s">
+      <c r="O7" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P7" s="113" t="s">
+      <c r="P7" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q7" s="113">
+      <c r="Q7" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="115">
+      <c r="A8" s="114">
         <v>211776124</v>
       </c>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="113">
+      <c r="C8" s="112">
         <v>1</v>
       </c>
-      <c r="D8" s="113">
+      <c r="D8" s="112">
         <v>1</v>
       </c>
-      <c r="E8" s="113">
+      <c r="E8" s="112">
         <v>1</v>
       </c>
-      <c r="F8" s="113">
+      <c r="F8" s="112">
         <v>1</v>
       </c>
-      <c r="G8" s="113">
+      <c r="G8" s="112">
         <v>1</v>
       </c>
-      <c r="H8" s="113">
+      <c r="H8" s="112">
         <v>1</v>
       </c>
-      <c r="I8" s="113">
+      <c r="I8" s="112">
         <v>1</v>
       </c>
-      <c r="J8" s="113">
+      <c r="J8" s="112">
         <v>1</v>
       </c>
-      <c r="K8" s="113">
+      <c r="K8" s="112">
         <v>1</v>
       </c>
-      <c r="L8" s="113">
+      <c r="L8" s="112">
         <v>1</v>
       </c>
-      <c r="M8" s="113">
+      <c r="M8" s="112">
         <v>1</v>
       </c>
-      <c r="N8" s="113">
+      <c r="N8" s="112">
         <v>1</v>
       </c>
-      <c r="O8" s="113" t="s">
+      <c r="O8" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q8" s="113">
+      <c r="Q8" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="115">
+      <c r="A9" s="114">
         <v>220981202</v>
       </c>
-      <c r="B9" s="115" t="s">
+      <c r="B9" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="113">
+      <c r="C9" s="112">
         <v>1</v>
       </c>
-      <c r="D9" s="113">
+      <c r="D9" s="112">
         <v>1</v>
       </c>
-      <c r="E9" s="113">
+      <c r="E9" s="112">
         <v>1</v>
       </c>
-      <c r="F9" s="113">
+      <c r="F9" s="112">
         <v>1</v>
       </c>
-      <c r="G9" s="113">
+      <c r="G9" s="112">
         <v>1</v>
       </c>
-      <c r="H9" s="113">
+      <c r="H9" s="112">
         <v>1</v>
       </c>
-      <c r="I9" s="113">
+      <c r="I9" s="112">
         <v>1</v>
       </c>
-      <c r="J9" s="113">
+      <c r="J9" s="112">
         <v>0</v>
       </c>
-      <c r="K9" s="113">
+      <c r="K9" s="112">
         <v>0</v>
       </c>
-      <c r="L9" s="113">
+      <c r="L9" s="112">
         <v>1</v>
       </c>
-      <c r="M9" s="113">
+      <c r="M9" s="112">
         <v>1</v>
       </c>
-      <c r="N9" s="113">
+      <c r="N9" s="112">
         <v>1</v>
       </c>
-      <c r="O9" s="113" t="s">
+      <c r="O9" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q9" s="113">
+      <c r="Q9" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="115">
+      <c r="A10" s="114">
         <v>398813438</v>
       </c>
-      <c r="B10" s="115" t="s">
+      <c r="B10" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="113">
+      <c r="C10" s="112">
         <v>1</v>
       </c>
-      <c r="D10" s="113">
+      <c r="D10" s="112">
         <v>1</v>
       </c>
-      <c r="E10" s="113">
+      <c r="E10" s="112">
         <v>1</v>
       </c>
-      <c r="F10" s="113">
+      <c r="F10" s="112">
         <v>1</v>
       </c>
-      <c r="G10" s="113">
+      <c r="G10" s="112">
         <v>1</v>
       </c>
-      <c r="H10" s="113">
+      <c r="H10" s="112">
         <v>1</v>
       </c>
-      <c r="I10" s="113">
+      <c r="I10" s="112">
         <v>1</v>
       </c>
-      <c r="J10" s="113">
+      <c r="J10" s="112">
         <v>1</v>
       </c>
-      <c r="K10" s="113">
+      <c r="K10" s="112">
         <v>1</v>
       </c>
-      <c r="L10" s="113">
+      <c r="L10" s="112">
         <v>1</v>
       </c>
-      <c r="M10" s="113">
+      <c r="M10" s="112">
         <v>1</v>
       </c>
-      <c r="N10" s="113">
+      <c r="N10" s="112">
         <v>1</v>
       </c>
-      <c r="O10" s="113" t="s">
+      <c r="O10" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P10" s="113" t="s">
+      <c r="P10" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q10" s="113">
+      <c r="Q10" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="115">
+      <c r="A11" s="114">
         <v>220981261</v>
       </c>
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="113">
+      <c r="C11" s="112">
         <v>1</v>
       </c>
-      <c r="D11" s="113">
+      <c r="D11" s="112">
         <v>1</v>
       </c>
-      <c r="E11" s="113">
+      <c r="E11" s="112">
         <v>1</v>
       </c>
-      <c r="F11" s="113">
+      <c r="F11" s="112">
         <v>1</v>
       </c>
-      <c r="G11" s="113">
+      <c r="G11" s="112">
         <v>1</v>
       </c>
-      <c r="H11" s="113">
+      <c r="H11" s="112">
         <v>1</v>
       </c>
-      <c r="I11" s="113">
+      <c r="I11" s="112">
         <v>1</v>
       </c>
-      <c r="J11" s="113">
+      <c r="J11" s="112">
         <v>1</v>
       </c>
-      <c r="K11" s="113">
+      <c r="K11" s="112">
         <v>1</v>
       </c>
-      <c r="L11" s="113">
+      <c r="L11" s="112">
         <v>1</v>
       </c>
-      <c r="M11" s="113">
+      <c r="M11" s="112">
         <v>0</v>
       </c>
-      <c r="N11" s="113">
+      <c r="N11" s="112">
         <v>1</v>
       </c>
-      <c r="O11" s="113" t="s">
+      <c r="O11" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P11" s="113" t="s">
+      <c r="P11" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q11" s="113">
+      <c r="Q11" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="115">
+      <c r="A12" s="114">
         <v>220981296</v>
       </c>
-      <c r="B12" s="115" t="s">
+      <c r="B12" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="113">
+      <c r="C12" s="112">
         <v>1</v>
       </c>
-      <c r="D12" s="113">
+      <c r="D12" s="112">
         <v>1</v>
       </c>
-      <c r="E12" s="113">
+      <c r="E12" s="112">
         <v>1</v>
       </c>
-      <c r="F12" s="113">
+      <c r="F12" s="112">
         <v>1</v>
       </c>
-      <c r="G12" s="113">
+      <c r="G12" s="112">
         <v>1</v>
       </c>
-      <c r="H12" s="113">
+      <c r="H12" s="112">
         <v>1</v>
       </c>
-      <c r="I12" s="113">
+      <c r="I12" s="112">
         <v>1</v>
       </c>
-      <c r="J12" s="113">
+      <c r="J12" s="112">
         <v>1</v>
       </c>
-      <c r="K12" s="113">
+      <c r="K12" s="112">
         <v>1</v>
       </c>
-      <c r="L12" s="113">
+      <c r="L12" s="112">
         <v>1</v>
       </c>
-      <c r="M12" s="113">
+      <c r="M12" s="112">
         <v>1</v>
       </c>
-      <c r="N12" s="113">
+      <c r="N12" s="112">
         <v>1</v>
       </c>
-      <c r="O12" s="113" t="s">
+      <c r="O12" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P12" s="113" t="s">
+      <c r="P12" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q12" s="113">
+      <c r="Q12" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="115">
+      <c r="A13" s="114">
         <v>220981229</v>
       </c>
-      <c r="B13" s="115" t="s">
+      <c r="B13" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="113">
+      <c r="C13" s="112">
         <v>1</v>
       </c>
-      <c r="D13" s="113">
+      <c r="D13" s="112">
         <v>1</v>
       </c>
-      <c r="E13" s="113">
+      <c r="E13" s="112">
         <v>1</v>
       </c>
-      <c r="F13" s="113">
+      <c r="F13" s="112">
         <v>1</v>
       </c>
-      <c r="G13" s="113">
+      <c r="G13" s="112">
         <v>0</v>
       </c>
-      <c r="H13" s="113">
+      <c r="H13" s="112">
         <v>1</v>
       </c>
-      <c r="I13" s="113">
+      <c r="I13" s="112">
         <v>1</v>
       </c>
-      <c r="J13" s="113">
+      <c r="J13" s="112">
         <v>1</v>
       </c>
-      <c r="K13" s="113">
+      <c r="K13" s="112">
         <v>1</v>
       </c>
-      <c r="L13" s="113">
+      <c r="L13" s="112">
         <v>0</v>
       </c>
-      <c r="M13" s="113">
+      <c r="M13" s="112">
         <v>0</v>
       </c>
-      <c r="N13" s="113">
+      <c r="N13" s="112">
         <v>1</v>
       </c>
-      <c r="O13" s="113" t="s">
+      <c r="O13" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P13" s="113" t="s">
+      <c r="P13" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q13" s="113">
+      <c r="Q13" s="112">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="115">
+      <c r="A14" s="114">
         <v>220981288</v>
       </c>
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="113">
+      <c r="C14" s="112">
         <v>1</v>
       </c>
-      <c r="D14" s="113">
+      <c r="D14" s="112">
         <v>1</v>
       </c>
-      <c r="E14" s="113">
+      <c r="E14" s="112">
         <v>1</v>
       </c>
-      <c r="F14" s="113">
+      <c r="F14" s="112">
         <v>1</v>
       </c>
-      <c r="G14" s="113">
+      <c r="G14" s="112">
         <v>1</v>
       </c>
-      <c r="H14" s="113">
+      <c r="H14" s="112">
         <v>1</v>
       </c>
-      <c r="I14" s="113">
+      <c r="I14" s="112">
         <v>1</v>
       </c>
-      <c r="J14" s="113">
+      <c r="J14" s="112">
         <v>1</v>
       </c>
-      <c r="K14" s="113">
+      <c r="K14" s="112">
         <v>1</v>
       </c>
-      <c r="L14" s="113">
+      <c r="L14" s="112">
         <v>1</v>
       </c>
-      <c r="M14" s="113">
+      <c r="M14" s="112">
         <v>1</v>
       </c>
-      <c r="N14" s="113">
+      <c r="N14" s="112">
         <v>1</v>
       </c>
-      <c r="O14" s="113" t="s">
+      <c r="O14" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="P14" s="113" t="s">
+      <c r="P14" s="112" t="s">
         <v>1091</v>
       </c>
-      <c r="Q14" s="113">
+      <c r="Q14" s="112">
         <v>1</v>
       </c>
     </row>
@@ -20065,39 +20269,39 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="109" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="111"/>
+      <c r="C19" s="110"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="111"/>
+      <c r="C20" s="110"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="111"/>
+      <c r="C21" s="110"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="111"/>
+      <c r="C22" s="110"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="111"/>
+      <c r="C23" s="110"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="111"/>
+      <c r="C24" s="110"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="111"/>
+      <c r="C25" s="110"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="111"/>
+      <c r="C26" s="110"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="111"/>
+      <c r="C27" s="110"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="111"/>
+      <c r="C28" s="110"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -20130,82 +20334,82 @@
       <c r="A2" s="23"/>
     </row>
     <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="80" t="s">
         <v>1100</v>
       </c>
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="147" t="s">
         <v>1101</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="136"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="129" t="s">
         <v>1099</v>
       </c>
-      <c r="D4" s="131" t="s">
+      <c r="D4" s="130" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="128" t="s">
         <v>991</v>
       </c>
-      <c r="C5" s="130" t="s">
+      <c r="C5" s="129" t="s">
         <v>1099</v>
       </c>
-      <c r="D5" s="131" t="s">
+      <c r="D5" s="130" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="129" t="s">
         <v>1099</v>
       </c>
-      <c r="D6" s="131" t="s">
+      <c r="D6" s="130" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="81" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="129" t="s">
         <v>1099</v>
       </c>
-      <c r="D7" s="131" t="s">
+      <c r="D7" s="130" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="130" t="s">
+      <c r="C8" s="129" t="s">
         <v>1099</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="130" t="s">
         <v>25</v>
       </c>
     </row>
@@ -20219,4 +20423,325 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C407C307-25D8-844C-8D75-C0561DBC7CB6}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="80" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="145" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B6" s="81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="153">
+        <v>1</v>
+      </c>
+      <c r="D6" s="153">
+        <v>1</v>
+      </c>
+      <c r="E6" s="153">
+        <v>1</v>
+      </c>
+      <c r="F6" s="153">
+        <v>0</v>
+      </c>
+      <c r="G6" s="153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="150"/>
+      <c r="B7" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="153">
+        <v>1</v>
+      </c>
+      <c r="D7" s="153">
+        <v>1</v>
+      </c>
+      <c r="E7" s="153">
+        <v>1</v>
+      </c>
+      <c r="F7" s="153">
+        <v>0</v>
+      </c>
+      <c r="G7" s="153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="150"/>
+      <c r="B8" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="153">
+        <v>1</v>
+      </c>
+      <c r="D8" s="153">
+        <v>1</v>
+      </c>
+      <c r="E8" s="153">
+        <v>1</v>
+      </c>
+      <c r="F8" s="153">
+        <v>0</v>
+      </c>
+      <c r="G8" s="153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="150"/>
+      <c r="B9" s="81" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="153">
+        <v>1</v>
+      </c>
+      <c r="D9" s="153">
+        <v>1</v>
+      </c>
+      <c r="E9" s="153">
+        <v>1</v>
+      </c>
+      <c r="F9" s="153">
+        <v>0</v>
+      </c>
+      <c r="G9" s="153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="150"/>
+      <c r="B10" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="153">
+        <v>1</v>
+      </c>
+      <c r="D10" s="153">
+        <v>1</v>
+      </c>
+      <c r="E10" s="153">
+        <v>1</v>
+      </c>
+      <c r="F10" s="153">
+        <v>0</v>
+      </c>
+      <c r="G10" s="153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="146"/>
+      <c r="B11" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="153">
+        <v>1</v>
+      </c>
+      <c r="D11" s="153">
+        <v>1</v>
+      </c>
+      <c r="E11" s="153">
+        <v>1</v>
+      </c>
+      <c r="F11" s="153">
+        <v>0</v>
+      </c>
+      <c r="G11" s="153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="137" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B12" s="81" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C12" s="153">
+        <v>1</v>
+      </c>
+      <c r="D12" s="153">
+        <v>1</v>
+      </c>
+      <c r="E12" s="153">
+        <v>1</v>
+      </c>
+      <c r="F12" s="153">
+        <v>0</v>
+      </c>
+      <c r="G12" s="153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="145" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C13" s="153">
+        <v>1</v>
+      </c>
+      <c r="D13" s="153">
+        <v>0</v>
+      </c>
+      <c r="E13" s="153">
+        <v>1</v>
+      </c>
+      <c r="F13" s="153">
+        <v>0</v>
+      </c>
+      <c r="G13" s="153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="150"/>
+      <c r="B14" s="81" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C14" s="153">
+        <v>1</v>
+      </c>
+      <c r="D14" s="153">
+        <v>0</v>
+      </c>
+      <c r="E14" s="153">
+        <v>1</v>
+      </c>
+      <c r="F14" s="153">
+        <v>0</v>
+      </c>
+      <c r="G14" s="153">
+        <v>1</v>
+      </c>
+      <c r="J14" s="139" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="146"/>
+      <c r="B15" s="81" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C15" s="153">
+        <v>1</v>
+      </c>
+      <c r="D15" s="153">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="153">
+        <v>1</v>
+      </c>
+      <c r="F15" s="153">
+        <v>0</v>
+      </c>
+      <c r="G15" s="153">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="154" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="151" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B16" s="152"/>
+      <c r="C16" s="155">
+        <f>AVERAGE(C6:C15)*100</f>
+        <v>100</v>
+      </c>
+      <c r="D16" s="155">
+        <f t="shared" ref="D16:G16" si="0">AVERAGE(D6:D15)*100</f>
+        <v>75</v>
+      </c>
+      <c r="E16" s="155">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F16" s="155">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="155">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A13:A15"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="C6:G15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF8687"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color rgb="FFABD090"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J15" r:id="rId1" xr:uid="{D943B7B7-D97E-4246-9183-37F966DE34E5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se suben las calificaciones finales
</commit_message>
<xml_diff>
--- a/grades/Calificaciones.xlsx
+++ b/grades/Calificaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcuspinera/Documents/levic/05_Projects_levic/Projects_git/UDG_MCD_Project_Dev_II/grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF16484-67F0-7544-A959-011672DDE32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7124A8-5432-564B-984E-2BBE1649C0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="27940" windowHeight="16440" xr2:uid="{48FBB0DA-F14C-344C-B744-CE4CDA02BE2C}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2285" uniqueCount="1136">
   <si>
     <t>Id. estudiante</t>
   </si>
@@ -4028,6 +4028,12 @@
   <si>
     <t>Cada punto a calificar se le asignará 0 si no se entregó, 0.5 si se entregó con errores y 1 si es correcto. La calificación del examen final es el promedio de todas las actividades del examen.</t>
   </si>
+  <si>
+    <t>Proyecto personal "Data Science Automation Tools"</t>
+  </si>
+  <si>
+    <t>https://github.com/marioph2022/ds_automation</t>
+  </si>
 </sst>
 </file>
 
@@ -4037,7 +4043,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0\ &quot;%&quot;"/>
+    <numFmt numFmtId="167" formatCode="0\ &quot;%&quot;"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -4690,7 +4696,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4968,6 +4974,21 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="16" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4992,20 +5013,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="16" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7923,7 +7932,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8260,15 +8269,15 @@
       </c>
       <c r="G12" s="124">
         <f>RESUMEN!C31</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H12" s="125">
         <f t="shared" si="0"/>
-        <v>97.989122400475338</v>
+        <v>100</v>
       </c>
       <c r="I12" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|15|10|__98__|</v>
+        <v>|220981296|Mario Palomino Hernández|30|24.7|18.3|15|15|__100__|</v>
       </c>
     </row>
     <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8355,9 +8364,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB78B30B-85E1-8742-88C2-F69873755D79}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A41" sqref="A41"/>
+      <selection pane="topRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9746,14 +9755,14 @@
       </c>
       <c r="C31" s="16">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E31" s="36">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F31" s="34">
         <v>0</v>
@@ -9946,7 +9955,7 @@
       </c>
       <c r="C50" s="16">
         <f t="shared" si="6"/>
-        <v>97.989122400475338</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -19320,10 +19329,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56003B35-B20E-7E41-B8AA-8807D2B14A4C}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19358,7 +19367,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="150" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="133" t="s">
@@ -19375,7 +19384,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="146"/>
+      <c r="A5" s="151"/>
       <c r="B5" s="133" t="s">
         <v>1102</v>
       </c>
@@ -19453,7 +19462,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="143" t="s">
+      <c r="A12" s="148" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="133" t="s">
@@ -19470,7 +19479,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="144"/>
+      <c r="A13" s="156"/>
       <c r="B13" s="133" t="s">
         <v>1109</v>
       </c>
@@ -19481,54 +19490,67 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="137" t="s">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="149"/>
+      <c r="B14" s="133" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C14" s="135" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D14" s="142" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="133"/>
-      <c r="C14" s="135"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="139" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="137" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="133" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C15" s="135" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D15" s="142" t="s">
-        <v>1104</v>
-      </c>
+      <c r="B15" s="133"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="131"/>
       <c r="E15" s="139" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="134" t="s">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="133" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C16" s="135" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D16" s="142" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E16" s="139" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="134" t="s">
         <v>1113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A12:A14"/>
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B15" xr:uid="{056D01C0-61E5-EE48-96CE-68F5E7E36218}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B16" xr:uid="{056D01C0-61E5-EE48-96CE-68F5E7E36218}">
       <formula1>"Proyecto personal, Publicación, Voluntariado, Hackathon, Otra"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1" xr:uid="{A22C7851-AA9B-3647-AB35-981668C8A869}"/>
+    <hyperlink ref="D16" r:id="rId1" xr:uid="{A22C7851-AA9B-3647-AB35-981668C8A869}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{CE298372-D79F-9644-BCDA-83ADF8BE8EAA}"/>
     <hyperlink ref="D12" r:id="rId3" xr:uid="{7C23D744-7619-8E44-B373-DF5473B7BDE3}"/>
-    <hyperlink ref="D13" r:id="rId4" xr:uid="{79F6FADB-05E6-D046-BCE4-9874A5879F96}"/>
+    <hyperlink ref="D14" r:id="rId4" xr:uid="{79F6FADB-05E6-D046-BCE4-9874A5879F96}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{B69CD813-D7F5-F04E-9A5B-A03E324ECE87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20337,11 +20359,11 @@
       <c r="A3" s="80" t="s">
         <v>1100</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="152" t="s">
         <v>1101</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="81" t="s">
@@ -20473,130 +20495,130 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="145" t="s">
+      <c r="A6" s="150" t="s">
         <v>1132</v>
       </c>
       <c r="B6" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="153">
+      <c r="C6" s="145">
         <v>1</v>
       </c>
-      <c r="D6" s="153">
+      <c r="D6" s="145">
         <v>1</v>
       </c>
-      <c r="E6" s="153">
+      <c r="E6" s="145">
         <v>1</v>
       </c>
-      <c r="F6" s="153">
+      <c r="F6" s="145">
         <v>0</v>
       </c>
-      <c r="G6" s="153">
+      <c r="G6" s="145">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="150"/>
+      <c r="A7" s="155"/>
       <c r="B7" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="153">
+      <c r="C7" s="145">
         <v>1</v>
       </c>
-      <c r="D7" s="153">
+      <c r="D7" s="145">
         <v>1</v>
       </c>
-      <c r="E7" s="153">
+      <c r="E7" s="145">
         <v>1</v>
       </c>
-      <c r="F7" s="153">
+      <c r="F7" s="145">
         <v>0</v>
       </c>
-      <c r="G7" s="153">
+      <c r="G7" s="145">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="150"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="153">
+      <c r="C8" s="145">
         <v>1</v>
       </c>
-      <c r="D8" s="153">
+      <c r="D8" s="145">
         <v>1</v>
       </c>
-      <c r="E8" s="153">
+      <c r="E8" s="145">
         <v>1</v>
       </c>
-      <c r="F8" s="153">
+      <c r="F8" s="145">
         <v>0</v>
       </c>
-      <c r="G8" s="153">
+      <c r="G8" s="145">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="150"/>
+      <c r="A9" s="155"/>
       <c r="B9" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="C9" s="153">
+      <c r="C9" s="145">
         <v>1</v>
       </c>
-      <c r="D9" s="153">
+      <c r="D9" s="145">
         <v>1</v>
       </c>
-      <c r="E9" s="153">
+      <c r="E9" s="145">
         <v>1</v>
       </c>
-      <c r="F9" s="153">
+      <c r="F9" s="145">
         <v>0</v>
       </c>
-      <c r="G9" s="153">
+      <c r="G9" s="145">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="150"/>
+      <c r="A10" s="155"/>
       <c r="B10" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="C10" s="153">
+      <c r="C10" s="145">
         <v>1</v>
       </c>
-      <c r="D10" s="153">
+      <c r="D10" s="145">
         <v>1</v>
       </c>
-      <c r="E10" s="153">
+      <c r="E10" s="145">
         <v>1</v>
       </c>
-      <c r="F10" s="153">
+      <c r="F10" s="145">
         <v>0</v>
       </c>
-      <c r="G10" s="153">
+      <c r="G10" s="145">
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="146"/>
+      <c r="A11" s="151"/>
       <c r="B11" s="81" t="s">
         <v>205</v>
       </c>
-      <c r="C11" s="153">
+      <c r="C11" s="145">
         <v>1</v>
       </c>
-      <c r="D11" s="153">
+      <c r="D11" s="145">
         <v>1</v>
       </c>
-      <c r="E11" s="153">
+      <c r="E11" s="145">
         <v>1</v>
       </c>
-      <c r="F11" s="153">
+      <c r="F11" s="145">
         <v>0</v>
       </c>
-      <c r="G11" s="153">
+      <c r="G11" s="145">
         <v>1</v>
       </c>
     </row>
@@ -20607,63 +20629,63 @@
       <c r="B12" s="81" t="s">
         <v>1122</v>
       </c>
-      <c r="C12" s="153">
+      <c r="C12" s="145">
         <v>1</v>
       </c>
-      <c r="D12" s="153">
+      <c r="D12" s="145">
         <v>1</v>
       </c>
-      <c r="E12" s="153">
+      <c r="E12" s="145">
         <v>1</v>
       </c>
-      <c r="F12" s="153">
+      <c r="F12" s="145">
         <v>0</v>
       </c>
-      <c r="G12" s="153">
+      <c r="G12" s="145">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="145" t="s">
+      <c r="A13" s="150" t="s">
         <v>1131</v>
       </c>
       <c r="B13" s="81" t="s">
         <v>1125</v>
       </c>
-      <c r="C13" s="153">
+      <c r="C13" s="145">
         <v>1</v>
       </c>
-      <c r="D13" s="153">
+      <c r="D13" s="145">
         <v>0</v>
       </c>
-      <c r="E13" s="153">
+      <c r="E13" s="145">
         <v>1</v>
       </c>
-      <c r="F13" s="153">
+      <c r="F13" s="145">
         <v>0</v>
       </c>
-      <c r="G13" s="153">
+      <c r="G13" s="145">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="150"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="81" t="s">
         <v>1126</v>
       </c>
-      <c r="C14" s="153">
+      <c r="C14" s="145">
         <v>1</v>
       </c>
-      <c r="D14" s="153">
+      <c r="D14" s="145">
         <v>0</v>
       </c>
-      <c r="E14" s="153">
+      <c r="E14" s="145">
         <v>1</v>
       </c>
-      <c r="F14" s="153">
+      <c r="F14" s="145">
         <v>0</v>
       </c>
-      <c r="G14" s="153">
+      <c r="G14" s="145">
         <v>1</v>
       </c>
       <c r="J14" s="139" t="s">
@@ -20671,51 +20693,51 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="146"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="81" t="s">
         <v>1121</v>
       </c>
-      <c r="C15" s="153">
+      <c r="C15" s="145">
         <v>1</v>
       </c>
-      <c r="D15" s="153">
+      <c r="D15" s="145">
         <v>0.5</v>
       </c>
-      <c r="E15" s="153">
+      <c r="E15" s="145">
         <v>1</v>
       </c>
-      <c r="F15" s="153">
+      <c r="F15" s="145">
         <v>0</v>
       </c>
-      <c r="G15" s="153">
+      <c r="G15" s="145">
         <v>0.5</v>
       </c>
-      <c r="J15" s="154" t="s">
+      <c r="J15" s="146" t="s">
         <v>1127</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="143" t="s">
         <v>1123</v>
       </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="155">
+      <c r="B16" s="144"/>
+      <c r="C16" s="147">
         <f>AVERAGE(C6:C15)*100</f>
         <v>100</v>
       </c>
-      <c r="D16" s="155">
+      <c r="D16" s="147">
         <f t="shared" ref="D16:G16" si="0">AVERAGE(D6:D15)*100</f>
         <v>75</v>
       </c>
-      <c r="E16" s="155">
+      <c r="E16" s="147">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F16" s="155">
+      <c r="F16" s="147">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="155">
+      <c r="G16" s="147">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>

</xml_diff>